<commit_message>
Slight increase in LPG tank rental
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B872128B-F9F8-4CFD-A932-4046B7C9E803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF1B590-FBFB-47E1-9574-BC3A648E807A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -13547,6 +13547,15 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13554,15 +13563,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13574,13 +13574,22 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13592,19 +13601,10 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13622,12 +13622,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13642,6 +13636,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -21173,8 +21173,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Y103" sqref="Y103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21364,12 +21364,12 @@
         <v>85</v>
       </c>
       <c r="U4" s="539"/>
-      <c r="V4" s="540" t="s">
+      <c r="V4" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="541"/>
-      <c r="X4" s="541"/>
-      <c r="Y4" s="542"/>
+      <c r="W4" s="532"/>
+      <c r="X4" s="532"/>
+      <c r="Y4" s="533"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21472,34 +21472,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="531" t="s">
+      <c r="H6" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="532"/>
-      <c r="J6" s="532"/>
-      <c r="K6" s="533"/>
-      <c r="L6" s="532" t="s">
+      <c r="I6" s="535"/>
+      <c r="J6" s="535"/>
+      <c r="K6" s="536"/>
+      <c r="L6" s="535" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="532"/>
-      <c r="N6" s="532"/>
-      <c r="O6" s="533"/>
-      <c r="P6" s="531" t="s">
+      <c r="M6" s="535"/>
+      <c r="N6" s="535"/>
+      <c r="O6" s="536"/>
+      <c r="P6" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="532"/>
-      <c r="R6" s="532"/>
-      <c r="S6" s="533"/>
-      <c r="T6" s="531" t="s">
+      <c r="Q6" s="535"/>
+      <c r="R6" s="535"/>
+      <c r="S6" s="536"/>
+      <c r="T6" s="534" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="533"/>
-      <c r="V6" s="531" t="s">
+      <c r="U6" s="536"/>
+      <c r="V6" s="534" t="s">
         <v>541</v>
       </c>
-      <c r="W6" s="532"/>
-      <c r="X6" s="532"/>
-      <c r="Y6" s="533"/>
+      <c r="W6" s="535"/>
+      <c r="X6" s="535"/>
+      <c r="Y6" s="536"/>
       <c r="Z6" s="61" t="s">
         <v>553</v>
       </c>
@@ -21997,20 +21997,20 @@
       </c>
       <c r="U11" s="30"/>
       <c r="V11" s="383">
-        <f>SUM(2.79+0.25)</f>
-        <v>3.04</v>
+        <f>2.79+0.35</f>
+        <v>3.14</v>
       </c>
       <c r="W11" s="383">
-        <f t="shared" ref="W11:Y11" si="11">SUM(2.79+0.25)</f>
-        <v>3.04</v>
+        <f t="shared" ref="W11:Y11" si="11">2.79+0.35</f>
+        <v>3.14</v>
       </c>
       <c r="X11" s="383">
         <f t="shared" si="11"/>
-        <v>3.04</v>
+        <v>3.14</v>
       </c>
       <c r="Y11" s="383">
         <f t="shared" si="11"/>
-        <v>3.04</v>
+        <v>3.14</v>
       </c>
       <c r="Z11" s="383">
         <f>0.12+0.15</f>
@@ -22105,20 +22105,20 @@
       </c>
       <c r="U12" s="24"/>
       <c r="V12" s="384">
-        <f>V11*($U$150/$U$149)</f>
-        <v>3.0656540084388189</v>
+        <f>V10+0.35</f>
+        <v>3.1635443037974689</v>
       </c>
       <c r="W12" s="384">
-        <f>W11*($U$150/$U$149)</f>
-        <v>3.0656540084388189</v>
+        <f t="shared" ref="W12:Y12" si="13">W10+0.35</f>
+        <v>3.1635443037974689</v>
       </c>
       <c r="X12" s="384">
-        <f>X11*($U$150/$U$149)</f>
-        <v>3.0656540084388189</v>
+        <f t="shared" si="13"/>
+        <v>3.1635443037974689</v>
       </c>
       <c r="Y12" s="384">
-        <f>Y11*($U$150/$U$149)</f>
-        <v>3.0656540084388189</v>
+        <f t="shared" si="13"/>
+        <v>3.1635443037974689</v>
       </c>
       <c r="Z12" s="384">
         <f>0.12+0.15</f>
@@ -22286,19 +22286,19 @@
       <c r="N14" s="32"/>
       <c r="O14" s="45"/>
       <c r="P14" s="247">
-        <f t="shared" ref="P14:S14" si="13">H14*0.7</f>
+        <f t="shared" ref="P14:S14" si="14">H14*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q14" s="248">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="R14" s="248">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="S14" s="249">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="T14" s="53">
@@ -22496,11 +22496,11 @@
       </c>
       <c r="AL16" s="104"/>
       <c r="AM16" s="103" t="str">
-        <f t="shared" ref="AM16:AN21" si="14">C18</f>
+        <f t="shared" ref="AM16:AN21" si="15">C18</f>
         <v>R-SH_Apt_ELC_HPN1</v>
       </c>
       <c r="AN16" s="103" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AO16" s="104" t="s">
@@ -22562,11 +22562,11 @@
       <c r="AJ17" s="34"/>
       <c r="AL17" s="106"/>
       <c r="AM17" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-HC_Apt_ELC_HPN1</v>
       </c>
       <c r="AN17" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AO17" s="106" t="s">
@@ -22651,7 +22651,7 @@
       <c r="AE18" s="264"/>
       <c r="AF18" s="264"/>
       <c r="AG18" s="85">
-        <f t="shared" ref="AG18:AG23" si="15">31.536*(AJ18/1000)</f>
+        <f t="shared" ref="AG18:AG23" si="16">31.536*(AJ18/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH18" s="88"/>
@@ -22663,11 +22663,11 @@
       </c>
       <c r="AL18" s="106"/>
       <c r="AM18" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-SH_Apt_ELC_HPN2</v>
       </c>
       <c r="AN18" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AO18" s="106" t="s">
@@ -22763,7 +22763,7 @@
       <c r="AE19" s="73"/>
       <c r="AF19" s="73"/>
       <c r="AG19" s="63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH19" s="66"/>
@@ -22775,11 +22775,11 @@
       </c>
       <c r="AL19" s="106"/>
       <c r="AM19" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
       <c r="AN19" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AO19" s="106" t="s">
@@ -22863,7 +22863,7 @@
       <c r="AE20" s="72"/>
       <c r="AF20" s="72"/>
       <c r="AG20" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH20" s="65"/>
@@ -22875,11 +22875,11 @@
       </c>
       <c r="AL20" s="213"/>
       <c r="AM20" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-SH_Apt_ELC_HPN3</v>
       </c>
       <c r="AN20" s="105" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AO20" s="106" t="s">
@@ -22935,15 +22935,15 @@
         <v>0.7</v>
       </c>
       <c r="Q21" s="23">
-        <f t="shared" ref="Q21:S21" si="16">I21*0.7</f>
+        <f t="shared" ref="Q21:S21" si="17">I21*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R21" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.86333333333333329</v>
       </c>
       <c r="S21" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="T21" s="53">
@@ -22976,7 +22976,7 @@
       <c r="AE21" s="73"/>
       <c r="AF21" s="73"/>
       <c r="AG21" s="63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AH21" s="66"/>
@@ -22988,11 +22988,11 @@
       </c>
       <c r="AL21" s="112"/>
       <c r="AM21" s="108" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
       <c r="AN21" s="108" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AO21" s="109" t="s">
@@ -23078,7 +23078,7 @@
       <c r="AE22" s="72"/>
       <c r="AF22" s="72"/>
       <c r="AG22" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH22" s="65"/>
@@ -23191,7 +23191,7 @@
       <c r="AE23" s="73"/>
       <c r="AF23" s="73"/>
       <c r="AG23" s="63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH23" s="66"/>
@@ -23320,15 +23320,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q25" s="20">
-        <f t="shared" ref="Q25:S25" si="17">I25*0.7</f>
+        <f t="shared" ref="Q25:S25" si="18">I25*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R25" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="S25" s="56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="T25" s="89">
@@ -23362,7 +23362,7 @@
       <c r="AE25" s="85"/>
       <c r="AF25" s="85"/>
       <c r="AG25" s="85">
-        <f t="shared" ref="AG25:AG26" si="18">31.536*(AJ25/1000)</f>
+        <f t="shared" ref="AG25:AG26" si="19">31.536*(AJ25/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AH25" s="88"/>
@@ -23434,15 +23434,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q26" s="26">
-        <f t="shared" ref="Q26" si="19">I26*0.7</f>
+        <f t="shared" ref="Q26" si="20">I26*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="R26" s="26">
-        <f t="shared" ref="R26" si="20">J26*0.7</f>
+        <f t="shared" ref="R26" si="21">J26*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="S26" s="59">
-        <f t="shared" ref="S26" si="21">K26*0.7</f>
+        <f t="shared" ref="S26" si="22">K26*0.7</f>
         <v>1.2444444444444445</v>
       </c>
       <c r="T26" s="27">
@@ -23476,7 +23476,7 @@
       <c r="AE26" s="64"/>
       <c r="AF26" s="64"/>
       <c r="AG26" s="64">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AH26" s="67"/>
@@ -23609,11 +23609,11 @@
         <v>2.5409999999999995</v>
       </c>
       <c r="R28" s="26">
-        <f t="shared" ref="R28:S28" si="22">J28*0.7</f>
+        <f t="shared" ref="R28:S28" si="23">J28*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S28" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2.7299999999999995</v>
       </c>
       <c r="T28" s="260">
@@ -23625,15 +23625,15 @@
         <v>8.3046953586497896</v>
       </c>
       <c r="W28" s="79">
-        <f t="shared" ref="W28:Y28" si="23">(W21+W10)*0.8</f>
+        <f t="shared" ref="W28:Y28" si="24">(W21+W10)*0.8</f>
         <v>7.7598479662447266</v>
       </c>
       <c r="X28" s="79">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>7.2640368391561196</v>
       </c>
       <c r="Y28" s="79">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>7.2150005738396636</v>
       </c>
       <c r="Z28" s="265">
@@ -23818,7 +23818,7 @@
       <c r="AE30" s="85"/>
       <c r="AF30" s="85"/>
       <c r="AG30" s="85">
-        <f t="shared" ref="AG30:AG31" si="24">31.536*(AJ30/1000)</f>
+        <f t="shared" ref="AG30:AG31" si="25">31.536*(AJ30/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AH30" s="88"/>
@@ -23921,7 +23921,7 @@
       <c r="AE31" s="63"/>
       <c r="AF31" s="63"/>
       <c r="AG31" s="64">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AH31" s="67"/>
@@ -24036,7 +24036,7 @@
       <c r="AE33" s="85"/>
       <c r="AF33" s="85"/>
       <c r="AG33" s="85">
-        <f t="shared" ref="AG33:AG34" si="25">31.536*(AJ33/1000)</f>
+        <f t="shared" ref="AG33:AG34" si="26">31.536*(AJ33/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH33" s="88"/>
@@ -24115,7 +24115,7 @@
       <c r="AE34" s="63"/>
       <c r="AF34" s="63"/>
       <c r="AG34" s="63">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH34" s="66"/>
@@ -24233,7 +24233,7 @@
       <c r="AE36" s="85"/>
       <c r="AF36" s="85"/>
       <c r="AG36" s="85">
-        <f t="shared" ref="AG36:AG37" si="26">31.536*(AJ36/1000)</f>
+        <f t="shared" ref="AG36:AG37" si="27">31.536*(AJ36/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH36" s="88"/>
@@ -24313,7 +24313,7 @@
       <c r="AE37" s="63"/>
       <c r="AF37" s="63"/>
       <c r="AG37" s="64">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AH37" s="67"/>
@@ -24554,12 +24554,12 @@
         <v>85</v>
       </c>
       <c r="U42" s="539"/>
-      <c r="V42" s="540" t="s">
+      <c r="V42" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="W42" s="541"/>
-      <c r="X42" s="541"/>
-      <c r="Y42" s="542"/>
+      <c r="W42" s="532"/>
+      <c r="X42" s="532"/>
+      <c r="Y42" s="533"/>
       <c r="Z42" s="60"/>
       <c r="AA42" s="60"/>
       <c r="AB42" s="68" t="s">
@@ -24660,34 +24660,34 @@
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
       <c r="G44" s="39"/>
-      <c r="H44" s="531" t="s">
+      <c r="H44" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="532"/>
-      <c r="J44" s="532"/>
-      <c r="K44" s="533"/>
-      <c r="L44" s="532" t="s">
+      <c r="I44" s="535"/>
+      <c r="J44" s="535"/>
+      <c r="K44" s="536"/>
+      <c r="L44" s="535" t="s">
         <v>34</v>
       </c>
-      <c r="M44" s="532"/>
-      <c r="N44" s="532"/>
-      <c r="O44" s="533"/>
-      <c r="P44" s="531" t="s">
+      <c r="M44" s="535"/>
+      <c r="N44" s="535"/>
+      <c r="O44" s="536"/>
+      <c r="P44" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="Q44" s="532"/>
-      <c r="R44" s="532"/>
-      <c r="S44" s="533"/>
-      <c r="T44" s="534" t="s">
+      <c r="Q44" s="535"/>
+      <c r="R44" s="535"/>
+      <c r="S44" s="536"/>
+      <c r="T44" s="540" t="s">
         <v>68</v>
       </c>
-      <c r="U44" s="535"/>
-      <c r="V44" s="534" t="s">
+      <c r="U44" s="541"/>
+      <c r="V44" s="540" t="s">
         <v>541</v>
       </c>
-      <c r="W44" s="536"/>
-      <c r="X44" s="536"/>
-      <c r="Y44" s="535"/>
+      <c r="W44" s="542"/>
+      <c r="X44" s="542"/>
+      <c r="Y44" s="541"/>
       <c r="Z44" s="377" t="s">
         <v>553</v>
       </c>
@@ -24783,15 +24783,15 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="W45" s="383">
-        <f t="shared" ref="W45:Y45" si="27">W49*1.3</f>
+        <f t="shared" ref="W45:Y45" si="28">W49*1.3</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="X45" s="383">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y45" s="383">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z45" s="383">
@@ -24804,7 +24804,7 @@
       <c r="AE45" s="72"/>
       <c r="AF45" s="72"/>
       <c r="AG45" s="62">
-        <f t="shared" ref="AG45:AG83" si="28">31.536*(AJ45/1000)</f>
+        <f t="shared" ref="AG45:AG83" si="29">31.536*(AJ45/1000)</f>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH45" s="65"/>
@@ -24818,11 +24818,11 @@
         <v>31</v>
       </c>
       <c r="AM45" s="105" t="str">
-        <f t="shared" ref="AM45:AM60" si="29">C45</f>
+        <f t="shared" ref="AM45:AM60" si="30">C45</f>
         <v>R-SH_Att_KER_N1</v>
       </c>
       <c r="AN45" s="105" t="str">
-        <f t="shared" ref="AN45:AN60" si="30">D45</f>
+        <f t="shared" ref="AN45:AN60" si="31">D45</f>
         <v>Residential Kerosene Heating Oil - New 1 SH</v>
       </c>
       <c r="AO45" s="106" t="s">
@@ -24872,15 +24872,15 @@
         <v>0.7</v>
       </c>
       <c r="Q46" s="23">
-        <f t="shared" ref="Q46:Q48" si="31">I46*0.7</f>
+        <f t="shared" ref="Q46:Q48" si="32">I46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R46" s="23">
-        <f t="shared" ref="R46:R48" si="32">J46*0.7</f>
+        <f t="shared" ref="R46:R48" si="33">J46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S46" s="57">
-        <f t="shared" ref="S46:S48" si="33">K46*0.7</f>
+        <f t="shared" ref="S46:S48" si="34">K46*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T46" s="53">
@@ -24892,15 +24892,15 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="W46" s="384">
-        <f t="shared" ref="W46:Y46" si="34">W50*1.3</f>
+        <f t="shared" ref="W46:Y46" si="35">W50*1.3</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="X46" s="384">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y46" s="384">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Z46" s="384">
@@ -24913,7 +24913,7 @@
       <c r="AE46" s="73"/>
       <c r="AF46" s="73"/>
       <c r="AG46" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH46" s="66"/>
@@ -24925,11 +24925,11 @@
       </c>
       <c r="AL46" s="106"/>
       <c r="AM46" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AN46" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AO46" s="106" t="s">
@@ -24979,15 +24979,15 @@
         <v>0.7</v>
       </c>
       <c r="Q47" s="29">
-        <f t="shared" si="31"/>
-        <v>0.7</v>
-      </c>
-      <c r="R47" s="29">
         <f t="shared" si="32"/>
         <v>0.7</v>
       </c>
+      <c r="R47" s="29">
+        <f t="shared" si="33"/>
+        <v>0.7</v>
+      </c>
       <c r="S47" s="58">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.7</v>
       </c>
       <c r="T47" s="54">
@@ -25025,7 +25025,7 @@
         <v>5</v>
       </c>
       <c r="AG47" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH47" s="65"/>
@@ -25037,11 +25037,11 @@
       </c>
       <c r="AL47" s="106"/>
       <c r="AM47" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AN47" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AO47" s="106" t="s">
@@ -25091,15 +25091,15 @@
         <v>0.7</v>
       </c>
       <c r="Q48" s="23">
-        <f t="shared" si="31"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R48" s="23">
         <f t="shared" si="32"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R48" s="23">
+        <f t="shared" si="33"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S48" s="57">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T48" s="53">
@@ -25149,11 +25149,11 @@
       </c>
       <c r="AL48" s="106"/>
       <c r="AM48" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AN48" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AO48" s="107" t="s">
@@ -25209,15 +25209,15 @@
         <v>3.25</v>
       </c>
       <c r="W49" s="383">
-        <f t="shared" ref="W49:Y49" si="35">3.25</f>
+        <f t="shared" ref="W49:Y49" si="36">3.25</f>
         <v>3.25</v>
       </c>
       <c r="X49" s="383">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.25</v>
       </c>
       <c r="Y49" s="383">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.25</v>
       </c>
       <c r="Z49" s="383">
@@ -25230,7 +25230,7 @@
       <c r="AE49" s="72"/>
       <c r="AF49" s="72"/>
       <c r="AG49" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH49" s="65"/>
@@ -25242,11 +25242,11 @@
       </c>
       <c r="AL49" s="106"/>
       <c r="AM49" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AN49" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AO49" s="106" t="s">
@@ -25296,15 +25296,15 @@
         <v>0.7</v>
       </c>
       <c r="Q50" s="23">
-        <f t="shared" ref="Q50:Q52" si="36">I50*0.7</f>
+        <f t="shared" ref="Q50:Q52" si="37">I50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R50" s="23">
-        <f t="shared" ref="R50:R52" si="37">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="38">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="57">
-        <f t="shared" ref="S50:S52" si="38">K50*0.7</f>
+        <f t="shared" ref="S50:S52" si="39">K50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T50" s="53">
@@ -25337,7 +25337,7 @@
       <c r="AE50" s="73"/>
       <c r="AF50" s="73"/>
       <c r="AG50" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH50" s="66"/>
@@ -25349,11 +25349,11 @@
       </c>
       <c r="AL50" s="106"/>
       <c r="AM50" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AN50" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AO50" s="106" t="s">
@@ -25403,15 +25403,15 @@
         <v>0.7</v>
       </c>
       <c r="Q51" s="29">
-        <f t="shared" si="36"/>
-        <v>0.7</v>
-      </c>
-      <c r="R51" s="29">
         <f t="shared" si="37"/>
         <v>0.7</v>
       </c>
+      <c r="R51" s="29">
+        <f t="shared" si="38"/>
+        <v>0.7</v>
+      </c>
       <c r="S51" s="58">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.7</v>
       </c>
       <c r="T51" s="54">
@@ -25447,7 +25447,7 @@
         <v>5</v>
       </c>
       <c r="AG51" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH51" s="65"/>
@@ -25459,11 +25459,11 @@
       </c>
       <c r="AL51" s="106"/>
       <c r="AM51" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AN51" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AO51" s="106" t="s">
@@ -25513,15 +25513,15 @@
         <v>0.7</v>
       </c>
       <c r="Q52" s="23">
-        <f t="shared" si="36"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="R52" s="23">
         <f t="shared" si="37"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="R52" s="23">
+        <f t="shared" si="38"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="S52" s="57">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T52" s="53">
@@ -25559,7 +25559,7 @@
         <v>5</v>
       </c>
       <c r="AG52" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH52" s="66"/>
@@ -25571,11 +25571,11 @@
       </c>
       <c r="AL52" s="106"/>
       <c r="AM52" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AN52" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AO52" s="106" t="s">
@@ -25629,20 +25629,20 @@
       </c>
       <c r="U53" s="41"/>
       <c r="V53" s="383">
-        <f>SUM(V49+0.25)</f>
-        <v>3.5</v>
+        <f>SUM(V49+0.3)</f>
+        <v>3.55</v>
       </c>
       <c r="W53" s="383">
-        <f t="shared" ref="W53:Y53" si="39">SUM(W49+0.25)</f>
-        <v>3.5</v>
+        <f>SUM(W49+0.3)</f>
+        <v>3.55</v>
       </c>
       <c r="X53" s="383">
-        <f t="shared" si="39"/>
-        <v>3.5</v>
+        <f>SUM(X49+0.3)</f>
+        <v>3.55</v>
       </c>
       <c r="Y53" s="383">
-        <f t="shared" si="39"/>
-        <v>3.5</v>
+        <f>SUM(Y49+0.3)</f>
+        <v>3.55</v>
       </c>
       <c r="Z53" s="383">
         <f>SUM(0.12+0.15)</f>
@@ -25655,7 +25655,7 @@
       <c r="AE53" s="72"/>
       <c r="AF53" s="72"/>
       <c r="AG53" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH53" s="65"/>
@@ -25667,11 +25667,11 @@
       </c>
       <c r="AL53" s="106"/>
       <c r="AM53" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AN53" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AO53" s="106" t="s">
@@ -25737,20 +25737,20 @@
       </c>
       <c r="U54" s="25"/>
       <c r="V54" s="384">
-        <f>V49*($U$152/$U$151)+0.25</f>
-        <v>3.5402892561983474</v>
+        <f>V49*($U$152/$U$151)+0.3</f>
+        <v>3.5902892561983473</v>
       </c>
       <c r="W54" s="384">
-        <f t="shared" ref="W54:Y54" si="43">W49*($U$152/$U$151)+0.25</f>
-        <v>3.5402892561983474</v>
+        <f>W49*($U$152/$U$151)+0.3</f>
+        <v>3.5902892561983473</v>
       </c>
       <c r="X54" s="384">
-        <f t="shared" si="43"/>
-        <v>3.5402892561983474</v>
+        <f>X49*($U$152/$U$151)+0.3</f>
+        <v>3.5902892561983473</v>
       </c>
       <c r="Y54" s="384">
-        <f t="shared" si="43"/>
-        <v>3.5402892561983474</v>
+        <f>Y49*($U$152/$U$151)+0.3</f>
+        <v>3.5902892561983473</v>
       </c>
       <c r="Z54" s="383">
         <f>SUM(0.12+0.15)</f>
@@ -25763,7 +25763,7 @@
       <c r="AE54" s="73"/>
       <c r="AF54" s="73"/>
       <c r="AG54" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH54" s="66"/>
@@ -25775,11 +25775,11 @@
       </c>
       <c r="AL54" s="106"/>
       <c r="AM54" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AN54" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AO54" s="106" t="s">
@@ -25857,7 +25857,7 @@
       <c r="AE55" s="72"/>
       <c r="AF55" s="72"/>
       <c r="AG55" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH55" s="65"/>
@@ -25869,11 +25869,11 @@
       </c>
       <c r="AL55" s="106"/>
       <c r="AM55" s="105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AN55" s="105" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AO55" s="106" t="s">
@@ -25919,19 +25919,19 @@
       <c r="N56" s="32"/>
       <c r="O56" s="45"/>
       <c r="P56" s="22">
-        <f t="shared" ref="P56:S60" si="44">H56*0.7</f>
+        <f t="shared" ref="P56:S60" si="43">H56*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q56" s="23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="R56" s="23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="S56" s="57">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
       <c r="T56" s="53">
@@ -25964,7 +25964,7 @@
       <c r="AE56" s="73"/>
       <c r="AF56" s="73"/>
       <c r="AG56" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH56" s="66"/>
@@ -25976,11 +25976,11 @@
       </c>
       <c r="AL56" s="109"/>
       <c r="AM56" s="108" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AN56" s="108" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AO56" s="109" t="s">
@@ -26059,7 +26059,7 @@
       <c r="AE57" s="73"/>
       <c r="AF57" s="73"/>
       <c r="AG57" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH57" s="66"/>
@@ -26074,7 +26074,7 @@
         <v>603</v>
       </c>
       <c r="AN57" s="108" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential  Stove New 1 - SH</v>
       </c>
       <c r="AO57" s="106" t="s">
@@ -26118,19 +26118,19 @@
       <c r="N58" s="32"/>
       <c r="O58" s="45"/>
       <c r="P58" s="22">
-        <f t="shared" ref="P58" si="45">H58*0.7</f>
+        <f t="shared" ref="P58" si="44">H58*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="Q58" s="23">
-        <f t="shared" ref="Q58" si="46">I58*0.7</f>
+        <f t="shared" ref="Q58" si="45">I58*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="R58" s="23">
-        <f t="shared" ref="R58" si="47">J58*0.7</f>
+        <f t="shared" ref="R58" si="46">J58*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="S58" s="57">
-        <f t="shared" ref="S58" si="48">K58*0.7</f>
+        <f t="shared" ref="S58" si="47">K58*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="T58" s="53">
@@ -26163,7 +26163,7 @@
       <c r="AE58" s="73"/>
       <c r="AF58" s="73"/>
       <c r="AG58" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH58" s="66"/>
@@ -26178,7 +26178,7 @@
         <v>604</v>
       </c>
       <c r="AN58" s="108" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential  Stove with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AO58" s="109" t="s">
@@ -26233,19 +26233,19 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="W59" s="62">
-        <f t="shared" ref="W59:Z60" si="49">W45</f>
+        <f t="shared" ref="W59:Z60" si="48">W45</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="X59" s="62">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y59" s="62">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z59" s="62">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>0.12</v>
       </c>
       <c r="AA59" s="65"/>
@@ -26267,11 +26267,11 @@
       </c>
       <c r="AL59" s="109"/>
       <c r="AM59" s="108" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SH_Att_HVO_N1</v>
       </c>
       <c r="AN59" s="108" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AO59" s="109" t="s">
@@ -26316,19 +26316,19 @@
       <c r="N60" s="50"/>
       <c r="O60" s="51"/>
       <c r="P60" s="256">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="Q60" s="26">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="R60" s="26">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="S60" s="59">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="T60" s="55">
@@ -26340,19 +26340,19 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="W60" s="62">
-        <f t="shared" ref="W60:Y60" si="50">W46</f>
+        <f t="shared" ref="W60:Y60" si="49">W46</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="X60" s="62">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y60" s="62">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Z60" s="62">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>0.12</v>
       </c>
       <c r="AA60" s="66"/>
@@ -26362,7 +26362,7 @@
       <c r="AE60" s="73"/>
       <c r="AF60" s="73"/>
       <c r="AG60" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH60" s="67"/>
@@ -26374,11 +26374,11 @@
       </c>
       <c r="AL60" s="109"/>
       <c r="AM60" s="108" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>R-SW_Att_HVO_N1</v>
       </c>
       <c r="AN60" s="108" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AO60" s="109" t="s">
@@ -26515,7 +26515,7 @@
       <c r="AE62" s="84"/>
       <c r="AF62" s="84"/>
       <c r="AG62" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AH62" s="83"/>
@@ -26527,11 +26527,11 @@
       </c>
       <c r="AL62" s="104"/>
       <c r="AM62" s="103" t="str">
-        <f t="shared" ref="AM62:AN68" si="51">C64</f>
+        <f t="shared" ref="AM62:AN68" si="50">C64</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AN62" s="103" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AO62" s="104" t="s">
@@ -26584,11 +26584,11 @@
       <c r="AJ63" s="34"/>
       <c r="AL63" s="106"/>
       <c r="AM63" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AN63" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AO63" s="106" t="s">
@@ -26673,7 +26673,7 @@
       <c r="AE64" s="85"/>
       <c r="AF64" s="85"/>
       <c r="AG64" s="85">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.220752</v>
       </c>
       <c r="AH64" s="88"/>
@@ -26685,11 +26685,11 @@
       </c>
       <c r="AL64" s="106"/>
       <c r="AM64" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AN64" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AO64" s="106" t="s">
@@ -26785,7 +26785,7 @@
       <c r="AE65" s="63"/>
       <c r="AF65" s="63"/>
       <c r="AG65" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AH65" s="66"/>
@@ -26797,11 +26797,11 @@
       </c>
       <c r="AL65" s="106"/>
       <c r="AM65" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AN65" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AO65" s="106" t="s">
@@ -26884,7 +26884,7 @@
       <c r="AE66" s="62"/>
       <c r="AF66" s="62"/>
       <c r="AG66" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.220752</v>
       </c>
       <c r="AH66" s="65"/>
@@ -26896,11 +26896,11 @@
       </c>
       <c r="AL66" s="213"/>
       <c r="AM66" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="AN66" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AO66" s="106" t="s">
@@ -26955,15 +26955,15 @@
         <v>0.7</v>
       </c>
       <c r="Q67" s="23">
-        <f t="shared" ref="Q67:Q68" si="52">I67*0.7</f>
+        <f t="shared" ref="Q67:Q68" si="51">I67*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R67" s="23">
-        <f t="shared" ref="R67:R68" si="53">J67*0.7</f>
+        <f t="shared" ref="R67:R68" si="52">J67*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S67" s="57">
-        <f t="shared" ref="S67:S68" si="54">K67*0.7</f>
+        <f t="shared" ref="S67:S68" si="53">K67*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T67" s="53">
@@ -26996,7 +26996,7 @@
       <c r="AE67" s="63"/>
       <c r="AF67" s="63"/>
       <c r="AG67" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AH67" s="66"/>
@@ -27008,11 +27008,11 @@
       </c>
       <c r="AL67" s="213"/>
       <c r="AM67" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AN67" s="105" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AO67" s="106" t="s">
@@ -27064,15 +27064,15 @@
         <v>0.7</v>
       </c>
       <c r="Q68" s="29">
+        <f t="shared" si="51"/>
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="R68" s="29">
         <f t="shared" si="52"/>
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="R68" s="29">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="S68" s="58">
         <f t="shared" si="53"/>
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="S68" s="58">
-        <f t="shared" si="54"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T68" s="54">
@@ -27110,7 +27110,7 @@
         <v>5</v>
       </c>
       <c r="AG68" s="62">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AH68" s="65"/>
@@ -27122,11 +27122,11 @@
       </c>
       <c r="AL68" s="112"/>
       <c r="AM68" s="108" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AN68" s="108" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AO68" s="109" t="s">
@@ -27212,7 +27212,7 @@
       <c r="AE69" s="63"/>
       <c r="AF69" s="63"/>
       <c r="AG69" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.220752</v>
       </c>
       <c r="AH69" s="66"/>
@@ -27326,7 +27326,7 @@
       <c r="AE70" s="86"/>
       <c r="AF70" s="86"/>
       <c r="AG70" s="86">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AH70" s="91"/>
@@ -27455,15 +27455,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q72" s="20">
-        <f t="shared" ref="Q72:Q73" si="55">I72*0.7</f>
+        <f t="shared" ref="Q72:Q73" si="54">I72*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R72" s="20">
-        <f t="shared" ref="R72:R73" si="56">J72*0.7</f>
+        <f t="shared" ref="R72:R73" si="55">J72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S72" s="56">
-        <f t="shared" ref="S72:S73" si="57">K72*0.7</f>
+        <f t="shared" ref="S72:S73" si="56">K72*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T72" s="89">
@@ -27497,7 +27497,7 @@
       <c r="AE72" s="85"/>
       <c r="AF72" s="85"/>
       <c r="AG72" s="85">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH72" s="88"/>
@@ -27569,15 +27569,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q73" s="26">
+        <f t="shared" si="54"/>
+        <v>1.2055555555555555</v>
+      </c>
+      <c r="R73" s="26">
         <f t="shared" si="55"/>
         <v>1.2055555555555555</v>
       </c>
-      <c r="R73" s="26">
+      <c r="S73" s="59">
         <f t="shared" si="56"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="S73" s="59">
-        <f t="shared" si="57"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T73" s="27">
@@ -27740,15 +27740,15 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q75" s="26">
-        <f t="shared" ref="Q75" si="58">I75*0.7</f>
+        <f t="shared" ref="Q75" si="57">I75*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R75" s="26">
-        <f t="shared" ref="R75" si="59">J75*0.7</f>
+        <f t="shared" ref="R75" si="58">J75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S75" s="59">
-        <f t="shared" ref="S75" si="60">K75*0.7</f>
+        <f t="shared" ref="S75" si="59">K75*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T75" s="3">
@@ -27759,15 +27759,15 @@
         <v>9.5138179028489738</v>
       </c>
       <c r="W75" s="79">
-        <f t="shared" ref="W75:Y75" si="61">(W67+W50)*0.8</f>
+        <f t="shared" ref="W75:Y75" si="60">(W67+W50)*0.8</f>
         <v>8.8944751180388462</v>
       </c>
       <c r="X75" s="79">
-        <f t="shared" si="61"/>
+        <f t="shared" si="60"/>
         <v>8.3308731838616321</v>
       </c>
       <c r="Y75" s="79">
-        <f t="shared" si="61"/>
+        <f t="shared" si="60"/>
         <v>8.2751323332287203</v>
       </c>
       <c r="Z75" s="375">
@@ -27788,7 +27788,7 @@
         <v>5</v>
       </c>
       <c r="AG75" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.42415920000000001</v>
       </c>
       <c r="AH75" s="83"/>
@@ -27950,7 +27950,7 @@
       <c r="AE77" s="85"/>
       <c r="AF77" s="85"/>
       <c r="AG77" s="85">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH77" s="88"/>
@@ -28035,7 +28035,7 @@
       <c r="AE78" s="64"/>
       <c r="AF78" s="64"/>
       <c r="AG78" s="64">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AH78" s="67"/>
@@ -28150,7 +28150,7 @@
       <c r="AE80" s="85"/>
       <c r="AF80" s="85"/>
       <c r="AG80" s="85">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AH80" s="88"/>
@@ -28229,7 +28229,7 @@
       <c r="AE81" s="63"/>
       <c r="AF81" s="63"/>
       <c r="AG81" s="63">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AH81" s="67"/>
@@ -28347,7 +28347,7 @@
       <c r="AE83" s="93"/>
       <c r="AF83" s="93"/>
       <c r="AG83" s="93">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AH83" s="92"/>
@@ -28510,12 +28510,12 @@
         <v>85</v>
       </c>
       <c r="U90" s="539"/>
-      <c r="V90" s="540" t="s">
+      <c r="V90" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="W90" s="541"/>
-      <c r="X90" s="541"/>
-      <c r="Y90" s="542"/>
+      <c r="W90" s="532"/>
+      <c r="X90" s="532"/>
+      <c r="Y90" s="533"/>
       <c r="Z90" s="60"/>
       <c r="AA90" s="60"/>
       <c r="AB90" s="68" t="s">
@@ -28616,34 +28616,34 @@
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="39"/>
-      <c r="H92" s="531" t="s">
+      <c r="H92" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="I92" s="532"/>
-      <c r="J92" s="532"/>
-      <c r="K92" s="533"/>
-      <c r="L92" s="532" t="s">
+      <c r="I92" s="535"/>
+      <c r="J92" s="535"/>
+      <c r="K92" s="536"/>
+      <c r="L92" s="535" t="s">
         <v>34</v>
       </c>
-      <c r="M92" s="532"/>
-      <c r="N92" s="532"/>
-      <c r="O92" s="533"/>
-      <c r="P92" s="531" t="s">
+      <c r="M92" s="535"/>
+      <c r="N92" s="535"/>
+      <c r="O92" s="536"/>
+      <c r="P92" s="534" t="s">
         <v>34</v>
       </c>
-      <c r="Q92" s="532"/>
-      <c r="R92" s="532"/>
-      <c r="S92" s="533"/>
-      <c r="T92" s="534" t="s">
+      <c r="Q92" s="535"/>
+      <c r="R92" s="535"/>
+      <c r="S92" s="536"/>
+      <c r="T92" s="540" t="s">
         <v>68</v>
       </c>
-      <c r="U92" s="535"/>
-      <c r="V92" s="534" t="s">
+      <c r="U92" s="541"/>
+      <c r="V92" s="540" t="s">
         <v>541</v>
       </c>
-      <c r="W92" s="536"/>
-      <c r="X92" s="536"/>
-      <c r="Y92" s="535"/>
+      <c r="W92" s="542"/>
+      <c r="X92" s="542"/>
+      <c r="Y92" s="541"/>
       <c r="Z92" s="377" t="s">
         <v>553</v>
       </c>
@@ -28739,15 +28739,15 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="W93" s="383">
-        <f t="shared" ref="W93:Y93" si="62">W97*1.3</f>
+        <f t="shared" ref="W93:Y93" si="61">W97*1.3</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="X93" s="383">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y93" s="383">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z93" s="383">
@@ -28760,7 +28760,7 @@
       <c r="AE93" s="72"/>
       <c r="AF93" s="72"/>
       <c r="AG93" s="62">
-        <f t="shared" ref="AG93:AG131" si="63">31.536*(AJ93/1000)</f>
+        <f t="shared" ref="AG93:AG131" si="62">31.536*(AJ93/1000)</f>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH93" s="65"/>
@@ -28828,15 +28828,15 @@
         <v>0.7</v>
       </c>
       <c r="Q94" s="23">
-        <f t="shared" ref="Q94:Q96" si="64">I94*0.7</f>
+        <f t="shared" ref="Q94:Q96" si="63">I94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R94" s="23">
-        <f t="shared" ref="R94:R96" si="65">J94*0.7</f>
+        <f t="shared" ref="R94:R96" si="64">J94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S94" s="57">
-        <f t="shared" ref="S94:S96" si="66">K94*0.7</f>
+        <f t="shared" ref="S94:S96" si="65">K94*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T94" s="53">
@@ -28848,15 +28848,15 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="W94" s="384">
-        <f t="shared" ref="W94:Y94" si="67">W98*1.3</f>
+        <f t="shared" ref="W94:Y94" si="66">W98*1.3</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="X94" s="384">
-        <f t="shared" si="67"/>
+        <f t="shared" si="66"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y94" s="384">
-        <f t="shared" si="67"/>
+        <f t="shared" si="66"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z94" s="384">
@@ -28869,7 +28869,7 @@
       <c r="AE94" s="73"/>
       <c r="AF94" s="73"/>
       <c r="AG94" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH94" s="66"/>
@@ -28881,11 +28881,11 @@
       </c>
       <c r="AL94" s="106"/>
       <c r="AM94" s="105" t="str">
-        <f t="shared" ref="AM94:AM108" si="68">C94</f>
+        <f t="shared" ref="AM94:AM108" si="67">C94</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AN94" s="105" t="str">
-        <f t="shared" ref="AN94:AN108" si="69">D94</f>
+        <f t="shared" ref="AN94:AN108" si="68">D94</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AO94" s="106" t="s">
@@ -28935,15 +28935,15 @@
         <v>0.7</v>
       </c>
       <c r="Q95" s="29">
+        <f t="shared" si="63"/>
+        <v>0.7</v>
+      </c>
+      <c r="R95" s="29">
         <f t="shared" si="64"/>
         <v>0.7</v>
       </c>
-      <c r="R95" s="29">
+      <c r="S95" s="58">
         <f t="shared" si="65"/>
-        <v>0.7</v>
-      </c>
-      <c r="S95" s="58">
-        <f t="shared" si="66"/>
         <v>0.7</v>
       </c>
       <c r="T95" s="54">
@@ -28981,7 +28981,7 @@
         <v>5</v>
       </c>
       <c r="AG95" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH95" s="65"/>
@@ -28993,11 +28993,11 @@
       </c>
       <c r="AL95" s="106"/>
       <c r="AM95" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_KER_N2</v>
+      </c>
+      <c r="AN95" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_KER_N2</v>
-      </c>
-      <c r="AN95" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AO95" s="106" t="s">
@@ -29047,15 +29047,15 @@
         <v>0.7</v>
       </c>
       <c r="Q96" s="23">
+        <f t="shared" si="63"/>
+        <v>0.71749999999999992</v>
+      </c>
+      <c r="R96" s="23">
         <f t="shared" si="64"/>
         <v>0.71749999999999992</v>
       </c>
-      <c r="R96" s="23">
+      <c r="S96" s="57">
         <f t="shared" si="65"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S96" s="57">
-        <f t="shared" si="66"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T96" s="53">
@@ -29093,7 +29093,7 @@
         <v>5</v>
       </c>
       <c r="AG96" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH96" s="66"/>
@@ -29105,11 +29105,11 @@
       </c>
       <c r="AL96" s="106"/>
       <c r="AM96" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_KER_N3</v>
+      </c>
+      <c r="AN96" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_KER_N3</v>
-      </c>
-      <c r="AN96" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AO96" s="107" t="s">
@@ -29165,15 +29165,15 @@
         <v>3.5249999999999999</v>
       </c>
       <c r="W97" s="383">
-        <f t="shared" ref="W97:Y97" si="70">3.525</f>
+        <f t="shared" ref="W97:Y97" si="69">3.525</f>
         <v>3.5249999999999999</v>
       </c>
       <c r="X97" s="383">
-        <f t="shared" si="70"/>
+        <f t="shared" si="69"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Y97" s="383">
-        <f t="shared" si="70"/>
+        <f t="shared" si="69"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Z97" s="383">
@@ -29186,7 +29186,7 @@
       <c r="AE97" s="72"/>
       <c r="AF97" s="72"/>
       <c r="AG97" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH97" s="65"/>
@@ -29198,11 +29198,11 @@
       </c>
       <c r="AL97" s="106"/>
       <c r="AM97" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SH_Det_GAS_N1</v>
+      </c>
+      <c r="AN97" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SH_Det_GAS_N1</v>
-      </c>
-      <c r="AN97" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AO97" s="106" t="s">
@@ -29252,15 +29252,15 @@
         <v>0.7</v>
       </c>
       <c r="Q98" s="23">
-        <f t="shared" ref="Q98:Q100" si="71">I98*0.7</f>
+        <f t="shared" ref="Q98:Q100" si="70">I98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R98" s="23">
-        <f t="shared" ref="R98:R100" si="72">J98*0.7</f>
+        <f t="shared" ref="R98:R100" si="71">J98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S98" s="57">
-        <f t="shared" ref="S98:S100" si="73">K98*0.7</f>
+        <f t="shared" ref="S98:S100" si="72">K98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T98" s="53">
@@ -29293,7 +29293,7 @@
       <c r="AE98" s="73"/>
       <c r="AF98" s="73"/>
       <c r="AG98" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH98" s="66"/>
@@ -29305,11 +29305,11 @@
       </c>
       <c r="AL98" s="106"/>
       <c r="AM98" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_GAS_N1</v>
+      </c>
+      <c r="AN98" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_GAS_N1</v>
-      </c>
-      <c r="AN98" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AO98" s="106" t="s">
@@ -29359,15 +29359,15 @@
         <v>0.7</v>
       </c>
       <c r="Q99" s="29">
+        <f t="shared" si="70"/>
+        <v>0.7</v>
+      </c>
+      <c r="R99" s="29">
         <f t="shared" si="71"/>
         <v>0.7</v>
       </c>
-      <c r="R99" s="29">
+      <c r="S99" s="58">
         <f t="shared" si="72"/>
-        <v>0.7</v>
-      </c>
-      <c r="S99" s="58">
-        <f t="shared" si="73"/>
         <v>0.7</v>
       </c>
       <c r="T99" s="54">
@@ -29403,7 +29403,7 @@
         <v>5</v>
       </c>
       <c r="AG99" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH99" s="65"/>
@@ -29415,11 +29415,11 @@
       </c>
       <c r="AL99" s="106"/>
       <c r="AM99" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_GAS_N2</v>
+      </c>
+      <c r="AN99" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_GAS_N2</v>
-      </c>
-      <c r="AN99" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AO99" s="106" t="s">
@@ -29469,15 +29469,15 @@
         <v>0.7</v>
       </c>
       <c r="Q100" s="23">
+        <f t="shared" si="70"/>
+        <v>0.71749999999999992</v>
+      </c>
+      <c r="R100" s="23">
         <f t="shared" si="71"/>
         <v>0.71749999999999992</v>
       </c>
-      <c r="R100" s="23">
+      <c r="S100" s="57">
         <f t="shared" si="72"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S100" s="57">
-        <f t="shared" si="73"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="T100" s="53">
@@ -29515,7 +29515,7 @@
         <v>5</v>
       </c>
       <c r="AG100" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH100" s="66"/>
@@ -29527,11 +29527,11 @@
       </c>
       <c r="AL100" s="106"/>
       <c r="AM100" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_GAS_N3</v>
+      </c>
+      <c r="AN100" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_GAS_N3</v>
-      </c>
-      <c r="AN100" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AO100" s="106" t="s">
@@ -29585,20 +29585,20 @@
       </c>
       <c r="U101" s="41"/>
       <c r="V101" s="383">
-        <f>V97+0.25</f>
-        <v>3.7749999999999999</v>
+        <f>V97+0.3</f>
+        <v>3.8249999999999997</v>
       </c>
       <c r="W101" s="383">
-        <f t="shared" ref="W101:Y101" si="74">W97+0.25</f>
-        <v>3.7749999999999999</v>
+        <f>W97+0.3</f>
+        <v>3.8249999999999997</v>
       </c>
       <c r="X101" s="383">
-        <f t="shared" si="74"/>
-        <v>3.7749999999999999</v>
+        <f>X97+0.3</f>
+        <v>3.8249999999999997</v>
       </c>
       <c r="Y101" s="383">
-        <f t="shared" si="74"/>
-        <v>3.7749999999999999</v>
+        <f>Y97+0.3</f>
+        <v>3.8249999999999997</v>
       </c>
       <c r="Z101" s="383">
         <f>SUM(0.12+0.15)</f>
@@ -29611,7 +29611,7 @@
       <c r="AE101" s="72"/>
       <c r="AF101" s="72"/>
       <c r="AG101" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH101" s="65"/>
@@ -29623,11 +29623,11 @@
       </c>
       <c r="AL101" s="106"/>
       <c r="AM101" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SH_Det_LPG_N1</v>
+      </c>
+      <c r="AN101" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SH_Det_LPG_N1</v>
-      </c>
-      <c r="AN101" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AO101" s="106" t="s">
@@ -29677,15 +29677,15 @@
         <v>0.7</v>
       </c>
       <c r="Q102" s="23">
-        <f t="shared" ref="Q102" si="75">I102*0.7</f>
+        <f t="shared" ref="Q102" si="73">I102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R102" s="23">
-        <f t="shared" ref="R102" si="76">J102*0.7</f>
+        <f t="shared" ref="R102" si="74">J102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S102" s="57">
-        <f t="shared" ref="S102" si="77">K102*0.7</f>
+        <f t="shared" ref="S102" si="75">K102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T102" s="53">
@@ -29693,20 +29693,20 @@
       </c>
       <c r="U102" s="25"/>
       <c r="V102" s="384">
-        <f>V98</f>
-        <v>3.8040057915057912</v>
+        <f>V98+0.3</f>
+        <v>4.1040057915057915</v>
       </c>
       <c r="W102" s="384">
-        <f t="shared" ref="W102:Y102" si="78">W98</f>
-        <v>3.8040057915057912</v>
+        <f>W98+0.3</f>
+        <v>4.1040057915057915</v>
       </c>
       <c r="X102" s="384">
-        <f t="shared" si="78"/>
-        <v>3.8040057915057912</v>
+        <f>X98+0.3</f>
+        <v>4.1040057915057915</v>
       </c>
       <c r="Y102" s="384">
-        <f t="shared" si="78"/>
-        <v>3.8040057915057912</v>
+        <f>Y98+0.3</f>
+        <v>4.1040057915057915</v>
       </c>
       <c r="Z102" s="383">
         <f>SUM(0.12+0.15)</f>
@@ -29719,7 +29719,7 @@
       <c r="AE102" s="73"/>
       <c r="AF102" s="73"/>
       <c r="AG102" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH102" s="66"/>
@@ -29731,11 +29731,11 @@
       </c>
       <c r="AL102" s="106"/>
       <c r="AM102" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_LPG_N1</v>
+      </c>
+      <c r="AN102" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_LPG_N1</v>
-      </c>
-      <c r="AN102" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AO102" s="106" t="s">
@@ -29813,7 +29813,7 @@
       <c r="AE103" s="72"/>
       <c r="AF103" s="72"/>
       <c r="AG103" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH103" s="65"/>
@@ -29825,11 +29825,11 @@
       </c>
       <c r="AL103" s="106"/>
       <c r="AM103" s="105" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SH_Det_WOO_N1</v>
+      </c>
+      <c r="AN103" s="105" t="str">
         <f t="shared" si="68"/>
-        <v>R-SH_Det_WOO_N1</v>
-      </c>
-      <c r="AN103" s="105" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AO103" s="106" t="s">
@@ -29875,19 +29875,19 @@
       <c r="N104" s="32"/>
       <c r="O104" s="45"/>
       <c r="P104" s="22">
-        <f t="shared" ref="P104:S104" si="79">H104*0.7</f>
+        <f t="shared" ref="P104:S104" si="76">H104*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q104" s="23">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="23">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="57">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0.7</v>
       </c>
       <c r="T104" s="53">
@@ -29899,15 +29899,15 @@
         <v>22.778925619834713</v>
       </c>
       <c r="W104" s="384">
-        <f t="shared" ref="W104" si="80">W103*($U$152/$U$151)</f>
+        <f t="shared" ref="W104" si="77">W103*($U$152/$U$151)</f>
         <v>22.04476084710744</v>
       </c>
       <c r="X104" s="384">
-        <f t="shared" ref="X104" si="81">X103*($U$152/$U$151)</f>
+        <f t="shared" ref="X104" si="78">X103*($U$152/$U$151)</f>
         <v>20.839163429752066</v>
       </c>
       <c r="Y104" s="384">
-        <f t="shared" ref="Y104" si="82">Y103*($U$152/$U$151)</f>
+        <f t="shared" ref="Y104" si="79">Y103*($U$152/$U$151)</f>
         <v>18.635439049586779</v>
       </c>
       <c r="Z104" s="384">
@@ -29920,7 +29920,7 @@
       <c r="AE104" s="73"/>
       <c r="AF104" s="73"/>
       <c r="AG104" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH104" s="66"/>
@@ -29932,11 +29932,11 @@
       </c>
       <c r="AL104" s="109"/>
       <c r="AM104" s="108" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_WOO_N1</v>
+      </c>
+      <c r="AN104" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_WOO_N1</v>
-      </c>
-      <c r="AN104" s="108" t="str">
-        <f t="shared" si="69"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AO104" s="109" t="s">
@@ -30015,7 +30015,7 @@
       <c r="AE105" s="73"/>
       <c r="AF105" s="73"/>
       <c r="AG105" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH105" s="66"/>
@@ -30030,7 +30030,7 @@
         <v>611</v>
       </c>
       <c r="AN105" s="108" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="68"/>
         <v>Residential  Stove New 1 - SH</v>
       </c>
       <c r="AO105" s="106" t="s">
@@ -30074,19 +30074,19 @@
       <c r="N106" s="32"/>
       <c r="O106" s="45"/>
       <c r="P106" s="22">
-        <f t="shared" ref="P106:P108" si="83">H106*0.7</f>
+        <f t="shared" ref="P106:P108" si="80">H106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="Q106" s="23">
-        <f t="shared" ref="Q106:Q108" si="84">I106*0.7</f>
+        <f t="shared" ref="Q106:Q108" si="81">I106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="R106" s="23">
-        <f t="shared" ref="R106:R108" si="85">J106*0.7</f>
+        <f t="shared" ref="R106:R108" si="82">J106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="S106" s="57">
-        <f t="shared" ref="S106:S108" si="86">K106*0.7</f>
+        <f t="shared" ref="S106:S108" si="83">K106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="T106" s="53">
@@ -30119,7 +30119,7 @@
       <c r="AE106" s="73"/>
       <c r="AF106" s="73"/>
       <c r="AG106" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH106" s="66"/>
@@ -30134,7 +30134,7 @@
         <v>612</v>
       </c>
       <c r="AN106" s="108" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="68"/>
         <v>Residential  Stove with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AO106" s="109" t="s">
@@ -30189,19 +30189,19 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="W107" s="62">
-        <f t="shared" ref="W107:Z107" si="87">W93</f>
+        <f t="shared" ref="W107:Z107" si="84">W93</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="X107" s="62">
-        <f t="shared" si="87"/>
+        <f t="shared" si="84"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y107" s="62">
-        <f t="shared" si="87"/>
+        <f t="shared" si="84"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z107" s="62">
-        <f t="shared" si="87"/>
+        <f t="shared" si="84"/>
         <v>0.12</v>
       </c>
       <c r="AA107" s="65"/>
@@ -30211,7 +30211,7 @@
       <c r="AE107" s="72"/>
       <c r="AF107" s="72"/>
       <c r="AG107" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH107" s="65"/>
@@ -30223,11 +30223,11 @@
       </c>
       <c r="AL107" s="109"/>
       <c r="AM107" s="108" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SH_Det_HVO_N1</v>
+      </c>
+      <c r="AN107" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>R-SH_Det_HVO_N1</v>
-      </c>
-      <c r="AN107" s="108" t="str">
-        <f t="shared" si="69"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AO107" s="109" t="s">
@@ -30272,19 +30272,19 @@
       <c r="N108" s="50"/>
       <c r="O108" s="51"/>
       <c r="P108" s="256">
+        <f t="shared" si="80"/>
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="Q108" s="26">
+        <f t="shared" si="81"/>
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="R108" s="26">
+        <f t="shared" si="82"/>
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="S108" s="59">
         <f t="shared" si="83"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="Q108" s="26">
-        <f t="shared" si="84"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="R108" s="26">
-        <f t="shared" si="85"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="S108" s="59">
-        <f t="shared" si="86"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="T108" s="55">
@@ -30296,19 +30296,19 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="W108" s="62">
-        <f t="shared" ref="W108:Z108" si="88">W94</f>
+        <f t="shared" ref="W108:Z108" si="85">W94</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="X108" s="62">
-        <f t="shared" si="88"/>
+        <f t="shared" si="85"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y108" s="62">
-        <f t="shared" si="88"/>
+        <f t="shared" si="85"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z108" s="62">
-        <f t="shared" si="88"/>
+        <f t="shared" si="85"/>
         <v>0.12</v>
       </c>
       <c r="AA108" s="66"/>
@@ -30318,7 +30318,7 @@
       <c r="AE108" s="73"/>
       <c r="AF108" s="73"/>
       <c r="AG108" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH108" s="67"/>
@@ -30330,11 +30330,11 @@
       </c>
       <c r="AL108" s="109"/>
       <c r="AM108" s="108" t="str">
+        <f t="shared" si="67"/>
+        <v>R-SW_Det_HVO_N1</v>
+      </c>
+      <c r="AN108" s="108" t="str">
         <f t="shared" si="68"/>
-        <v>R-SW_Det_HVO_N1</v>
-      </c>
-      <c r="AN108" s="108" t="str">
-        <f t="shared" si="69"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AO108" s="109" t="s">
@@ -30471,7 +30471,7 @@
       <c r="AE110" s="84"/>
       <c r="AF110" s="84"/>
       <c r="AG110" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AH110" s="83"/>
@@ -30483,11 +30483,11 @@
       </c>
       <c r="AL110" s="104"/>
       <c r="AM110" s="103" t="str">
-        <f t="shared" ref="AM110:AM116" si="89">C112</f>
+        <f t="shared" ref="AM110:AM116" si="86">C112</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AN110" s="103" t="str">
-        <f t="shared" ref="AN110:AN116" si="90">D112</f>
+        <f t="shared" ref="AN110:AN116" si="87">D112</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AO110" s="104" t="s">
@@ -30540,11 +30540,11 @@
       <c r="AJ111" s="34"/>
       <c r="AL111" s="106"/>
       <c r="AM111" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AN111" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AO111" s="106" t="s">
@@ -30626,7 +30626,7 @@
       <c r="AE112" s="85"/>
       <c r="AF112" s="85"/>
       <c r="AG112" s="85">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AH112" s="88"/>
@@ -30638,11 +30638,11 @@
       </c>
       <c r="AL112" s="106"/>
       <c r="AM112" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AN112" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AO112" s="106" t="s">
@@ -30732,7 +30732,7 @@
       <c r="AE113" s="63"/>
       <c r="AF113" s="63"/>
       <c r="AG113" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AH113" s="66"/>
@@ -30744,11 +30744,11 @@
       </c>
       <c r="AL113" s="106"/>
       <c r="AM113" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AN113" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AO113" s="106" t="s">
@@ -30828,7 +30828,7 @@
       <c r="AE114" s="62"/>
       <c r="AF114" s="62"/>
       <c r="AG114" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AH114" s="65"/>
@@ -30840,11 +30840,11 @@
       </c>
       <c r="AL114" s="213"/>
       <c r="AM114" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AN114" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AO114" s="106" t="s">
@@ -30896,15 +30896,15 @@
         <v>0.7</v>
       </c>
       <c r="Q115" s="23">
-        <f t="shared" ref="Q115:Q116" si="91">I115*0.7</f>
+        <f t="shared" ref="Q115:Q116" si="88">I115*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R115" s="23">
-        <f t="shared" ref="R115:R116" si="92">J115*0.7</f>
+        <f t="shared" ref="R115:R116" si="89">J115*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S115" s="57">
-        <f t="shared" ref="S115:S116" si="93">K115*0.7</f>
+        <f t="shared" ref="S115:S116" si="90">K115*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T115" s="53">
@@ -30916,15 +30916,15 @@
         <v>9.9300970464135023</v>
       </c>
       <c r="W115" s="384">
-        <f t="shared" ref="W115" si="94">W114*($U$150/$U$149)</f>
+        <f t="shared" ref="W115" si="91">W114*($U$150/$U$149)</f>
         <v>9.0363883122362889</v>
       </c>
       <c r="X115" s="384">
-        <f t="shared" ref="X115" si="95">X114*($U$150/$U$149)</f>
+        <f t="shared" ref="X115" si="92">X114*($U$150/$U$149)</f>
         <v>8.2231133641350223</v>
       </c>
       <c r="Y115" s="384">
-        <f t="shared" ref="Y115" si="96">Y114*($U$150/$U$149)</f>
+        <f t="shared" ref="Y115" si="93">Y114*($U$150/$U$149)</f>
         <v>8.1426795780590719</v>
       </c>
       <c r="Z115" s="384">
@@ -30937,7 +30937,7 @@
       <c r="AE115" s="63"/>
       <c r="AF115" s="63"/>
       <c r="AG115" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AH115" s="66"/>
@@ -30949,11 +30949,11 @@
       </c>
       <c r="AL115" s="213"/>
       <c r="AM115" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AN115" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AO115" s="106" t="s">
@@ -31005,15 +31005,15 @@
         <v>0.7</v>
       </c>
       <c r="Q116" s="29">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R116" s="29">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S116" s="58">
-        <f t="shared" si="93"/>
+        <f t="shared" si="90"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T116" s="54">
@@ -31051,7 +31051,7 @@
         <v>5</v>
       </c>
       <c r="AG116" s="62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AH116" s="65"/>
@@ -31063,11 +31063,11 @@
       </c>
       <c r="AL116" s="112"/>
       <c r="AM116" s="108" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AN116" s="108" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AO116" s="109" t="s">
@@ -31149,7 +31149,7 @@
       <c r="AE117" s="63"/>
       <c r="AF117" s="63"/>
       <c r="AG117" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AH117" s="66"/>
@@ -31255,7 +31255,7 @@
       <c r="AE118" s="86"/>
       <c r="AF118" s="86"/>
       <c r="AG118" s="86">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AH118" s="91"/>
@@ -31384,15 +31384,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q120" s="20">
-        <f t="shared" ref="Q120:Q121" si="97">I120*0.7</f>
+        <f t="shared" ref="Q120:Q121" si="94">I120*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R120" s="20">
-        <f t="shared" ref="R120:R121" si="98">J120*0.7</f>
+        <f t="shared" ref="R120:R121" si="95">J120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S120" s="56">
-        <f t="shared" ref="S120:S121" si="99">K120*0.7</f>
+        <f t="shared" ref="S120:S121" si="96">K120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T120" s="89">
@@ -31426,7 +31426,7 @@
       <c r="AE120" s="85"/>
       <c r="AF120" s="85"/>
       <c r="AG120" s="85">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH120" s="88"/>
@@ -31498,15 +31498,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q121" s="26">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>1.2055555555555555</v>
       </c>
       <c r="R121" s="26">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>1.2055555555555555</v>
       </c>
       <c r="S121" s="59">
-        <f t="shared" si="99"/>
+        <f t="shared" si="96"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T121" s="27">
@@ -31540,7 +31540,7 @@
       <c r="AE121" s="64"/>
       <c r="AF121" s="64"/>
       <c r="AG121" s="64">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH121" s="67"/>
@@ -31609,11 +31609,11 @@
       <c r="AJ122" s="34"/>
       <c r="AL122" s="216"/>
       <c r="AM122" s="103" t="str">
-        <f t="shared" ref="AM122:AM123" si="100">C128</f>
+        <f t="shared" ref="AM122:AM123" si="97">C128</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AN122" s="103" t="str">
-        <f t="shared" ref="AN122:AN123" si="101">D128</f>
+        <f t="shared" ref="AN122:AN123" si="98">D128</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AO122" s="104" t="s">
@@ -31669,15 +31669,15 @@
         <v>2.2889999999999997</v>
       </c>
       <c r="Q123" s="26">
-        <f t="shared" ref="Q123" si="102">I123*0.7</f>
+        <f t="shared" ref="Q123" si="99">I123*0.7</f>
         <v>2.5409999999999995</v>
       </c>
       <c r="R123" s="26">
-        <f t="shared" ref="R123" si="103">J123*0.7</f>
+        <f t="shared" ref="R123" si="100">J123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="S123" s="59">
-        <f t="shared" ref="S123" si="104">K123*0.7</f>
+        <f t="shared" ref="S123" si="101">K123*0.7</f>
         <v>2.7299999999999995</v>
       </c>
       <c r="T123" s="3">
@@ -31688,15 +31688,15 @@
         <v>10.987282270335434</v>
       </c>
       <c r="W123" s="79">
-        <f t="shared" ref="W123:Y123" si="105">(W115+W98)*0.8</f>
+        <f t="shared" ref="W123:Y123" si="102">(W115+W98)*0.8</f>
         <v>10.272315282993665</v>
       </c>
       <c r="X123" s="79">
-        <f t="shared" si="105"/>
+        <f t="shared" si="102"/>
         <v>9.6216953245126504</v>
       </c>
       <c r="Y123" s="79">
-        <f t="shared" si="105"/>
+        <f t="shared" si="102"/>
         <v>9.5573482956518898</v>
       </c>
       <c r="Z123" s="375">
@@ -31717,7 +31717,7 @@
         <v>5</v>
       </c>
       <c r="AG123" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.62441279999999999</v>
       </c>
       <c r="AH123" s="83"/>
@@ -31730,11 +31730,11 @@
       </c>
       <c r="AL123" s="2"/>
       <c r="AM123" s="105" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="97"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AN123" s="105" t="str">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AO123" s="106" t="s">
@@ -31879,7 +31879,7 @@
       <c r="AE125" s="85"/>
       <c r="AF125" s="85"/>
       <c r="AG125" s="85">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH125" s="88"/>
@@ -31964,7 +31964,7 @@
       <c r="AE126" s="64"/>
       <c r="AF126" s="64"/>
       <c r="AG126" s="64">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AH126" s="67"/>
@@ -32079,7 +32079,7 @@
       <c r="AE128" s="85"/>
       <c r="AF128" s="85"/>
       <c r="AG128" s="85">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AH128" s="88"/>
@@ -32158,7 +32158,7 @@
       <c r="AE129" s="63"/>
       <c r="AF129" s="63"/>
       <c r="AG129" s="63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AH129" s="67"/>
@@ -32273,7 +32273,7 @@
       <c r="AE131" s="93"/>
       <c r="AF131" s="93"/>
       <c r="AG131" s="93">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AH131" s="92"/>
@@ -32354,7 +32354,7 @@
         <v>3</v>
       </c>
       <c r="U145" s="381">
-        <f t="shared" ref="U145:U154" si="106">V145/$V$153</f>
+        <f t="shared" ref="U145:U154" si="103">V145/$V$153</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="V145" s="382">
@@ -32368,7 +32368,7 @@
         <v>5</v>
       </c>
       <c r="U146" s="381">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="V146" s="382">
@@ -32381,7 +32381,7 @@
         <v>8</v>
       </c>
       <c r="U147" s="381">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="V147" s="382">
@@ -32395,7 +32395,7 @@
         <v>10</v>
       </c>
       <c r="U148" s="381">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="V148" s="380">
@@ -32416,7 +32416,7 @@
         <v>15</v>
       </c>
       <c r="U149" s="371">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="V149" s="3">
@@ -32443,7 +32443,7 @@
         <v>18</v>
       </c>
       <c r="U150" s="371">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="V150" s="3">
@@ -32472,7 +32472,7 @@
         <v>20</v>
       </c>
       <c r="U151" s="381">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="V151" s="380">
@@ -32502,7 +32502,7 @@
         <v>24</v>
       </c>
       <c r="U152" s="371">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="V152" s="3">
@@ -32531,7 +32531,7 @@
         <v>30</v>
       </c>
       <c r="U153" s="371">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>1</v>
       </c>
       <c r="V153" s="3">
@@ -32560,7 +32560,7 @@
         <v>35</v>
       </c>
       <c r="U154" s="371">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="V154" s="3">
@@ -32605,6 +32605,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -32615,26 +32635,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -32780,12 +32780,12 @@
       <c r="I5" s="127"/>
       <c r="J5" s="127"/>
       <c r="K5" s="127"/>
-      <c r="L5" s="540" t="s">
+      <c r="L5" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="541"/>
-      <c r="N5" s="541"/>
-      <c r="O5" s="542"/>
+      <c r="M5" s="532"/>
+      <c r="N5" s="532"/>
+      <c r="O5" s="533"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -32816,12 +32816,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="534" t="s">
+      <c r="L6" s="540" t="s">
         <v>541</v>
       </c>
-      <c r="M6" s="536"/>
-      <c r="N6" s="536"/>
-      <c r="O6" s="535"/>
+      <c r="M6" s="542"/>
+      <c r="N6" s="542"/>
+      <c r="O6" s="541"/>
       <c r="P6" s="377" t="s">
         <v>553</v>
       </c>
@@ -33707,23 +33707,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="540" t="s">
+      <c r="L33" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="541"/>
-      <c r="N33" s="541"/>
-      <c r="O33" s="542"/>
+      <c r="M33" s="532"/>
+      <c r="N33" s="532"/>
+      <c r="O33" s="533"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L34" s="534" t="s">
+      <c r="L34" s="540" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="536"/>
-      <c r="N34" s="536"/>
-      <c r="O34" s="535"/>
+      <c r="M34" s="542"/>
+      <c r="N34" s="542"/>
+      <c r="O34" s="541"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -34070,11 +34070,11 @@
       </c>
       <c r="I4" s="538"/>
       <c r="J4" s="539"/>
-      <c r="K4" s="540" t="s">
+      <c r="K4" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="541"/>
-      <c r="M4" s="542"/>
+      <c r="L4" s="532"/>
+      <c r="M4" s="533"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -34100,16 +34100,16 @@
       <c r="G5" s="385" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="546" t="s">
+      <c r="H5" s="543" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="547"/>
-      <c r="J5" s="548"/>
-      <c r="K5" s="546" t="s">
+      <c r="I5" s="544"/>
+      <c r="J5" s="545"/>
+      <c r="K5" s="543" t="s">
         <v>330</v>
       </c>
-      <c r="L5" s="547"/>
-      <c r="M5" s="548"/>
+      <c r="L5" s="544"/>
+      <c r="M5" s="545"/>
       <c r="N5" s="386" t="s">
         <v>92</v>
       </c>
@@ -34126,23 +34126,23 @@
         <v>218</v>
       </c>
       <c r="AA5" s="208"/>
-      <c r="AB5" s="543" t="s">
+      <c r="AB5" s="546" t="s">
         <v>583</v>
       </c>
-      <c r="AC5" s="543"/>
+      <c r="AC5" s="546"/>
       <c r="AD5" s="388"/>
-      <c r="AE5" s="544" t="s">
+      <c r="AE5" s="547" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="544"/>
-      <c r="AG5" s="544" t="s">
+      <c r="AF5" s="547"/>
+      <c r="AG5" s="547" t="s">
         <v>584</v>
       </c>
-      <c r="AH5" s="544"/>
-      <c r="AI5" s="545" t="s">
+      <c r="AH5" s="547"/>
+      <c r="AI5" s="548" t="s">
         <v>585</v>
       </c>
-      <c r="AJ5" s="545"/>
+      <c r="AJ5" s="548"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="432" t="str">
@@ -34880,12 +34880,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="540" t="s">
+      <c r="L27" s="531" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="541"/>
-      <c r="N27" s="541"/>
-      <c r="O27" s="542"/>
+      <c r="M27" s="532"/>
+      <c r="N27" s="532"/>
+      <c r="O27" s="533"/>
       <c r="T27" s="210"/>
       <c r="U27" s="210"/>
     </row>
@@ -34893,12 +34893,12 @@
       <c r="J28" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L28" s="531" t="s">
+      <c r="L28" s="534" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="532"/>
-      <c r="N28" s="532"/>
-      <c r="O28" s="533"/>
+      <c r="M28" s="535"/>
+      <c r="N28" s="535"/>
+      <c r="O28" s="536"/>
       <c r="T28" s="210"/>
       <c r="U28" s="210"/>
     </row>
@@ -36288,16 +36288,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -36728,103 +36728,103 @@
       <c r="C4" s="283" t="s">
         <v>339</v>
       </c>
-      <c r="D4" s="550" t="s">
+      <c r="D4" s="549" t="s">
         <v>340</v>
       </c>
-      <c r="E4" s="549"/>
-      <c r="F4" s="549"/>
-      <c r="G4" s="549"/>
+      <c r="E4" s="550"/>
+      <c r="F4" s="550"/>
+      <c r="G4" s="550"/>
       <c r="H4" s="551"/>
-      <c r="I4" s="549" t="s">
+      <c r="I4" s="550" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="549"/>
-      <c r="K4" s="549"/>
-      <c r="L4" s="549"/>
+      <c r="J4" s="550"/>
+      <c r="K4" s="550"/>
+      <c r="L4" s="550"/>
       <c r="M4" s="551"/>
-      <c r="N4" s="549" t="s">
+      <c r="N4" s="550" t="s">
         <v>342</v>
       </c>
-      <c r="O4" s="549"/>
-      <c r="P4" s="549"/>
-      <c r="Q4" s="549"/>
+      <c r="O4" s="550"/>
+      <c r="P4" s="550"/>
+      <c r="Q4" s="550"/>
       <c r="R4" s="551"/>
-      <c r="S4" s="549" t="s">
+      <c r="S4" s="550" t="s">
         <v>343</v>
       </c>
-      <c r="T4" s="549"/>
-      <c r="U4" s="549"/>
-      <c r="V4" s="549"/>
+      <c r="T4" s="550"/>
+      <c r="U4" s="550"/>
+      <c r="V4" s="550"/>
       <c r="W4" s="551"/>
-      <c r="X4" s="549" t="s">
+      <c r="X4" s="550" t="s">
         <v>344</v>
       </c>
-      <c r="Y4" s="549"/>
-      <c r="Z4" s="549"/>
-      <c r="AA4" s="549"/>
+      <c r="Y4" s="550"/>
+      <c r="Z4" s="550"/>
+      <c r="AA4" s="550"/>
       <c r="AB4" s="551"/>
-      <c r="AC4" s="549" t="s">
+      <c r="AC4" s="550" t="s">
         <v>345</v>
       </c>
-      <c r="AD4" s="549"/>
-      <c r="AE4" s="549"/>
-      <c r="AF4" s="549"/>
+      <c r="AD4" s="550"/>
+      <c r="AE4" s="550"/>
+      <c r="AF4" s="550"/>
       <c r="AG4" s="551"/>
-      <c r="AH4" s="549" t="s">
+      <c r="AH4" s="550" t="s">
         <v>346</v>
       </c>
-      <c r="AI4" s="549"/>
-      <c r="AJ4" s="549"/>
-      <c r="AK4" s="549"/>
+      <c r="AI4" s="550"/>
+      <c r="AJ4" s="550"/>
+      <c r="AK4" s="550"/>
       <c r="AL4" s="551"/>
-      <c r="AM4" s="549" t="s">
+      <c r="AM4" s="550" t="s">
         <v>347</v>
       </c>
-      <c r="AN4" s="549"/>
-      <c r="AO4" s="549"/>
-      <c r="AP4" s="549"/>
+      <c r="AN4" s="550"/>
+      <c r="AO4" s="550"/>
+      <c r="AP4" s="550"/>
       <c r="AQ4" s="551"/>
-      <c r="AR4" s="549" t="s">
+      <c r="AR4" s="550" t="s">
         <v>348</v>
       </c>
-      <c r="AS4" s="549"/>
-      <c r="AT4" s="549"/>
-      <c r="AU4" s="549"/>
+      <c r="AS4" s="550"/>
+      <c r="AT4" s="550"/>
+      <c r="AU4" s="550"/>
       <c r="AV4" s="551"/>
-      <c r="AW4" s="549" t="s">
+      <c r="AW4" s="550" t="s">
         <v>349</v>
       </c>
-      <c r="AX4" s="549"/>
-      <c r="AY4" s="549"/>
-      <c r="AZ4" s="549"/>
-      <c r="BA4" s="549"/>
-      <c r="BB4" s="550" t="s">
+      <c r="AX4" s="550"/>
+      <c r="AY4" s="550"/>
+      <c r="AZ4" s="550"/>
+      <c r="BA4" s="550"/>
+      <c r="BB4" s="549" t="s">
         <v>350</v>
       </c>
-      <c r="BC4" s="549"/>
-      <c r="BD4" s="549"/>
-      <c r="BE4" s="549"/>
+      <c r="BC4" s="550"/>
+      <c r="BD4" s="550"/>
+      <c r="BE4" s="550"/>
       <c r="BF4" s="551"/>
-      <c r="BG4" s="549" t="s">
+      <c r="BG4" s="550" t="s">
         <v>351</v>
       </c>
-      <c r="BH4" s="549"/>
-      <c r="BI4" s="549"/>
-      <c r="BJ4" s="549"/>
-      <c r="BK4" s="549"/>
-      <c r="BL4" s="550" t="s">
+      <c r="BH4" s="550"/>
+      <c r="BI4" s="550"/>
+      <c r="BJ4" s="550"/>
+      <c r="BK4" s="550"/>
+      <c r="BL4" s="549" t="s">
         <v>352</v>
       </c>
-      <c r="BM4" s="549"/>
-      <c r="BN4" s="549"/>
-      <c r="BO4" s="549"/>
-      <c r="BP4" s="549"/>
-      <c r="BQ4" s="550" t="s">
+      <c r="BM4" s="550"/>
+      <c r="BN4" s="550"/>
+      <c r="BO4" s="550"/>
+      <c r="BP4" s="550"/>
+      <c r="BQ4" s="549" t="s">
         <v>353</v>
       </c>
-      <c r="BR4" s="549"/>
-      <c r="BS4" s="549"/>
-      <c r="BT4" s="549"/>
+      <c r="BR4" s="550"/>
+      <c r="BS4" s="550"/>
+      <c r="BT4" s="550"/>
       <c r="BU4" s="551"/>
       <c r="BV4" s="284" t="s">
         <v>354</v>
@@ -50418,11 +50418,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -50435,6 +50430,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -50457,23 +50457,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="558" t="s">
+      <c r="A1" s="556" t="s">
         <v>627</v>
       </c>
-      <c r="B1" s="560" t="s">
+      <c r="B1" s="558" t="s">
         <v>628</v>
       </c>
-      <c r="C1" s="561"/>
-      <c r="D1" s="561"/>
-      <c r="E1" s="561"/>
-      <c r="F1" s="562"/>
-      <c r="G1" s="560" t="s">
+      <c r="C1" s="559"/>
+      <c r="D1" s="559"/>
+      <c r="E1" s="559"/>
+      <c r="F1" s="560"/>
+      <c r="G1" s="558" t="s">
         <v>629</v>
       </c>
-      <c r="H1" s="561"/>
-      <c r="I1" s="561"/>
-      <c r="J1" s="561"/>
-      <c r="K1" s="562"/>
+      <c r="H1" s="559"/>
+      <c r="I1" s="559"/>
+      <c r="J1" s="559"/>
+      <c r="K1" s="560"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -50483,7 +50483,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="559"/>
+      <c r="A2" s="557"/>
       <c r="B2" s="454" t="s">
         <v>276</v>
       </c>
@@ -51976,11 +51976,11 @@
       <c r="Y48" t="s">
         <v>678</v>
       </c>
-      <c r="Z48" s="556" t="s">
+      <c r="Z48" s="561" t="s">
         <v>616</v>
       </c>
-      <c r="AA48" s="557"/>
-      <c r="AB48" s="557"/>
+      <c r="AA48" s="562"/>
+      <c r="AB48" s="562"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -52197,11 +52197,11 @@
       <c r="Y53" t="s">
         <v>680</v>
       </c>
-      <c r="Z53" s="556" t="s">
+      <c r="Z53" s="561" t="s">
         <v>615</v>
       </c>
-      <c r="AA53" s="557"/>
-      <c r="AB53" s="557"/>
+      <c r="AA53" s="562"/>
+      <c r="AB53" s="562"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -52403,11 +52403,11 @@
       <c r="Y59" t="s">
         <v>681</v>
       </c>
-      <c r="Z59" s="556" t="s">
+      <c r="Z59" s="561" t="s">
         <v>682</v>
       </c>
-      <c r="AA59" s="557"/>
-      <c r="AB59" s="557"/>
+      <c r="AA59" s="562"/>
+      <c r="AB59" s="562"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="474" t="str">
@@ -53244,17 +53244,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BIOGAS Share in new technology
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF1B590-FBFB-47E1-9574-BC3A648E807A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD811A08-E54A-4C35-8A65-0CA638390DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -8612,7 +8612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="741">
   <si>
     <t>Document type:</t>
   </si>
@@ -13547,15 +13547,6 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13563,6 +13554,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13574,22 +13574,13 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13601,10 +13592,19 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13622,6 +13622,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13636,12 +13642,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -21173,8 +21173,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Y103" sqref="Y103"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21364,12 +21364,12 @@
         <v>85</v>
       </c>
       <c r="U4" s="539"/>
-      <c r="V4" s="531" t="s">
+      <c r="V4" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="532"/>
-      <c r="X4" s="532"/>
-      <c r="Y4" s="533"/>
+      <c r="W4" s="541"/>
+      <c r="X4" s="541"/>
+      <c r="Y4" s="542"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21472,34 +21472,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="534" t="s">
+      <c r="H6" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="535"/>
-      <c r="J6" s="535"/>
-      <c r="K6" s="536"/>
-      <c r="L6" s="535" t="s">
+      <c r="I6" s="532"/>
+      <c r="J6" s="532"/>
+      <c r="K6" s="533"/>
+      <c r="L6" s="532" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="535"/>
-      <c r="N6" s="535"/>
-      <c r="O6" s="536"/>
-      <c r="P6" s="534" t="s">
+      <c r="M6" s="532"/>
+      <c r="N6" s="532"/>
+      <c r="O6" s="533"/>
+      <c r="P6" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="535"/>
-      <c r="R6" s="535"/>
-      <c r="S6" s="536"/>
-      <c r="T6" s="534" t="s">
+      <c r="Q6" s="532"/>
+      <c r="R6" s="532"/>
+      <c r="S6" s="533"/>
+      <c r="T6" s="531" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="536"/>
-      <c r="V6" s="534" t="s">
+      <c r="U6" s="533"/>
+      <c r="V6" s="531" t="s">
         <v>541</v>
       </c>
-      <c r="W6" s="535"/>
-      <c r="X6" s="535"/>
-      <c r="Y6" s="536"/>
+      <c r="W6" s="532"/>
+      <c r="X6" s="532"/>
+      <c r="Y6" s="533"/>
       <c r="Z6" s="61" t="s">
         <v>553</v>
       </c>
@@ -23582,19 +23582,19 @@
       </c>
       <c r="H28" s="383">
         <f>1*$AD$28+JRC_Data!AD18*(1.2-$AD$28)</f>
-        <v>3.2699999999999996</v>
+        <v>3.1549999999999998</v>
       </c>
       <c r="I28" s="383">
         <f>1*$AD$28+JRC_Data!AE18*(1.2-$AD$28)</f>
-        <v>3.6299999999999994</v>
+        <v>3.4950000000000001</v>
       </c>
       <c r="J28" s="383">
         <f>1*$AD$28+JRC_Data!AF18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="K28" s="383">
         <f>1*$AD$28+JRC_Data!AG18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="L28" s="49"/>
       <c r="M28" s="50"/>
@@ -23602,19 +23602,19 @@
       <c r="O28" s="51"/>
       <c r="P28" s="256">
         <f>H28*0.7</f>
-        <v>2.2889999999999997</v>
+        <v>2.2084999999999999</v>
       </c>
       <c r="Q28" s="26">
         <f>I28*0.7</f>
-        <v>2.5409999999999995</v>
+        <v>2.4464999999999999</v>
       </c>
       <c r="R28" s="26">
         <f t="shared" ref="R28:S28" si="23">J28*0.7</f>
-        <v>2.7299999999999995</v>
+        <v>2.625</v>
       </c>
       <c r="S28" s="59">
         <f t="shared" si="23"/>
-        <v>2.7299999999999995</v>
+        <v>2.625</v>
       </c>
       <c r="T28" s="260">
         <v>20</v>
@@ -23644,18 +23644,18 @@
       <c r="AB28" s="84"/>
       <c r="AC28" s="84"/>
       <c r="AD28" s="84">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AE28" s="73">
         <f>AD28</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AF28" s="66">
         <v>5</v>
       </c>
       <c r="AG28" s="82">
         <f>31.536*(AJ28/1000)</f>
-        <v>0.30274559999999995</v>
+        <v>0.32166719999999999</v>
       </c>
       <c r="AH28" s="83"/>
       <c r="AI28" s="83">
@@ -23663,7 +23663,7 @@
       </c>
       <c r="AJ28" s="83">
         <f>AJ10*AD28+AJ21*(1-AD28)</f>
-        <v>9.5999999999999979</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AL28" s="2"/>
       <c r="AM28" s="105" t="str">
@@ -24499,7 +24499,9 @@
       <c r="AD41" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="AE41" s="17"/>
+      <c r="AE41" s="17" t="s">
+        <v>736</v>
+      </c>
       <c r="AF41" s="17" t="s">
         <v>254</v>
       </c>
@@ -24554,12 +24556,12 @@
         <v>85</v>
       </c>
       <c r="U42" s="539"/>
-      <c r="V42" s="531" t="s">
+      <c r="V42" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="W42" s="532"/>
-      <c r="X42" s="532"/>
-      <c r="Y42" s="533"/>
+      <c r="W42" s="541"/>
+      <c r="X42" s="541"/>
+      <c r="Y42" s="542"/>
       <c r="Z42" s="60"/>
       <c r="AA42" s="60"/>
       <c r="AB42" s="68" t="s">
@@ -24571,7 +24573,9 @@
       <c r="AD42" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="AE42" s="71"/>
+      <c r="AE42" s="71" t="s">
+        <v>215</v>
+      </c>
       <c r="AF42" s="71" t="s">
         <v>253</v>
       </c>
@@ -24660,34 +24664,34 @@
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
       <c r="G44" s="39"/>
-      <c r="H44" s="534" t="s">
+      <c r="H44" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="535"/>
-      <c r="J44" s="535"/>
-      <c r="K44" s="536"/>
-      <c r="L44" s="535" t="s">
+      <c r="I44" s="532"/>
+      <c r="J44" s="532"/>
+      <c r="K44" s="533"/>
+      <c r="L44" s="532" t="s">
         <v>34</v>
       </c>
-      <c r="M44" s="535"/>
-      <c r="N44" s="535"/>
-      <c r="O44" s="536"/>
-      <c r="P44" s="534" t="s">
+      <c r="M44" s="532"/>
+      <c r="N44" s="532"/>
+      <c r="O44" s="533"/>
+      <c r="P44" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="Q44" s="535"/>
-      <c r="R44" s="535"/>
-      <c r="S44" s="536"/>
-      <c r="T44" s="540" t="s">
+      <c r="Q44" s="532"/>
+      <c r="R44" s="532"/>
+      <c r="S44" s="533"/>
+      <c r="T44" s="534" t="s">
         <v>68</v>
       </c>
-      <c r="U44" s="541"/>
-      <c r="V44" s="540" t="s">
+      <c r="U44" s="535"/>
+      <c r="V44" s="534" t="s">
         <v>541</v>
       </c>
-      <c r="W44" s="542"/>
-      <c r="X44" s="542"/>
-      <c r="Y44" s="541"/>
+      <c r="W44" s="536"/>
+      <c r="X44" s="536"/>
+      <c r="Y44" s="535"/>
       <c r="Z44" s="377" t="s">
         <v>553</v>
       </c>
@@ -25016,7 +25020,7 @@
       </c>
       <c r="AA47" s="65"/>
       <c r="AB47" s="42">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="AC47" s="72"/>
       <c r="AD47" s="72"/>
@@ -25438,7 +25442,7 @@
       </c>
       <c r="AA51" s="65"/>
       <c r="AB51" s="42">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="AC51" s="72"/>
       <c r="AD51" s="72"/>
@@ -27101,7 +27105,7 @@
       </c>
       <c r="AA68" s="62"/>
       <c r="AB68" s="72">
-        <v>0.1</v>
+        <v>0.66</v>
       </c>
       <c r="AC68" s="62"/>
       <c r="AD68" s="62"/>
@@ -27717,19 +27721,19 @@
       </c>
       <c r="H75" s="383">
         <f>1*$AD$28+JRC_Data!AD18*(1.2-$AD$28)</f>
-        <v>3.2699999999999996</v>
+        <v>3.1549999999999998</v>
       </c>
       <c r="I75" s="383">
         <f>1*$AD$28+JRC_Data!AE18*(1.2-$AD$28)</f>
-        <v>3.6299999999999994</v>
+        <v>3.4950000000000001</v>
       </c>
       <c r="J75" s="383">
         <f>1*$AD$28+JRC_Data!AF18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="K75" s="383">
         <f>1*$AD$28+JRC_Data!AG18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="L75" s="49"/>
       <c r="M75" s="50"/>
@@ -27737,19 +27741,19 @@
       <c r="O75" s="51"/>
       <c r="P75" s="256">
         <f>H75*0.7</f>
-        <v>2.2889999999999997</v>
+        <v>2.2084999999999999</v>
       </c>
       <c r="Q75" s="26">
         <f t="shared" ref="Q75" si="57">I75*0.7</f>
-        <v>2.5409999999999995</v>
+        <v>2.4464999999999999</v>
       </c>
       <c r="R75" s="26">
         <f t="shared" ref="R75" si="58">J75*0.7</f>
-        <v>2.7299999999999995</v>
+        <v>2.625</v>
       </c>
       <c r="S75" s="59">
         <f t="shared" ref="S75" si="59">K75*0.7</f>
-        <v>2.7299999999999995</v>
+        <v>2.625</v>
       </c>
       <c r="T75" s="3">
         <v>20</v>
@@ -27778,18 +27782,18 @@
       <c r="AB75" s="84"/>
       <c r="AC75" s="84"/>
       <c r="AD75" s="84">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AE75" s="73">
         <f>AD75</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AF75" s="83">
         <v>5</v>
       </c>
       <c r="AG75" s="82">
         <f t="shared" si="29"/>
-        <v>0.42415920000000001</v>
+        <v>0.45017639999999998</v>
       </c>
       <c r="AH75" s="83"/>
       <c r="AI75" s="83">
@@ -27797,7 +27801,7 @@
       </c>
       <c r="AJ75" s="83">
         <f>AJ50*AD75+AJ68*(1-AD75)</f>
-        <v>13.45</v>
+        <v>14.275</v>
       </c>
       <c r="AL75" s="2"/>
       <c r="AM75" s="105" t="str">
@@ -28455,7 +28459,9 @@
       <c r="AD89" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="AE89" s="17"/>
+      <c r="AE89" s="17" t="s">
+        <v>736</v>
+      </c>
       <c r="AF89" s="17" t="s">
         <v>254</v>
       </c>
@@ -28510,12 +28516,12 @@
         <v>85</v>
       </c>
       <c r="U90" s="539"/>
-      <c r="V90" s="531" t="s">
+      <c r="V90" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="W90" s="532"/>
-      <c r="X90" s="532"/>
-      <c r="Y90" s="533"/>
+      <c r="W90" s="541"/>
+      <c r="X90" s="541"/>
+      <c r="Y90" s="542"/>
       <c r="Z90" s="60"/>
       <c r="AA90" s="60"/>
       <c r="AB90" s="68" t="s">
@@ -28527,7 +28533,9 @@
       <c r="AD90" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="AE90" s="71"/>
+      <c r="AE90" s="71" t="s">
+        <v>215</v>
+      </c>
       <c r="AF90" s="71" t="s">
         <v>253</v>
       </c>
@@ -28616,34 +28624,34 @@
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="39"/>
-      <c r="H92" s="534" t="s">
+      <c r="H92" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="I92" s="535"/>
-      <c r="J92" s="535"/>
-      <c r="K92" s="536"/>
-      <c r="L92" s="535" t="s">
+      <c r="I92" s="532"/>
+      <c r="J92" s="532"/>
+      <c r="K92" s="533"/>
+      <c r="L92" s="532" t="s">
         <v>34</v>
       </c>
-      <c r="M92" s="535"/>
-      <c r="N92" s="535"/>
-      <c r="O92" s="536"/>
-      <c r="P92" s="534" t="s">
+      <c r="M92" s="532"/>
+      <c r="N92" s="532"/>
+      <c r="O92" s="533"/>
+      <c r="P92" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="Q92" s="535"/>
-      <c r="R92" s="535"/>
-      <c r="S92" s="536"/>
-      <c r="T92" s="540" t="s">
+      <c r="Q92" s="532"/>
+      <c r="R92" s="532"/>
+      <c r="S92" s="533"/>
+      <c r="T92" s="534" t="s">
         <v>68</v>
       </c>
-      <c r="U92" s="541"/>
-      <c r="V92" s="540" t="s">
+      <c r="U92" s="535"/>
+      <c r="V92" s="534" t="s">
         <v>541</v>
       </c>
-      <c r="W92" s="542"/>
-      <c r="X92" s="542"/>
-      <c r="Y92" s="541"/>
+      <c r="W92" s="536"/>
+      <c r="X92" s="536"/>
+      <c r="Y92" s="535"/>
       <c r="Z92" s="377" t="s">
         <v>553</v>
       </c>
@@ -28972,7 +28980,7 @@
       </c>
       <c r="AA95" s="65"/>
       <c r="AB95" s="42">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="AC95" s="72"/>
       <c r="AD95" s="72"/>
@@ -29394,7 +29402,7 @@
       </c>
       <c r="AA99" s="65"/>
       <c r="AB99" s="42">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="AC99" s="72"/>
       <c r="AD99" s="72"/>
@@ -29585,19 +29593,19 @@
       </c>
       <c r="U101" s="41"/>
       <c r="V101" s="383">
-        <f>V97+0.3</f>
+        <f t="shared" ref="V101:Y102" si="73">V97+0.3</f>
         <v>3.8249999999999997</v>
       </c>
       <c r="W101" s="383">
-        <f>W97+0.3</f>
+        <f t="shared" si="73"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="X101" s="383">
-        <f>X97+0.3</f>
+        <f t="shared" si="73"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="Y101" s="383">
-        <f>Y97+0.3</f>
+        <f t="shared" si="73"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="Z101" s="383">
@@ -29677,15 +29685,15 @@
         <v>0.7</v>
       </c>
       <c r="Q102" s="23">
-        <f t="shared" ref="Q102" si="73">I102*0.7</f>
+        <f t="shared" ref="Q102" si="74">I102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R102" s="23">
-        <f t="shared" ref="R102" si="74">J102*0.7</f>
+        <f t="shared" ref="R102" si="75">J102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S102" s="57">
-        <f t="shared" ref="S102" si="75">K102*0.7</f>
+        <f t="shared" ref="S102" si="76">K102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T102" s="53">
@@ -29693,19 +29701,19 @@
       </c>
       <c r="U102" s="25"/>
       <c r="V102" s="384">
-        <f>V98+0.3</f>
+        <f t="shared" si="73"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="W102" s="384">
-        <f>W98+0.3</f>
+        <f t="shared" si="73"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="X102" s="384">
-        <f>X98+0.3</f>
+        <f t="shared" si="73"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="Y102" s="384">
-        <f>Y98+0.3</f>
+        <f t="shared" si="73"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="Z102" s="383">
@@ -29875,19 +29883,19 @@
       <c r="N104" s="32"/>
       <c r="O104" s="45"/>
       <c r="P104" s="22">
-        <f t="shared" ref="P104:S104" si="76">H104*0.7</f>
+        <f t="shared" ref="P104:S104" si="77">H104*0.7</f>
         <v>0.7</v>
       </c>
       <c r="Q104" s="23">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.7</v>
       </c>
       <c r="R104" s="23">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.7</v>
       </c>
       <c r="S104" s="57">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.7</v>
       </c>
       <c r="T104" s="53">
@@ -29899,15 +29907,15 @@
         <v>22.778925619834713</v>
       </c>
       <c r="W104" s="384">
-        <f t="shared" ref="W104" si="77">W103*($U$152/$U$151)</f>
+        <f t="shared" ref="W104" si="78">W103*($U$152/$U$151)</f>
         <v>22.04476084710744</v>
       </c>
       <c r="X104" s="384">
-        <f t="shared" ref="X104" si="78">X103*($U$152/$U$151)</f>
+        <f t="shared" ref="X104" si="79">X103*($U$152/$U$151)</f>
         <v>20.839163429752066</v>
       </c>
       <c r="Y104" s="384">
-        <f t="shared" ref="Y104" si="79">Y103*($U$152/$U$151)</f>
+        <f t="shared" ref="Y104" si="80">Y103*($U$152/$U$151)</f>
         <v>18.635439049586779</v>
       </c>
       <c r="Z104" s="384">
@@ -30074,19 +30082,19 @@
       <c r="N106" s="32"/>
       <c r="O106" s="45"/>
       <c r="P106" s="22">
-        <f t="shared" ref="P106:P108" si="80">H106*0.7</f>
+        <f t="shared" ref="P106:P108" si="81">H106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="Q106" s="23">
-        <f t="shared" ref="Q106:Q108" si="81">I106*0.7</f>
+        <f t="shared" ref="Q106:Q108" si="82">I106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="R106" s="23">
-        <f t="shared" ref="R106:R108" si="82">J106*0.7</f>
+        <f t="shared" ref="R106:R108" si="83">J106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="S106" s="57">
-        <f t="shared" ref="S106:S108" si="83">K106*0.7</f>
+        <f t="shared" ref="S106:S108" si="84">K106*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="T106" s="53">
@@ -30189,19 +30197,19 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="W107" s="62">
-        <f t="shared" ref="W107:Z107" si="84">W93</f>
+        <f t="shared" ref="W107:Z107" si="85">W93</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="X107" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y107" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z107" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>0.12</v>
       </c>
       <c r="AA107" s="65"/>
@@ -30272,19 +30280,19 @@
       <c r="N108" s="50"/>
       <c r="O108" s="51"/>
       <c r="P108" s="256">
-        <f t="shared" si="80"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="Q108" s="26">
         <f t="shared" si="81"/>
         <v>0.57399999999999995</v>
       </c>
-      <c r="R108" s="26">
+      <c r="Q108" s="26">
         <f t="shared" si="82"/>
         <v>0.57399999999999995</v>
       </c>
+      <c r="R108" s="26">
+        <f t="shared" si="83"/>
+        <v>0.57399999999999995</v>
+      </c>
       <c r="S108" s="59">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="T108" s="55">
@@ -30296,19 +30304,19 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="W108" s="62">
-        <f t="shared" ref="W108:Z108" si="85">W94</f>
+        <f t="shared" ref="W108:Z108" si="86">W94</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="X108" s="62">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y108" s="62">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z108" s="62">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>0.12</v>
       </c>
       <c r="AA108" s="66"/>
@@ -30483,11 +30491,11 @@
       </c>
       <c r="AL110" s="104"/>
       <c r="AM110" s="103" t="str">
-        <f t="shared" ref="AM110:AM116" si="86">C112</f>
+        <f t="shared" ref="AM110:AM116" si="87">C112</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AN110" s="103" t="str">
-        <f t="shared" ref="AN110:AN116" si="87">D112</f>
+        <f t="shared" ref="AN110:AN116" si="88">D112</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AO110" s="104" t="s">
@@ -30540,11 +30548,11 @@
       <c r="AJ111" s="34"/>
       <c r="AL111" s="106"/>
       <c r="AM111" s="105" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AN111" s="105" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AO111" s="106" t="s">
@@ -30638,11 +30646,11 @@
       </c>
       <c r="AL112" s="106"/>
       <c r="AM112" s="105" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AN112" s="105" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AO112" s="106" t="s">
@@ -30744,11 +30752,11 @@
       </c>
       <c r="AL113" s="106"/>
       <c r="AM113" s="105" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AN113" s="105" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AO113" s="106" t="s">
@@ -30840,11 +30848,11 @@
       </c>
       <c r="AL114" s="213"/>
       <c r="AM114" s="105" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AN114" s="105" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AO114" s="106" t="s">
@@ -30896,15 +30904,15 @@
         <v>0.7</v>
       </c>
       <c r="Q115" s="23">
-        <f t="shared" ref="Q115:Q116" si="88">I115*0.7</f>
+        <f t="shared" ref="Q115:Q116" si="89">I115*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="R115" s="23">
-        <f t="shared" ref="R115:R116" si="89">J115*0.7</f>
+        <f t="shared" ref="R115:R116" si="90">J115*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="S115" s="57">
-        <f t="shared" ref="S115:S116" si="90">K115*0.7</f>
+        <f t="shared" ref="S115:S116" si="91">K115*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="T115" s="53">
@@ -30916,15 +30924,15 @@
         <v>9.9300970464135023</v>
       </c>
       <c r="W115" s="384">
-        <f t="shared" ref="W115" si="91">W114*($U$150/$U$149)</f>
+        <f t="shared" ref="W115" si="92">W114*($U$150/$U$149)</f>
         <v>9.0363883122362889</v>
       </c>
       <c r="X115" s="384">
-        <f t="shared" ref="X115" si="92">X114*($U$150/$U$149)</f>
+        <f t="shared" ref="X115" si="93">X114*($U$150/$U$149)</f>
         <v>8.2231133641350223</v>
       </c>
       <c r="Y115" s="384">
-        <f t="shared" ref="Y115" si="93">Y114*($U$150/$U$149)</f>
+        <f t="shared" ref="Y115" si="94">Y114*($U$150/$U$149)</f>
         <v>8.1426795780590719</v>
       </c>
       <c r="Z115" s="384">
@@ -30949,11 +30957,11 @@
       </c>
       <c r="AL115" s="213"/>
       <c r="AM115" s="105" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AN115" s="105" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AO115" s="106" t="s">
@@ -31005,15 +31013,15 @@
         <v>0.7</v>
       </c>
       <c r="Q116" s="29">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="R116" s="29">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="S116" s="58">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T116" s="54">
@@ -31042,7 +31050,7 @@
       </c>
       <c r="AA116" s="62"/>
       <c r="AB116" s="72">
-        <v>0.1</v>
+        <v>0.66</v>
       </c>
       <c r="AC116" s="62"/>
       <c r="AD116" s="62"/>
@@ -31063,11 +31071,11 @@
       </c>
       <c r="AL116" s="112"/>
       <c r="AM116" s="108" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AN116" s="108" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AO116" s="109" t="s">
@@ -31384,15 +31392,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="Q120" s="20">
-        <f t="shared" ref="Q120:Q121" si="94">I120*0.7</f>
+        <f t="shared" ref="Q120:Q121" si="95">I120*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="R120" s="20">
-        <f t="shared" ref="R120:R121" si="95">J120*0.7</f>
+        <f t="shared" ref="R120:R121" si="96">J120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="S120" s="56">
-        <f t="shared" ref="S120:S121" si="96">K120*0.7</f>
+        <f t="shared" ref="S120:S121" si="97">K120*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T120" s="89">
@@ -31498,15 +31506,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="Q121" s="26">
-        <f t="shared" si="94"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="R121" s="26">
         <f t="shared" si="95"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="R121" s="26">
+        <f t="shared" si="96"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="S121" s="59">
-        <f t="shared" si="96"/>
+        <f t="shared" si="97"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="T121" s="27">
@@ -31609,11 +31617,11 @@
       <c r="AJ122" s="34"/>
       <c r="AL122" s="216"/>
       <c r="AM122" s="103" t="str">
-        <f t="shared" ref="AM122:AM123" si="97">C128</f>
+        <f t="shared" ref="AM122:AM123" si="98">C128</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AN122" s="103" t="str">
-        <f t="shared" ref="AN122:AN123" si="98">D128</f>
+        <f t="shared" ref="AN122:AN123" si="99">D128</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AO122" s="104" t="s">
@@ -31646,19 +31654,19 @@
       </c>
       <c r="H123" s="383">
         <f>1*$AD$28+JRC_Data!AD18*(1.2-$AD$28)</f>
-        <v>3.2699999999999996</v>
+        <v>3.1549999999999998</v>
       </c>
       <c r="I123" s="383">
         <f>1*$AD$28+JRC_Data!AE18*(1.2-$AD$28)</f>
-        <v>3.6299999999999994</v>
+        <v>3.4950000000000001</v>
       </c>
       <c r="J123" s="383">
         <f>1*$AD$28+JRC_Data!AF18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="K123" s="383">
         <f>1*$AD$28+JRC_Data!AG18*(1.2-$AD$28)</f>
-        <v>3.8999999999999995</v>
+        <v>3.75</v>
       </c>
       <c r="L123" s="49"/>
       <c r="M123" s="50"/>
@@ -31666,19 +31674,19 @@
       <c r="O123" s="51"/>
       <c r="P123" s="256">
         <f>H123*0.7</f>
-        <v>2.2889999999999997</v>
+        <v>2.2084999999999999</v>
       </c>
       <c r="Q123" s="26">
-        <f t="shared" ref="Q123" si="99">I123*0.7</f>
-        <v>2.5409999999999995</v>
+        <f t="shared" ref="Q123" si="100">I123*0.7</f>
+        <v>2.4464999999999999</v>
       </c>
       <c r="R123" s="26">
-        <f t="shared" ref="R123" si="100">J123*0.7</f>
-        <v>2.7299999999999995</v>
+        <f t="shared" ref="R123" si="101">J123*0.7</f>
+        <v>2.625</v>
       </c>
       <c r="S123" s="59">
-        <f t="shared" ref="S123" si="101">K123*0.7</f>
-        <v>2.7299999999999995</v>
+        <f t="shared" ref="S123" si="102">K123*0.7</f>
+        <v>2.625</v>
       </c>
       <c r="T123" s="3">
         <v>20</v>
@@ -31688,15 +31696,15 @@
         <v>10.987282270335434</v>
       </c>
       <c r="W123" s="79">
-        <f t="shared" ref="W123:Y123" si="102">(W115+W98)*0.8</f>
+        <f t="shared" ref="W123:Y123" si="103">(W115+W98)*0.8</f>
         <v>10.272315282993665</v>
       </c>
       <c r="X123" s="79">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>9.6216953245126504</v>
       </c>
       <c r="Y123" s="79">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>9.5573482956518898</v>
       </c>
       <c r="Z123" s="375">
@@ -31707,18 +31715,18 @@
       <c r="AB123" s="84"/>
       <c r="AC123" s="84"/>
       <c r="AD123" s="84">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AE123" s="73">
         <f>AD123</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="AF123" s="83">
         <v>5</v>
       </c>
       <c r="AG123" s="82">
         <f t="shared" si="62"/>
-        <v>0.62441279999999999</v>
+        <v>0.66540960000000005</v>
       </c>
       <c r="AH123" s="83"/>
       <c r="AI123" s="83">
@@ -31726,15 +31734,15 @@
       </c>
       <c r="AJ123" s="83">
         <f>AJ98*AD123+AJ116*(1-AD123)</f>
-        <v>19.799999999999997</v>
+        <v>21.1</v>
       </c>
       <c r="AL123" s="2"/>
       <c r="AM123" s="105" t="str">
-        <f t="shared" si="97"/>
+        <f t="shared" si="98"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AN123" s="105" t="str">
-        <f t="shared" si="98"/>
+        <f t="shared" si="99"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AO123" s="106" t="s">
@@ -32354,7 +32362,7 @@
         <v>3</v>
       </c>
       <c r="U145" s="381">
-        <f t="shared" ref="U145:U154" si="103">V145/$V$153</f>
+        <f t="shared" ref="U145:U154" si="104">V145/$V$153</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="V145" s="382">
@@ -32368,7 +32376,7 @@
         <v>5</v>
       </c>
       <c r="U146" s="381">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="V146" s="382">
@@ -32381,7 +32389,7 @@
         <v>8</v>
       </c>
       <c r="U147" s="381">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="V147" s="382">
@@ -32395,7 +32403,7 @@
         <v>10</v>
       </c>
       <c r="U148" s="381">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="V148" s="380">
@@ -32416,7 +32424,7 @@
         <v>15</v>
       </c>
       <c r="U149" s="371">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="V149" s="3">
@@ -32443,7 +32451,7 @@
         <v>18</v>
       </c>
       <c r="U150" s="371">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="V150" s="3">
@@ -32472,7 +32480,7 @@
         <v>20</v>
       </c>
       <c r="U151" s="381">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="V151" s="380">
@@ -32502,7 +32510,7 @@
         <v>24</v>
       </c>
       <c r="U152" s="371">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="V152" s="3">
@@ -32531,7 +32539,7 @@
         <v>30</v>
       </c>
       <c r="U153" s="371">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>1</v>
       </c>
       <c r="V153" s="3">
@@ -32560,7 +32568,7 @@
         <v>35</v>
       </c>
       <c r="U154" s="371">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="V154" s="3">
@@ -32605,26 +32613,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -32635,6 +32623,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -32780,12 +32788,12 @@
       <c r="I5" s="127"/>
       <c r="J5" s="127"/>
       <c r="K5" s="127"/>
-      <c r="L5" s="531" t="s">
+      <c r="L5" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="532"/>
-      <c r="N5" s="532"/>
-      <c r="O5" s="533"/>
+      <c r="M5" s="541"/>
+      <c r="N5" s="541"/>
+      <c r="O5" s="542"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -32816,12 +32824,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="540" t="s">
+      <c r="L6" s="534" t="s">
         <v>541</v>
       </c>
-      <c r="M6" s="542"/>
-      <c r="N6" s="542"/>
-      <c r="O6" s="541"/>
+      <c r="M6" s="536"/>
+      <c r="N6" s="536"/>
+      <c r="O6" s="535"/>
       <c r="P6" s="377" t="s">
         <v>553</v>
       </c>
@@ -33707,23 +33715,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="531" t="s">
+      <c r="L33" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="532"/>
-      <c r="N33" s="532"/>
-      <c r="O33" s="533"/>
+      <c r="M33" s="541"/>
+      <c r="N33" s="541"/>
+      <c r="O33" s="542"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L34" s="540" t="s">
+      <c r="L34" s="534" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="542"/>
-      <c r="N34" s="542"/>
-      <c r="O34" s="541"/>
+      <c r="M34" s="536"/>
+      <c r="N34" s="536"/>
+      <c r="O34" s="535"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -34070,11 +34078,11 @@
       </c>
       <c r="I4" s="538"/>
       <c r="J4" s="539"/>
-      <c r="K4" s="531" t="s">
+      <c r="K4" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="532"/>
-      <c r="M4" s="533"/>
+      <c r="L4" s="541"/>
+      <c r="M4" s="542"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -34100,16 +34108,16 @@
       <c r="G5" s="385" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="543" t="s">
+      <c r="H5" s="546" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="544"/>
-      <c r="J5" s="545"/>
-      <c r="K5" s="543" t="s">
+      <c r="I5" s="547"/>
+      <c r="J5" s="548"/>
+      <c r="K5" s="546" t="s">
         <v>330</v>
       </c>
-      <c r="L5" s="544"/>
-      <c r="M5" s="545"/>
+      <c r="L5" s="547"/>
+      <c r="M5" s="548"/>
       <c r="N5" s="386" t="s">
         <v>92</v>
       </c>
@@ -34126,23 +34134,23 @@
         <v>218</v>
       </c>
       <c r="AA5" s="208"/>
-      <c r="AB5" s="546" t="s">
+      <c r="AB5" s="543" t="s">
         <v>583</v>
       </c>
-      <c r="AC5" s="546"/>
+      <c r="AC5" s="543"/>
       <c r="AD5" s="388"/>
-      <c r="AE5" s="547" t="s">
+      <c r="AE5" s="544" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="547"/>
-      <c r="AG5" s="547" t="s">
+      <c r="AF5" s="544"/>
+      <c r="AG5" s="544" t="s">
         <v>584</v>
       </c>
-      <c r="AH5" s="547"/>
-      <c r="AI5" s="548" t="s">
+      <c r="AH5" s="544"/>
+      <c r="AI5" s="545" t="s">
         <v>585</v>
       </c>
-      <c r="AJ5" s="548"/>
+      <c r="AJ5" s="545"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="432" t="str">
@@ -34880,12 +34888,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="531" t="s">
+      <c r="L27" s="540" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="532"/>
-      <c r="N27" s="532"/>
-      <c r="O27" s="533"/>
+      <c r="M27" s="541"/>
+      <c r="N27" s="541"/>
+      <c r="O27" s="542"/>
       <c r="T27" s="210"/>
       <c r="U27" s="210"/>
     </row>
@@ -34893,12 +34901,12 @@
       <c r="J28" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L28" s="534" t="s">
+      <c r="L28" s="531" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="535"/>
-      <c r="N28" s="535"/>
-      <c r="O28" s="536"/>
+      <c r="M28" s="532"/>
+      <c r="N28" s="532"/>
+      <c r="O28" s="533"/>
       <c r="T28" s="210"/>
       <c r="U28" s="210"/>
     </row>
@@ -36288,16 +36296,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -36728,103 +36736,103 @@
       <c r="C4" s="283" t="s">
         <v>339</v>
       </c>
-      <c r="D4" s="549" t="s">
+      <c r="D4" s="550" t="s">
         <v>340</v>
       </c>
-      <c r="E4" s="550"/>
-      <c r="F4" s="550"/>
-      <c r="G4" s="550"/>
+      <c r="E4" s="549"/>
+      <c r="F4" s="549"/>
+      <c r="G4" s="549"/>
       <c r="H4" s="551"/>
-      <c r="I4" s="550" t="s">
+      <c r="I4" s="549" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="550"/>
-      <c r="K4" s="550"/>
-      <c r="L4" s="550"/>
+      <c r="J4" s="549"/>
+      <c r="K4" s="549"/>
+      <c r="L4" s="549"/>
       <c r="M4" s="551"/>
-      <c r="N4" s="550" t="s">
+      <c r="N4" s="549" t="s">
         <v>342</v>
       </c>
-      <c r="O4" s="550"/>
-      <c r="P4" s="550"/>
-      <c r="Q4" s="550"/>
+      <c r="O4" s="549"/>
+      <c r="P4" s="549"/>
+      <c r="Q4" s="549"/>
       <c r="R4" s="551"/>
-      <c r="S4" s="550" t="s">
+      <c r="S4" s="549" t="s">
         <v>343</v>
       </c>
-      <c r="T4" s="550"/>
-      <c r="U4" s="550"/>
-      <c r="V4" s="550"/>
+      <c r="T4" s="549"/>
+      <c r="U4" s="549"/>
+      <c r="V4" s="549"/>
       <c r="W4" s="551"/>
-      <c r="X4" s="550" t="s">
+      <c r="X4" s="549" t="s">
         <v>344</v>
       </c>
-      <c r="Y4" s="550"/>
-      <c r="Z4" s="550"/>
-      <c r="AA4" s="550"/>
+      <c r="Y4" s="549"/>
+      <c r="Z4" s="549"/>
+      <c r="AA4" s="549"/>
       <c r="AB4" s="551"/>
-      <c r="AC4" s="550" t="s">
+      <c r="AC4" s="549" t="s">
         <v>345</v>
       </c>
-      <c r="AD4" s="550"/>
-      <c r="AE4" s="550"/>
-      <c r="AF4" s="550"/>
+      <c r="AD4" s="549"/>
+      <c r="AE4" s="549"/>
+      <c r="AF4" s="549"/>
       <c r="AG4" s="551"/>
-      <c r="AH4" s="550" t="s">
+      <c r="AH4" s="549" t="s">
         <v>346</v>
       </c>
-      <c r="AI4" s="550"/>
-      <c r="AJ4" s="550"/>
-      <c r="AK4" s="550"/>
+      <c r="AI4" s="549"/>
+      <c r="AJ4" s="549"/>
+      <c r="AK4" s="549"/>
       <c r="AL4" s="551"/>
-      <c r="AM4" s="550" t="s">
+      <c r="AM4" s="549" t="s">
         <v>347</v>
       </c>
-      <c r="AN4" s="550"/>
-      <c r="AO4" s="550"/>
-      <c r="AP4" s="550"/>
+      <c r="AN4" s="549"/>
+      <c r="AO4" s="549"/>
+      <c r="AP4" s="549"/>
       <c r="AQ4" s="551"/>
-      <c r="AR4" s="550" t="s">
+      <c r="AR4" s="549" t="s">
         <v>348</v>
       </c>
-      <c r="AS4" s="550"/>
-      <c r="AT4" s="550"/>
-      <c r="AU4" s="550"/>
+      <c r="AS4" s="549"/>
+      <c r="AT4" s="549"/>
+      <c r="AU4" s="549"/>
       <c r="AV4" s="551"/>
-      <c r="AW4" s="550" t="s">
+      <c r="AW4" s="549" t="s">
         <v>349</v>
       </c>
-      <c r="AX4" s="550"/>
-      <c r="AY4" s="550"/>
-      <c r="AZ4" s="550"/>
-      <c r="BA4" s="550"/>
-      <c r="BB4" s="549" t="s">
+      <c r="AX4" s="549"/>
+      <c r="AY4" s="549"/>
+      <c r="AZ4" s="549"/>
+      <c r="BA4" s="549"/>
+      <c r="BB4" s="550" t="s">
         <v>350</v>
       </c>
-      <c r="BC4" s="550"/>
-      <c r="BD4" s="550"/>
-      <c r="BE4" s="550"/>
+      <c r="BC4" s="549"/>
+      <c r="BD4" s="549"/>
+      <c r="BE4" s="549"/>
       <c r="BF4" s="551"/>
-      <c r="BG4" s="550" t="s">
+      <c r="BG4" s="549" t="s">
         <v>351</v>
       </c>
-      <c r="BH4" s="550"/>
-      <c r="BI4" s="550"/>
-      <c r="BJ4" s="550"/>
-      <c r="BK4" s="550"/>
-      <c r="BL4" s="549" t="s">
+      <c r="BH4" s="549"/>
+      <c r="BI4" s="549"/>
+      <c r="BJ4" s="549"/>
+      <c r="BK4" s="549"/>
+      <c r="BL4" s="550" t="s">
         <v>352</v>
       </c>
-      <c r="BM4" s="550"/>
-      <c r="BN4" s="550"/>
-      <c r="BO4" s="550"/>
-      <c r="BP4" s="550"/>
-      <c r="BQ4" s="549" t="s">
+      <c r="BM4" s="549"/>
+      <c r="BN4" s="549"/>
+      <c r="BO4" s="549"/>
+      <c r="BP4" s="549"/>
+      <c r="BQ4" s="550" t="s">
         <v>353</v>
       </c>
-      <c r="BR4" s="550"/>
-      <c r="BS4" s="550"/>
-      <c r="BT4" s="550"/>
+      <c r="BR4" s="549"/>
+      <c r="BS4" s="549"/>
+      <c r="BT4" s="549"/>
       <c r="BU4" s="551"/>
       <c r="BV4" s="284" t="s">
         <v>354</v>
@@ -50418,6 +50426,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -50430,11 +50443,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -50457,23 +50465,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="556" t="s">
+      <c r="A1" s="558" t="s">
         <v>627</v>
       </c>
-      <c r="B1" s="558" t="s">
+      <c r="B1" s="560" t="s">
         <v>628</v>
       </c>
-      <c r="C1" s="559"/>
-      <c r="D1" s="559"/>
-      <c r="E1" s="559"/>
-      <c r="F1" s="560"/>
-      <c r="G1" s="558" t="s">
+      <c r="C1" s="561"/>
+      <c r="D1" s="561"/>
+      <c r="E1" s="561"/>
+      <c r="F1" s="562"/>
+      <c r="G1" s="560" t="s">
         <v>629</v>
       </c>
-      <c r="H1" s="559"/>
-      <c r="I1" s="559"/>
-      <c r="J1" s="559"/>
-      <c r="K1" s="560"/>
+      <c r="H1" s="561"/>
+      <c r="I1" s="561"/>
+      <c r="J1" s="561"/>
+      <c r="K1" s="562"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -50483,7 +50491,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="557"/>
+      <c r="A2" s="559"/>
       <c r="B2" s="454" t="s">
         <v>276</v>
       </c>
@@ -51976,11 +51984,11 @@
       <c r="Y48" t="s">
         <v>678</v>
       </c>
-      <c r="Z48" s="561" t="s">
+      <c r="Z48" s="556" t="s">
         <v>616</v>
       </c>
-      <c r="AA48" s="562"/>
-      <c r="AB48" s="562"/>
+      <c r="AA48" s="557"/>
+      <c r="AB48" s="557"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -52197,11 +52205,11 @@
       <c r="Y53" t="s">
         <v>680</v>
       </c>
-      <c r="Z53" s="561" t="s">
+      <c r="Z53" s="556" t="s">
         <v>615</v>
       </c>
-      <c r="AA53" s="562"/>
-      <c r="AB53" s="562"/>
+      <c r="AA53" s="557"/>
+      <c r="AB53" s="557"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -52403,11 +52411,11 @@
       <c r="Y59" t="s">
         <v>681</v>
       </c>
-      <c r="Z59" s="561" t="s">
+      <c r="Z59" s="556" t="s">
         <v>682</v>
       </c>
-      <c r="AA59" s="562"/>
-      <c r="AB59" s="562"/>
+      <c r="AA59" s="557"/>
+      <c r="AB59" s="557"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="474" t="str">
@@ -53244,17 +53252,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Buildings come in 2019, not 2020 check small dummies
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78188AD5-97EC-42C9-9D9B-814EB055DB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BA5A0E-737C-4DEE-8191-9395728C5A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -13498,15 +13498,6 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13514,6 +13505,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13525,22 +13525,13 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13552,10 +13543,19 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13573,6 +13573,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13587,12 +13593,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -18349,7 +18349,7 @@
   <dimension ref="A2:AM103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18511,7 +18511,7 @@
         <v>2.045375452121146E-4</v>
       </c>
       <c r="J6" s="129">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L6" s="3">
         <f>I6/0.0000036</f>
@@ -18726,7 +18726,7 @@
         <v>7.5784815901851145E-4</v>
       </c>
       <c r="J12" s="129">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L12" s="4">
         <f>I12/0.0000036</f>
@@ -18926,7 +18926,7 @@
         <v>3.7645780249386E-3</v>
       </c>
       <c r="J18" s="129">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L18" s="4">
         <f>I18/0.0000036</f>
@@ -19219,7 +19219,7 @@
       <c r="AL26" s="4"/>
       <c r="AM26" s="4"/>
     </row>
-    <row r="27" spans="2:39" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:39" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
         <v>211</v>
       </c>
@@ -20707,12 +20707,12 @@
         <v>85</v>
       </c>
       <c r="U4" s="535"/>
-      <c r="V4" s="527" t="s">
+      <c r="V4" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="528"/>
-      <c r="X4" s="528"/>
-      <c r="Y4" s="529"/>
+      <c r="W4" s="537"/>
+      <c r="X4" s="537"/>
+      <c r="Y4" s="538"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -20815,34 +20815,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="530" t="s">
+      <c r="H6" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="531"/>
-      <c r="J6" s="531"/>
-      <c r="K6" s="532"/>
-      <c r="L6" s="531" t="s">
+      <c r="I6" s="528"/>
+      <c r="J6" s="528"/>
+      <c r="K6" s="529"/>
+      <c r="L6" s="528" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="531"/>
-      <c r="N6" s="531"/>
-      <c r="O6" s="532"/>
-      <c r="P6" s="530" t="s">
+      <c r="M6" s="528"/>
+      <c r="N6" s="528"/>
+      <c r="O6" s="529"/>
+      <c r="P6" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="531"/>
-      <c r="R6" s="531"/>
-      <c r="S6" s="532"/>
-      <c r="T6" s="530" t="s">
+      <c r="Q6" s="528"/>
+      <c r="R6" s="528"/>
+      <c r="S6" s="529"/>
+      <c r="T6" s="527" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="532"/>
-      <c r="V6" s="530" t="s">
+      <c r="U6" s="529"/>
+      <c r="V6" s="527" t="s">
         <v>525</v>
       </c>
-      <c r="W6" s="531"/>
-      <c r="X6" s="531"/>
-      <c r="Y6" s="532"/>
+      <c r="W6" s="528"/>
+      <c r="X6" s="528"/>
+      <c r="Y6" s="529"/>
       <c r="Z6" s="61" t="s">
         <v>537</v>
       </c>
@@ -23899,12 +23899,12 @@
         <v>85</v>
       </c>
       <c r="U42" s="535"/>
-      <c r="V42" s="527" t="s">
+      <c r="V42" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="W42" s="528"/>
-      <c r="X42" s="528"/>
-      <c r="Y42" s="529"/>
+      <c r="W42" s="537"/>
+      <c r="X42" s="537"/>
+      <c r="Y42" s="538"/>
       <c r="Z42" s="60"/>
       <c r="AA42" s="60"/>
       <c r="AB42" s="68" t="s">
@@ -24007,34 +24007,34 @@
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
       <c r="G44" s="39"/>
-      <c r="H44" s="530" t="s">
+      <c r="H44" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="531"/>
-      <c r="J44" s="531"/>
-      <c r="K44" s="532"/>
-      <c r="L44" s="531" t="s">
+      <c r="I44" s="528"/>
+      <c r="J44" s="528"/>
+      <c r="K44" s="529"/>
+      <c r="L44" s="528" t="s">
         <v>34</v>
       </c>
-      <c r="M44" s="531"/>
-      <c r="N44" s="531"/>
-      <c r="O44" s="532"/>
-      <c r="P44" s="530" t="s">
+      <c r="M44" s="528"/>
+      <c r="N44" s="528"/>
+      <c r="O44" s="529"/>
+      <c r="P44" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="Q44" s="531"/>
-      <c r="R44" s="531"/>
-      <c r="S44" s="532"/>
-      <c r="T44" s="536" t="s">
+      <c r="Q44" s="528"/>
+      <c r="R44" s="528"/>
+      <c r="S44" s="529"/>
+      <c r="T44" s="530" t="s">
         <v>68</v>
       </c>
-      <c r="U44" s="537"/>
-      <c r="V44" s="536" t="s">
+      <c r="U44" s="531"/>
+      <c r="V44" s="530" t="s">
         <v>525</v>
       </c>
-      <c r="W44" s="538"/>
-      <c r="X44" s="538"/>
-      <c r="Y44" s="537"/>
+      <c r="W44" s="532"/>
+      <c r="X44" s="532"/>
+      <c r="Y44" s="531"/>
       <c r="Z44" s="373" t="s">
         <v>537</v>
       </c>
@@ -27859,12 +27859,12 @@
         <v>85</v>
       </c>
       <c r="U90" s="535"/>
-      <c r="V90" s="527" t="s">
+      <c r="V90" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="W90" s="528"/>
-      <c r="X90" s="528"/>
-      <c r="Y90" s="529"/>
+      <c r="W90" s="537"/>
+      <c r="X90" s="537"/>
+      <c r="Y90" s="538"/>
       <c r="Z90" s="60"/>
       <c r="AA90" s="60"/>
       <c r="AB90" s="68" t="s">
@@ -27967,34 +27967,34 @@
       <c r="E92" s="38"/>
       <c r="F92" s="38"/>
       <c r="G92" s="39"/>
-      <c r="H92" s="530" t="s">
+      <c r="H92" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="I92" s="531"/>
-      <c r="J92" s="531"/>
-      <c r="K92" s="532"/>
-      <c r="L92" s="531" t="s">
+      <c r="I92" s="528"/>
+      <c r="J92" s="528"/>
+      <c r="K92" s="529"/>
+      <c r="L92" s="528" t="s">
         <v>34</v>
       </c>
-      <c r="M92" s="531"/>
-      <c r="N92" s="531"/>
-      <c r="O92" s="532"/>
-      <c r="P92" s="530" t="s">
+      <c r="M92" s="528"/>
+      <c r="N92" s="528"/>
+      <c r="O92" s="529"/>
+      <c r="P92" s="527" t="s">
         <v>34</v>
       </c>
-      <c r="Q92" s="531"/>
-      <c r="R92" s="531"/>
-      <c r="S92" s="532"/>
-      <c r="T92" s="536" t="s">
+      <c r="Q92" s="528"/>
+      <c r="R92" s="528"/>
+      <c r="S92" s="529"/>
+      <c r="T92" s="530" t="s">
         <v>68</v>
       </c>
-      <c r="U92" s="537"/>
-      <c r="V92" s="536" t="s">
+      <c r="U92" s="531"/>
+      <c r="V92" s="530" t="s">
         <v>525</v>
       </c>
-      <c r="W92" s="538"/>
-      <c r="X92" s="538"/>
-      <c r="Y92" s="537"/>
+      <c r="W92" s="532"/>
+      <c r="X92" s="532"/>
+      <c r="Y92" s="531"/>
       <c r="Z92" s="373" t="s">
         <v>537</v>
       </c>
@@ -31956,26 +31956,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -31986,6 +31966,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -32131,12 +32131,12 @@
       <c r="I5" s="127"/>
       <c r="J5" s="127"/>
       <c r="K5" s="127"/>
-      <c r="L5" s="527" t="s">
+      <c r="L5" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="528"/>
-      <c r="N5" s="528"/>
-      <c r="O5" s="529"/>
+      <c r="M5" s="537"/>
+      <c r="N5" s="537"/>
+      <c r="O5" s="538"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -32167,12 +32167,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="536" t="s">
+      <c r="L6" s="530" t="s">
         <v>525</v>
       </c>
-      <c r="M6" s="538"/>
-      <c r="N6" s="538"/>
-      <c r="O6" s="537"/>
+      <c r="M6" s="532"/>
+      <c r="N6" s="532"/>
+      <c r="O6" s="531"/>
       <c r="P6" s="373" t="s">
         <v>537</v>
       </c>
@@ -33058,23 +33058,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="527" t="s">
+      <c r="L33" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="528"/>
-      <c r="N33" s="528"/>
-      <c r="O33" s="529"/>
+      <c r="M33" s="537"/>
+      <c r="N33" s="537"/>
+      <c r="O33" s="538"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L34" s="536" t="s">
+      <c r="L34" s="530" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="538"/>
-      <c r="N34" s="538"/>
-      <c r="O34" s="537"/>
+      <c r="M34" s="532"/>
+      <c r="N34" s="532"/>
+      <c r="O34" s="531"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -33421,11 +33421,11 @@
       </c>
       <c r="I4" s="534"/>
       <c r="J4" s="535"/>
-      <c r="K4" s="527" t="s">
+      <c r="K4" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="528"/>
-      <c r="M4" s="529"/>
+      <c r="L4" s="537"/>
+      <c r="M4" s="538"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -33451,16 +33451,16 @@
       <c r="G5" s="381" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="539" t="s">
+      <c r="H5" s="542" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="540"/>
-      <c r="J5" s="541"/>
-      <c r="K5" s="539" t="s">
+      <c r="I5" s="543"/>
+      <c r="J5" s="544"/>
+      <c r="K5" s="542" t="s">
         <v>314</v>
       </c>
-      <c r="L5" s="540"/>
-      <c r="M5" s="541"/>
+      <c r="L5" s="543"/>
+      <c r="M5" s="544"/>
       <c r="N5" s="382" t="s">
         <v>92</v>
       </c>
@@ -33477,23 +33477,23 @@
         <v>218</v>
       </c>
       <c r="AA5" s="207"/>
-      <c r="AB5" s="542" t="s">
+      <c r="AB5" s="539" t="s">
         <v>567</v>
       </c>
-      <c r="AC5" s="542"/>
+      <c r="AC5" s="539"/>
       <c r="AD5" s="384"/>
-      <c r="AE5" s="543" t="s">
+      <c r="AE5" s="540" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="543"/>
-      <c r="AG5" s="543" t="s">
+      <c r="AF5" s="540"/>
+      <c r="AG5" s="540" t="s">
         <v>568</v>
       </c>
-      <c r="AH5" s="543"/>
-      <c r="AI5" s="544" t="s">
+      <c r="AH5" s="540"/>
+      <c r="AI5" s="541" t="s">
         <v>569</v>
       </c>
-      <c r="AJ5" s="544"/>
+      <c r="AJ5" s="541"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="428" t="str">
@@ -34231,12 +34231,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="527" t="s">
+      <c r="L27" s="536" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="528"/>
-      <c r="N27" s="528"/>
-      <c r="O27" s="529"/>
+      <c r="M27" s="537"/>
+      <c r="N27" s="537"/>
+      <c r="O27" s="538"/>
       <c r="T27" s="209"/>
       <c r="U27" s="209"/>
     </row>
@@ -34244,12 +34244,12 @@
       <c r="J28" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L28" s="530" t="s">
+      <c r="L28" s="527" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="531"/>
-      <c r="N28" s="531"/>
-      <c r="O28" s="532"/>
+      <c r="M28" s="528"/>
+      <c r="N28" s="528"/>
+      <c r="O28" s="529"/>
       <c r="T28" s="209"/>
       <c r="U28" s="209"/>
     </row>
@@ -35639,16 +35639,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -36079,103 +36079,103 @@
       <c r="C4" s="279" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="545" t="s">
+      <c r="D4" s="546" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="546"/>
-      <c r="F4" s="546"/>
-      <c r="G4" s="546"/>
+      <c r="E4" s="545"/>
+      <c r="F4" s="545"/>
+      <c r="G4" s="545"/>
       <c r="H4" s="547"/>
-      <c r="I4" s="546" t="s">
+      <c r="I4" s="545" t="s">
         <v>325</v>
       </c>
-      <c r="J4" s="546"/>
-      <c r="K4" s="546"/>
-      <c r="L4" s="546"/>
+      <c r="J4" s="545"/>
+      <c r="K4" s="545"/>
+      <c r="L4" s="545"/>
       <c r="M4" s="547"/>
-      <c r="N4" s="546" t="s">
+      <c r="N4" s="545" t="s">
         <v>326</v>
       </c>
-      <c r="O4" s="546"/>
-      <c r="P4" s="546"/>
-      <c r="Q4" s="546"/>
+      <c r="O4" s="545"/>
+      <c r="P4" s="545"/>
+      <c r="Q4" s="545"/>
       <c r="R4" s="547"/>
-      <c r="S4" s="546" t="s">
+      <c r="S4" s="545" t="s">
         <v>327</v>
       </c>
-      <c r="T4" s="546"/>
-      <c r="U4" s="546"/>
-      <c r="V4" s="546"/>
+      <c r="T4" s="545"/>
+      <c r="U4" s="545"/>
+      <c r="V4" s="545"/>
       <c r="W4" s="547"/>
-      <c r="X4" s="546" t="s">
+      <c r="X4" s="545" t="s">
         <v>328</v>
       </c>
-      <c r="Y4" s="546"/>
-      <c r="Z4" s="546"/>
-      <c r="AA4" s="546"/>
+      <c r="Y4" s="545"/>
+      <c r="Z4" s="545"/>
+      <c r="AA4" s="545"/>
       <c r="AB4" s="547"/>
-      <c r="AC4" s="546" t="s">
+      <c r="AC4" s="545" t="s">
         <v>329</v>
       </c>
-      <c r="AD4" s="546"/>
-      <c r="AE4" s="546"/>
-      <c r="AF4" s="546"/>
+      <c r="AD4" s="545"/>
+      <c r="AE4" s="545"/>
+      <c r="AF4" s="545"/>
       <c r="AG4" s="547"/>
-      <c r="AH4" s="546" t="s">
+      <c r="AH4" s="545" t="s">
         <v>330</v>
       </c>
-      <c r="AI4" s="546"/>
-      <c r="AJ4" s="546"/>
-      <c r="AK4" s="546"/>
+      <c r="AI4" s="545"/>
+      <c r="AJ4" s="545"/>
+      <c r="AK4" s="545"/>
       <c r="AL4" s="547"/>
-      <c r="AM4" s="546" t="s">
+      <c r="AM4" s="545" t="s">
         <v>331</v>
       </c>
-      <c r="AN4" s="546"/>
-      <c r="AO4" s="546"/>
-      <c r="AP4" s="546"/>
+      <c r="AN4" s="545"/>
+      <c r="AO4" s="545"/>
+      <c r="AP4" s="545"/>
       <c r="AQ4" s="547"/>
-      <c r="AR4" s="546" t="s">
+      <c r="AR4" s="545" t="s">
         <v>332</v>
       </c>
-      <c r="AS4" s="546"/>
-      <c r="AT4" s="546"/>
-      <c r="AU4" s="546"/>
+      <c r="AS4" s="545"/>
+      <c r="AT4" s="545"/>
+      <c r="AU4" s="545"/>
       <c r="AV4" s="547"/>
-      <c r="AW4" s="546" t="s">
+      <c r="AW4" s="545" t="s">
         <v>333</v>
       </c>
-      <c r="AX4" s="546"/>
-      <c r="AY4" s="546"/>
-      <c r="AZ4" s="546"/>
-      <c r="BA4" s="546"/>
-      <c r="BB4" s="545" t="s">
+      <c r="AX4" s="545"/>
+      <c r="AY4" s="545"/>
+      <c r="AZ4" s="545"/>
+      <c r="BA4" s="545"/>
+      <c r="BB4" s="546" t="s">
         <v>334</v>
       </c>
-      <c r="BC4" s="546"/>
-      <c r="BD4" s="546"/>
-      <c r="BE4" s="546"/>
+      <c r="BC4" s="545"/>
+      <c r="BD4" s="545"/>
+      <c r="BE4" s="545"/>
       <c r="BF4" s="547"/>
-      <c r="BG4" s="546" t="s">
+      <c r="BG4" s="545" t="s">
         <v>335</v>
       </c>
-      <c r="BH4" s="546"/>
-      <c r="BI4" s="546"/>
-      <c r="BJ4" s="546"/>
-      <c r="BK4" s="546"/>
-      <c r="BL4" s="545" t="s">
+      <c r="BH4" s="545"/>
+      <c r="BI4" s="545"/>
+      <c r="BJ4" s="545"/>
+      <c r="BK4" s="545"/>
+      <c r="BL4" s="546" t="s">
         <v>336</v>
       </c>
-      <c r="BM4" s="546"/>
-      <c r="BN4" s="546"/>
-      <c r="BO4" s="546"/>
-      <c r="BP4" s="546"/>
-      <c r="BQ4" s="545" t="s">
+      <c r="BM4" s="545"/>
+      <c r="BN4" s="545"/>
+      <c r="BO4" s="545"/>
+      <c r="BP4" s="545"/>
+      <c r="BQ4" s="546" t="s">
         <v>337</v>
       </c>
-      <c r="BR4" s="546"/>
-      <c r="BS4" s="546"/>
-      <c r="BT4" s="546"/>
+      <c r="BR4" s="545"/>
+      <c r="BS4" s="545"/>
+      <c r="BT4" s="545"/>
       <c r="BU4" s="547"/>
       <c r="BV4" s="280" t="s">
         <v>338</v>
@@ -49769,6 +49769,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -49781,11 +49786,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -49808,23 +49808,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="552" t="s">
+      <c r="A1" s="554" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="554" t="s">
+      <c r="B1" s="556" t="s">
         <v>612</v>
       </c>
-      <c r="C1" s="555"/>
-      <c r="D1" s="555"/>
-      <c r="E1" s="555"/>
-      <c r="F1" s="556"/>
-      <c r="G1" s="554" t="s">
+      <c r="C1" s="557"/>
+      <c r="D1" s="557"/>
+      <c r="E1" s="557"/>
+      <c r="F1" s="558"/>
+      <c r="G1" s="556" t="s">
         <v>613</v>
       </c>
-      <c r="H1" s="555"/>
-      <c r="I1" s="555"/>
-      <c r="J1" s="555"/>
-      <c r="K1" s="556"/>
+      <c r="H1" s="557"/>
+      <c r="I1" s="557"/>
+      <c r="J1" s="557"/>
+      <c r="K1" s="558"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -49834,7 +49834,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="553"/>
+      <c r="A2" s="555"/>
       <c r="B2" s="450" t="s">
         <v>270</v>
       </c>
@@ -51327,11 +51327,11 @@
       <c r="Y48" t="s">
         <v>662</v>
       </c>
-      <c r="Z48" s="557" t="s">
+      <c r="Z48" s="552" t="s">
         <v>600</v>
       </c>
-      <c r="AA48" s="558"/>
-      <c r="AB48" s="558"/>
+      <c r="AA48" s="553"/>
+      <c r="AB48" s="553"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -51548,11 +51548,11 @@
       <c r="Y53" t="s">
         <v>664</v>
       </c>
-      <c r="Z53" s="557" t="s">
+      <c r="Z53" s="552" t="s">
         <v>599</v>
       </c>
-      <c r="AA53" s="558"/>
-      <c r="AB53" s="558"/>
+      <c r="AA53" s="553"/>
+      <c r="AB53" s="553"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -51754,11 +51754,11 @@
       <c r="Y59" t="s">
         <v>665</v>
       </c>
-      <c r="Z59" s="557" t="s">
+      <c r="Z59" s="552" t="s">
         <v>666</v>
       </c>
-      <c r="AA59" s="558"/>
-      <c r="AB59" s="558"/>
+      <c r="AA59" s="553"/>
+      <c r="AB59" s="553"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="470" t="str">
@@ -52595,17 +52595,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update House numbers - NDQ06
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3A78F9-8EE2-4FF9-AAF9-23CDCB31132F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031AEBA-F47C-4024-9EB7-C20B0E29B4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -13540,6 +13540,15 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13547,15 +13556,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13567,13 +13567,22 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13585,19 +13594,10 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13615,12 +13615,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13635,6 +13629,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -14438,57 +14438,57 @@
       <sheetData sheetId="11">
         <row r="6">
           <cell r="L6">
-            <v>7.5784815901851145E-4</v>
+            <v>3.1499640433377643E-4</v>
           </cell>
         </row>
         <row r="8">
           <cell r="L8">
-            <v>6.1667922907240368E-3</v>
+            <v>2.5632013151118248E-3</v>
           </cell>
         </row>
         <row r="9">
           <cell r="L9">
-            <v>7.3612177725668258E-4</v>
+            <v>3.0596592500527567E-4</v>
           </cell>
         </row>
         <row r="10">
           <cell r="L10">
-            <v>5.2407143773435417E-4</v>
+            <v>2.1782809199424584E-4</v>
           </cell>
         </row>
         <row r="51">
           <cell r="L51">
-            <v>2.045375452121146E-4</v>
+            <v>1.3249013578385519E-4</v>
           </cell>
         </row>
         <row r="53">
           <cell r="L53">
-            <v>4.1672182679251225E-3</v>
+            <v>2.6993348022525303E-3</v>
           </cell>
         </row>
         <row r="54">
           <cell r="L54">
-            <v>5.0182384146831558E-4</v>
+            <v>3.2505870170077217E-4</v>
           </cell>
         </row>
         <row r="55">
           <cell r="L55">
-            <v>3.8041601576060773E-4</v>
+            <v>2.4641622412260611E-4</v>
           </cell>
         </row>
         <row r="96">
           <cell r="L96">
-            <v>3.7645780249386E-3</v>
+            <v>2.4058665241777602E-3</v>
           </cell>
         </row>
         <row r="98">
           <cell r="L98">
-            <v>6.6666794692434245E-3</v>
+            <v>4.2605415152040874E-3</v>
           </cell>
         </row>
         <row r="100">
           <cell r="L100">
-            <v>1.0463165232771768E-3</v>
+            <v>6.686799636959782E-4</v>
           </cell>
         </row>
         <row r="104">
@@ -18390,8 +18390,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AM103"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18550,14 +18550,14 @@
       </c>
       <c r="I6" s="236">
         <f>[1]ArchetypeDemand!$L$51</f>
-        <v>2.045375452121146E-4</v>
+        <v>1.3249013578385519E-4</v>
       </c>
       <c r="J6" s="129">
         <v>2019</v>
       </c>
       <c r="L6" s="3">
         <f>I6/0.0000036</f>
-        <v>56.815984781142944</v>
+        <v>36.802815495515333</v>
       </c>
       <c r="S6" s="223" t="s">
         <v>256</v>
@@ -18620,12 +18620,12 @@
       <c r="H8" s="62"/>
       <c r="I8" s="238">
         <f>[1]ArchetypeDemand!$L$53</f>
-        <v>4.1672182679251225E-3</v>
+        <v>2.6993348022525303E-3</v>
       </c>
       <c r="J8" s="58"/>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
-        <v>1157.5606299792007</v>
+        <v>749.81522284792516</v>
       </c>
       <c r="S8" s="223" t="s">
         <v>258</v>
@@ -18654,12 +18654,12 @@
       <c r="H9" s="63"/>
       <c r="I9" s="237">
         <f>[1]ArchetypeDemand!$L$54</f>
-        <v>5.0182384146831558E-4</v>
+        <v>3.2505870170077217E-4</v>
       </c>
       <c r="J9" s="57"/>
       <c r="L9" s="4">
         <f t="shared" si="0"/>
-        <v>139.39551151897655</v>
+        <v>90.294083805770057</v>
       </c>
       <c r="S9" s="226" t="s">
         <v>259</v>
@@ -18688,12 +18688,12 @@
       <c r="H10" s="86"/>
       <c r="I10" s="239">
         <f>[1]ArchetypeDemand!$L$55</f>
-        <v>3.8041601576060773E-4</v>
+        <v>2.4641622412260611E-4</v>
       </c>
       <c r="J10" s="95"/>
       <c r="L10" s="4">
         <f t="shared" si="0"/>
-        <v>105.67111548905771</v>
+        <v>68.448951145168365</v>
       </c>
       <c r="S10" s="223" t="s">
         <v>260</v>
@@ -18765,14 +18765,14 @@
       </c>
       <c r="I12" s="236">
         <f>[1]ArchetypeDemand!$L$6</f>
-        <v>7.5784815901851145E-4</v>
+        <v>3.1499640433377643E-4</v>
       </c>
       <c r="J12" s="129">
         <v>2019</v>
       </c>
       <c r="L12" s="4">
         <f>I12/0.0000036</f>
-        <v>210.51337750514207</v>
+        <v>87.499001203826793</v>
       </c>
       <c r="S12" s="223" t="s">
         <v>262</v>
@@ -18835,12 +18835,12 @@
       <c r="H14" s="62"/>
       <c r="I14" s="238">
         <f>[1]ArchetypeDemand!$L$8</f>
-        <v>6.1667922907240368E-3</v>
+        <v>2.5632013151118248E-3</v>
       </c>
       <c r="J14" s="58"/>
       <c r="L14" s="4">
         <f t="shared" si="1"/>
-        <v>1712.9978585344547</v>
+        <v>712.00036530884029</v>
       </c>
       <c r="S14" s="231" t="s">
         <v>270</v>
@@ -18869,12 +18869,12 @@
       <c r="H15" s="63"/>
       <c r="I15" s="237">
         <f>[1]ArchetypeDemand!$L$9</f>
-        <v>7.3612177725668258E-4</v>
+        <v>3.0596592500527567E-4</v>
       </c>
       <c r="J15" s="57"/>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>204.4782714601896</v>
+        <v>84.990534723687688</v>
       </c>
       <c r="S15" s="235" t="s">
         <v>271</v>
@@ -18900,12 +18900,12 @@
       <c r="H16" s="86"/>
       <c r="I16" s="239">
         <f>[1]ArchetypeDemand!$L$10</f>
-        <v>5.2407143773435417E-4</v>
+        <v>2.1782809199424584E-4</v>
       </c>
       <c r="J16" s="95"/>
       <c r="L16" s="4">
         <f t="shared" si="1"/>
-        <v>145.57539937065394</v>
+        <v>60.507803331734962</v>
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.2">
@@ -18965,14 +18965,14 @@
       </c>
       <c r="I18" s="236">
         <f>[1]ArchetypeDemand!$L$96</f>
-        <v>3.7645780249386E-3</v>
+        <v>2.4058665241777602E-3</v>
       </c>
       <c r="J18" s="129">
         <v>2019</v>
       </c>
       <c r="L18" s="4">
         <f>I18/0.0000036</f>
-        <v>1045.7161180385001</v>
+        <v>668.29625671604458</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
@@ -19043,12 +19043,12 @@
       <c r="H20" s="62"/>
       <c r="I20" s="238">
         <f>[1]ArchetypeDemand!$L$98</f>
-        <v>6.6666794692434245E-3</v>
+        <v>4.2605415152040874E-3</v>
       </c>
       <c r="J20" s="58"/>
       <c r="L20" s="4">
         <f t="shared" si="2"/>
-        <v>1851.8554081231734</v>
+        <v>1183.4837542233577</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
@@ -19119,12 +19119,12 @@
       <c r="H22" s="86"/>
       <c r="I22" s="239">
         <f>[1]ArchetypeDemand!$L$100</f>
-        <v>1.0463165232771768E-3</v>
+        <v>6.686799636959782E-4</v>
       </c>
       <c r="J22" s="95"/>
       <c r="L22" s="4">
         <f t="shared" si="2"/>
-        <v>290.64347868810466</v>
+        <v>185.74443435999396</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
@@ -20558,7 +20558,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AT166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
@@ -20754,12 +20754,12 @@
         <v>85</v>
       </c>
       <c r="V4" s="535"/>
-      <c r="W4" s="536" t="s">
+      <c r="W4" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="X4" s="537"/>
-      <c r="Y4" s="537"/>
-      <c r="Z4" s="538"/>
+      <c r="X4" s="528"/>
+      <c r="Y4" s="528"/>
+      <c r="Z4" s="529"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="60"/>
       <c r="AC4" s="68" t="s">
@@ -20864,34 +20864,34 @@
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="39"/>
-      <c r="I6" s="527" t="s">
+      <c r="I6" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="528"/>
-      <c r="K6" s="528"/>
-      <c r="L6" s="529"/>
-      <c r="M6" s="528" t="s">
+      <c r="J6" s="531"/>
+      <c r="K6" s="531"/>
+      <c r="L6" s="532"/>
+      <c r="M6" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="528"/>
-      <c r="O6" s="528"/>
-      <c r="P6" s="529"/>
-      <c r="Q6" s="527" t="s">
+      <c r="N6" s="531"/>
+      <c r="O6" s="531"/>
+      <c r="P6" s="532"/>
+      <c r="Q6" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="528"/>
-      <c r="S6" s="528"/>
-      <c r="T6" s="529"/>
-      <c r="U6" s="527" t="s">
+      <c r="R6" s="531"/>
+      <c r="S6" s="531"/>
+      <c r="T6" s="532"/>
+      <c r="U6" s="530" t="s">
         <v>68</v>
       </c>
-      <c r="V6" s="529"/>
-      <c r="W6" s="527" t="s">
+      <c r="V6" s="532"/>
+      <c r="W6" s="530" t="s">
         <v>525</v>
       </c>
-      <c r="X6" s="528"/>
-      <c r="Y6" s="528"/>
-      <c r="Z6" s="529"/>
+      <c r="X6" s="531"/>
+      <c r="Y6" s="531"/>
+      <c r="Z6" s="532"/>
       <c r="AA6" s="61" t="s">
         <v>537</v>
       </c>
@@ -22180,11 +22180,11 @@
       </c>
       <c r="AM19" s="106"/>
       <c r="AN19" s="105" t="str">
-        <f>C25</f>
+        <f t="shared" ref="AN19:AO21" si="17">C25</f>
         <v>R-SW_Apt_ELC_HPN1</v>
       </c>
       <c r="AO19" s="105" t="str">
-        <f>D25</f>
+        <f t="shared" si="17"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AP19" s="106" t="s">
@@ -22283,11 +22283,11 @@
       </c>
       <c r="AM20" s="212"/>
       <c r="AN20" s="105" t="str">
-        <f>C26</f>
+        <f t="shared" si="17"/>
         <v>R-SH_Apt_ELC_HPN3</v>
       </c>
       <c r="AO20" s="105" t="str">
-        <f>D26</f>
+        <f t="shared" si="17"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AP20" s="106" t="s">
@@ -22349,15 +22349,15 @@
         <v>9.5039999999999996</v>
       </c>
       <c r="X21" s="379">
-        <f t="shared" ref="X21:Z21" si="17">X20+0.6+(0.28*5)</f>
+        <f t="shared" ref="X21:Z21" si="18">X20+0.6+(0.28*5)</f>
         <v>8.82864</v>
       </c>
       <c r="Y21" s="379">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.2140623999999995</v>
       </c>
       <c r="Z21" s="379">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.1532799999999988</v>
       </c>
       <c r="AA21" s="379">
@@ -22370,7 +22370,7 @@
       <c r="AF21" s="72"/>
       <c r="AG21" s="72"/>
       <c r="AH21" s="62">
-        <f t="shared" ref="AH21:AH24" si="18">31.536*(AK21/1000)</f>
+        <f t="shared" ref="AH21:AH24" si="19">31.536*(AK21/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI21" s="65"/>
@@ -22382,11 +22382,11 @@
       </c>
       <c r="AM21" s="112"/>
       <c r="AN21" s="108" t="str">
-        <f>C27</f>
+        <f t="shared" si="17"/>
         <v>R-HC_Apt_ELC_HPN2</v>
       </c>
       <c r="AO21" s="108" t="str">
-        <f>D27</f>
+        <f t="shared" si="17"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AP21" s="109" t="s">
@@ -22448,15 +22448,15 @@
         <v>9.6039999999999992</v>
       </c>
       <c r="X22" s="379">
-        <f t="shared" ref="X22:Z22" si="19">X20+0.6+(0.3*5)</f>
+        <f t="shared" ref="X22:Z22" si="20">X20+0.6+(0.3*5)</f>
         <v>8.9286399999999997</v>
       </c>
       <c r="Y22" s="379">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.314062400000001</v>
       </c>
       <c r="Z22" s="379">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.2532800000000002</v>
       </c>
       <c r="AA22" s="379">
@@ -22469,7 +22469,7 @@
       <c r="AF22" s="72"/>
       <c r="AG22" s="72"/>
       <c r="AH22" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI22" s="65"/>
@@ -22547,15 +22547,15 @@
         <v>10.103999999999999</v>
       </c>
       <c r="X23" s="379">
-        <f t="shared" ref="X23:Z23" si="20">X20+0.6+(0.4*5)</f>
+        <f t="shared" ref="X23:Z23" si="21">X20+0.6+(0.4*5)</f>
         <v>9.4286399999999997</v>
       </c>
       <c r="Y23" s="379">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8.814062400000001</v>
       </c>
       <c r="Z23" s="379">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8.7532800000000002</v>
       </c>
       <c r="AA23" s="379">
@@ -22568,7 +22568,7 @@
       <c r="AF23" s="72"/>
       <c r="AG23" s="72"/>
       <c r="AH23" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI23" s="65"/>
@@ -22646,15 +22646,15 @@
         <v>10.603999999999999</v>
       </c>
       <c r="X24" s="379">
-        <f t="shared" ref="X24:Z24" si="21">X20+0.6+(0.5*5)</f>
+        <f t="shared" ref="X24:Z24" si="22">X20+0.6+(0.5*5)</f>
         <v>9.9286399999999997</v>
       </c>
       <c r="Y24" s="379">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.314062400000001</v>
       </c>
       <c r="Z24" s="379">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.2532800000000002</v>
       </c>
       <c r="AA24" s="379">
@@ -22667,7 +22667,7 @@
       <c r="AF24" s="72"/>
       <c r="AG24" s="72"/>
       <c r="AH24" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI24" s="65"/>
@@ -22740,15 +22740,15 @@
         <v>0.7</v>
       </c>
       <c r="R25" s="23">
-        <f t="shared" ref="R25:T25" si="22">J25*0.7</f>
+        <f t="shared" ref="R25:T25" si="23">J25*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="S25" s="23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.86333333333333329</v>
       </c>
       <c r="T25" s="57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="U25" s="53">
@@ -23129,15 +23129,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="R29" s="20">
-        <f t="shared" ref="R29:T29" si="23">J29*0.7</f>
+        <f t="shared" ref="R29:T29" si="24">J29*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="S29" s="20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="T29" s="56">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.4691358024691357</v>
       </c>
       <c r="U29" s="89">
@@ -23171,7 +23171,7 @@
       <c r="AF29" s="85"/>
       <c r="AG29" s="85"/>
       <c r="AH29" s="85">
-        <f t="shared" ref="AH29:AH30" si="24">31.536*(AK29/1000)</f>
+        <f t="shared" ref="AH29:AH30" si="25">31.536*(AK29/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AI29" s="88"/>
@@ -23244,15 +23244,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="R30" s="26">
-        <f t="shared" ref="R30" si="25">J30*0.7</f>
+        <f t="shared" ref="R30" si="26">J30*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="S30" s="26">
-        <f t="shared" ref="S30" si="26">K30*0.7</f>
+        <f t="shared" ref="S30" si="27">K30*0.7</f>
         <v>1.2055555555555555</v>
       </c>
       <c r="T30" s="59">
-        <f t="shared" ref="T30" si="27">L30*0.7</f>
+        <f t="shared" ref="T30" si="28">L30*0.7</f>
         <v>1.2444444444444445</v>
       </c>
       <c r="U30" s="27">
@@ -23286,7 +23286,7 @@
       <c r="AF30" s="64"/>
       <c r="AG30" s="64"/>
       <c r="AH30" s="64">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AI30" s="67"/>
@@ -23401,11 +23401,11 @@
         <v>2.4464999999999999</v>
       </c>
       <c r="S32" s="26">
-        <f t="shared" ref="S32:T32" si="28">K32*0.7</f>
+        <f t="shared" ref="S32:T32" si="29">K32*0.7</f>
         <v>2.625</v>
       </c>
       <c r="T32" s="59">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.625</v>
       </c>
       <c r="U32" s="256">
@@ -23574,7 +23574,7 @@
       <c r="AF34" s="85"/>
       <c r="AG34" s="85"/>
       <c r="AH34" s="85">
-        <f t="shared" ref="AH34:AH35" si="29">31.536*(AK34/1000)</f>
+        <f t="shared" ref="AH34:AH35" si="30">31.536*(AK34/1000)</f>
         <v>0.56764799999999993</v>
       </c>
       <c r="AI34" s="88"/>
@@ -23660,7 +23660,7 @@
       <c r="AF35" s="63"/>
       <c r="AG35" s="63"/>
       <c r="AH35" s="64">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.56764799999999993</v>
       </c>
       <c r="AI35" s="67"/>
@@ -23777,7 +23777,7 @@
       <c r="AF37" s="85"/>
       <c r="AG37" s="85"/>
       <c r="AH37" s="85">
-        <f t="shared" ref="AH37:AH38" si="30">31.536*(AK37/1000)</f>
+        <f t="shared" ref="AH37:AH38" si="31">31.536*(AK37/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI37" s="88"/>
@@ -23867,7 +23867,7 @@
       <c r="AF38" s="63"/>
       <c r="AG38" s="63"/>
       <c r="AH38" s="63">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI38" s="66"/>
@@ -24035,7 +24035,7 @@
       <c r="AF40" s="85"/>
       <c r="AG40" s="85"/>
       <c r="AH40" s="85">
-        <f t="shared" ref="AH40:AH41" si="31">31.536*(AK40/1000)</f>
+        <f t="shared" ref="AH40:AH41" si="32">31.536*(AK40/1000)</f>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI40" s="88"/>
@@ -24139,7 +24139,7 @@
       <c r="AF41" s="63"/>
       <c r="AG41" s="63"/>
       <c r="AH41" s="64">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.15768000000000001</v>
       </c>
       <c r="AI41" s="67"/>
@@ -24320,11 +24320,11 @@
         <v>31</v>
       </c>
       <c r="AN45" s="105" t="str">
-        <f t="shared" ref="AN45:AN60" si="32">C49</f>
+        <f t="shared" ref="AN45:AN60" si="33">C49</f>
         <v>R-SH_Att_KER_N1</v>
       </c>
       <c r="AO45" s="105" t="str">
-        <f t="shared" ref="AO45:AO60" si="33">D49</f>
+        <f t="shared" ref="AO45:AO60" si="34">D49</f>
         <v>Residential Kerosene Heating Oil - New 1 SH</v>
       </c>
       <c r="AP45" s="106" t="s">
@@ -24377,12 +24377,12 @@
         <v>85</v>
       </c>
       <c r="V46" s="535"/>
-      <c r="W46" s="536" t="s">
+      <c r="W46" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="X46" s="537"/>
-      <c r="Y46" s="537"/>
-      <c r="Z46" s="538"/>
+      <c r="X46" s="528"/>
+      <c r="Y46" s="528"/>
+      <c r="Z46" s="529"/>
       <c r="AA46" s="60"/>
       <c r="AB46" s="60"/>
       <c r="AC46" s="68" t="s">
@@ -24410,11 +24410,11 @@
       <c r="AK46" s="60"/>
       <c r="AM46" s="106"/>
       <c r="AN46" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_KER_N1</v>
       </c>
       <c r="AO46" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AP46" s="106" t="s">
@@ -24468,11 +24468,11 @@
       <c r="AK47" s="372"/>
       <c r="AM47" s="106"/>
       <c r="AN47" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_KER_N2</v>
       </c>
       <c r="AO47" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AP47" s="106" t="s">
@@ -24495,34 +24495,34 @@
       <c r="F48" s="38"/>
       <c r="G48" s="38"/>
       <c r="H48" s="39"/>
-      <c r="I48" s="527" t="s">
+      <c r="I48" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="J48" s="528"/>
-      <c r="K48" s="528"/>
-      <c r="L48" s="529"/>
-      <c r="M48" s="528" t="s">
+      <c r="J48" s="531"/>
+      <c r="K48" s="531"/>
+      <c r="L48" s="532"/>
+      <c r="M48" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="N48" s="528"/>
-      <c r="O48" s="528"/>
-      <c r="P48" s="529"/>
-      <c r="Q48" s="527" t="s">
+      <c r="N48" s="531"/>
+      <c r="O48" s="531"/>
+      <c r="P48" s="532"/>
+      <c r="Q48" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="R48" s="528"/>
-      <c r="S48" s="528"/>
-      <c r="T48" s="529"/>
-      <c r="U48" s="530" t="s">
+      <c r="R48" s="531"/>
+      <c r="S48" s="531"/>
+      <c r="T48" s="532"/>
+      <c r="U48" s="536" t="s">
         <v>68</v>
       </c>
-      <c r="V48" s="531"/>
-      <c r="W48" s="530" t="s">
+      <c r="V48" s="537"/>
+      <c r="W48" s="536" t="s">
         <v>525</v>
       </c>
-      <c r="X48" s="532"/>
-      <c r="Y48" s="532"/>
-      <c r="Z48" s="531"/>
+      <c r="X48" s="538"/>
+      <c r="Y48" s="538"/>
+      <c r="Z48" s="537"/>
       <c r="AA48" s="373" t="s">
         <v>537</v>
       </c>
@@ -24554,11 +24554,11 @@
       </c>
       <c r="AM48" s="106"/>
       <c r="AN48" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_KER_N3</v>
       </c>
       <c r="AO48" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AP48" s="107" t="s">
@@ -24615,15 +24615,15 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="X49" s="379">
-        <f t="shared" ref="X49:Z49" si="34">X53*1.3</f>
+        <f t="shared" ref="X49:Z49" si="35">X53*1.3</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y49" s="379">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z49" s="379">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="AA49" s="379">
@@ -24636,7 +24636,7 @@
       <c r="AF49" s="72"/>
       <c r="AG49" s="72"/>
       <c r="AH49" s="62">
-        <f t="shared" ref="AH49:AH87" si="35">31.536*(AK49/1000)</f>
+        <f t="shared" ref="AH49:AH87" si="36">31.536*(AK49/1000)</f>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI49" s="65"/>
@@ -24648,11 +24648,11 @@
       </c>
       <c r="AM49" s="106"/>
       <c r="AN49" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Att_GAS_N1</v>
       </c>
       <c r="AO49" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AP49" s="106" t="s">
@@ -24703,15 +24703,15 @@
         <v>0.7</v>
       </c>
       <c r="R50" s="23">
-        <f t="shared" ref="R50:R52" si="36">J50*0.7</f>
+        <f t="shared" ref="R50:R52" si="37">J50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S50" s="23">
-        <f t="shared" ref="S50:S52" si="37">K50*0.7</f>
+        <f t="shared" ref="S50:S52" si="38">K50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T50" s="57">
-        <f t="shared" ref="T50:T52" si="38">L50*0.7</f>
+        <f t="shared" ref="T50:T52" si="39">L50*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U50" s="53">
@@ -24723,15 +24723,15 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="X50" s="380">
-        <f t="shared" ref="X50:Z50" si="39">X54*1.3</f>
+        <f t="shared" ref="X50:Z50" si="40">X54*1.3</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y50" s="380">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="Z50" s="380">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>4.2773760330578519</v>
       </c>
       <c r="AA50" s="380">
@@ -24744,7 +24744,7 @@
       <c r="AF50" s="73"/>
       <c r="AG50" s="73"/>
       <c r="AH50" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI50" s="66"/>
@@ -24756,11 +24756,11 @@
       </c>
       <c r="AM50" s="106"/>
       <c r="AN50" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_GAS_N1</v>
       </c>
       <c r="AO50" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AP50" s="106" t="s">
@@ -24811,15 +24811,15 @@
         <v>0.7</v>
       </c>
       <c r="R51" s="29">
-        <f t="shared" si="36"/>
-        <v>0.7</v>
-      </c>
-      <c r="S51" s="29">
         <f t="shared" si="37"/>
         <v>0.7</v>
       </c>
+      <c r="S51" s="29">
+        <f t="shared" si="38"/>
+        <v>0.7</v>
+      </c>
       <c r="T51" s="58">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.7</v>
       </c>
       <c r="U51" s="54">
@@ -24857,7 +24857,7 @@
         <v>5</v>
       </c>
       <c r="AH51" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI51" s="65"/>
@@ -24869,11 +24869,11 @@
       </c>
       <c r="AM51" s="106"/>
       <c r="AN51" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_GAS_N2</v>
       </c>
       <c r="AO51" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AP51" s="106" t="s">
@@ -24924,15 +24924,15 @@
         <v>0.7</v>
       </c>
       <c r="R52" s="23">
-        <f t="shared" si="36"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S52" s="23">
         <f t="shared" si="37"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="S52" s="23">
+        <f t="shared" si="38"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="T52" s="57">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="U52" s="53">
@@ -24982,11 +24982,11 @@
       </c>
       <c r="AM52" s="106"/>
       <c r="AN52" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_GAS_N3</v>
       </c>
       <c r="AO52" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AP52" s="106" t="s">
@@ -25045,15 +25045,15 @@
         <v>3.25</v>
       </c>
       <c r="X53" s="379">
-        <f t="shared" ref="X53:Z53" si="40">3.25</f>
+        <f t="shared" ref="X53:Z53" si="41">3.25</f>
         <v>3.25</v>
       </c>
       <c r="Y53" s="379">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3.25</v>
       </c>
       <c r="Z53" s="379">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3.25</v>
       </c>
       <c r="AA53" s="379">
@@ -25066,7 +25066,7 @@
       <c r="AF53" s="72"/>
       <c r="AG53" s="72"/>
       <c r="AH53" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI53" s="65"/>
@@ -25078,11 +25078,11 @@
       </c>
       <c r="AM53" s="106"/>
       <c r="AN53" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Att_LPG_N1</v>
       </c>
       <c r="AO53" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AP53" s="106" t="s">
@@ -25133,15 +25133,15 @@
         <v>0.7</v>
       </c>
       <c r="R54" s="23">
-        <f t="shared" ref="R54:R56" si="41">J54*0.7</f>
+        <f t="shared" ref="R54:R56" si="42">J54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S54" s="23">
-        <f t="shared" ref="S54:S56" si="42">K54*0.7</f>
+        <f t="shared" ref="S54:S56" si="43">K54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T54" s="57">
-        <f t="shared" ref="T54:T56" si="43">L54*0.7</f>
+        <f t="shared" ref="T54:T56" si="44">L54*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U54" s="53">
@@ -25174,7 +25174,7 @@
       <c r="AF54" s="73"/>
       <c r="AG54" s="73"/>
       <c r="AH54" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI54" s="66"/>
@@ -25186,11 +25186,11 @@
       </c>
       <c r="AM54" s="106"/>
       <c r="AN54" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_LPG_N1</v>
       </c>
       <c r="AO54" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AP54" s="106" t="s">
@@ -25241,15 +25241,15 @@
         <v>0.7</v>
       </c>
       <c r="R55" s="29">
-        <f t="shared" si="41"/>
-        <v>0.7</v>
-      </c>
-      <c r="S55" s="29">
         <f t="shared" si="42"/>
         <v>0.7</v>
       </c>
+      <c r="S55" s="29">
+        <f t="shared" si="43"/>
+        <v>0.7</v>
+      </c>
       <c r="T55" s="58">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.7</v>
       </c>
       <c r="U55" s="54">
@@ -25285,7 +25285,7 @@
         <v>5</v>
       </c>
       <c r="AH55" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI55" s="65"/>
@@ -25297,11 +25297,11 @@
       </c>
       <c r="AM55" s="106"/>
       <c r="AN55" s="105" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Att_WOO_N1</v>
       </c>
       <c r="AO55" s="105" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AP55" s="106" t="s">
@@ -25352,15 +25352,15 @@
         <v>0.7</v>
       </c>
       <c r="R56" s="23">
-        <f t="shared" si="41"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S56" s="23">
         <f t="shared" si="42"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="S56" s="23">
+        <f t="shared" si="43"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="T56" s="57">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="U56" s="53">
@@ -25398,7 +25398,7 @@
         <v>5</v>
       </c>
       <c r="AH56" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI56" s="66"/>
@@ -25410,11 +25410,11 @@
       </c>
       <c r="AM56" s="109"/>
       <c r="AN56" s="108" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_WOO_N1</v>
       </c>
       <c r="AO56" s="108" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AP56" s="109" t="s">
@@ -25495,7 +25495,7 @@
       <c r="AF57" s="72"/>
       <c r="AG57" s="72"/>
       <c r="AH57" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI57" s="65"/>
@@ -25510,7 +25510,7 @@
         <v>587</v>
       </c>
       <c r="AO57" s="108" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential  Stove New 1 - SH</v>
       </c>
       <c r="AP57" s="106" t="s">
@@ -25559,15 +25559,15 @@
         <v>0.7</v>
       </c>
       <c r="R58" s="23">
-        <f t="shared" ref="R58" si="44">J58*0.7</f>
+        <f t="shared" ref="R58" si="45">J58*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S58" s="23">
-        <f t="shared" ref="S58" si="45">K58*0.7</f>
+        <f t="shared" ref="S58" si="46">K58*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T58" s="57">
-        <f t="shared" ref="T58" si="46">L58*0.7</f>
+        <f t="shared" ref="T58" si="47">L58*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U58" s="53">
@@ -25601,7 +25601,7 @@
       <c r="AF58" s="73"/>
       <c r="AG58" s="73"/>
       <c r="AH58" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI58" s="66"/>
@@ -25616,7 +25616,7 @@
         <v>588</v>
       </c>
       <c r="AO58" s="108" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential  Stove with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AP58" s="109" t="s">
@@ -25693,7 +25693,7 @@
       <c r="AF59" s="72"/>
       <c r="AG59" s="72"/>
       <c r="AH59" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI59" s="65"/>
@@ -25705,11 +25705,11 @@
       </c>
       <c r="AM59" s="109"/>
       <c r="AN59" s="108" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SH_Att_HVO_N1</v>
       </c>
       <c r="AO59" s="108" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AP59" s="109" t="s">
@@ -25756,19 +25756,19 @@
       <c r="O60" s="32"/>
       <c r="P60" s="45"/>
       <c r="Q60" s="22">
-        <f t="shared" ref="Q60:T64" si="47">I60*0.7</f>
+        <f t="shared" ref="Q60:T64" si="48">I60*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R60" s="23">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.7</v>
       </c>
       <c r="S60" s="23">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.7</v>
       </c>
       <c r="T60" s="57">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.7</v>
       </c>
       <c r="U60" s="53">
@@ -25801,7 +25801,7 @@
       <c r="AF60" s="73"/>
       <c r="AG60" s="73"/>
       <c r="AH60" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI60" s="66"/>
@@ -25813,11 +25813,11 @@
       </c>
       <c r="AM60" s="109"/>
       <c r="AN60" s="108" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>R-SW_Att_HVO_N1</v>
       </c>
       <c r="AO60" s="108" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AP60" s="109" t="s">
@@ -25897,7 +25897,7 @@
       <c r="AF61" s="73"/>
       <c r="AG61" s="73"/>
       <c r="AH61" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI61" s="66"/>
@@ -25960,19 +25960,19 @@
       <c r="O62" s="32"/>
       <c r="P62" s="45"/>
       <c r="Q62" s="22">
-        <f t="shared" ref="Q62" si="48">I62*0.7</f>
+        <f t="shared" ref="Q62" si="49">I62*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="R62" s="23">
-        <f t="shared" ref="R62" si="49">J62*0.7</f>
+        <f t="shared" ref="R62" si="50">J62*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="S62" s="23">
-        <f t="shared" ref="S62" si="50">K62*0.7</f>
+        <f t="shared" ref="S62" si="51">K62*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="T62" s="57">
-        <f t="shared" ref="T62" si="51">L62*0.7</f>
+        <f t="shared" ref="T62" si="52">L62*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="U62" s="53">
@@ -26005,7 +26005,7 @@
       <c r="AF62" s="73"/>
       <c r="AG62" s="73"/>
       <c r="AH62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI62" s="66"/>
@@ -26017,11 +26017,11 @@
       </c>
       <c r="AM62" s="104"/>
       <c r="AN62" s="103" t="str">
-        <f t="shared" ref="AN62:AO68" si="52">C68</f>
+        <f t="shared" ref="AN62:AO68" si="53">C68</f>
         <v>R-SH_Att_ELC_HPN1</v>
       </c>
       <c r="AO62" s="103" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AP62" s="104" t="s">
@@ -26079,19 +26079,19 @@
         <v>4.2250000000000005</v>
       </c>
       <c r="X63" s="62">
-        <f t="shared" ref="X63:AA64" si="53">X49</f>
+        <f t="shared" ref="X63:AA64" si="54">X49</f>
         <v>4.2250000000000005</v>
       </c>
       <c r="Y63" s="62">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="Z63" s="62">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>4.2250000000000005</v>
       </c>
       <c r="AA63" s="62">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>0.12</v>
       </c>
       <c r="AB63" s="65"/>
@@ -26113,11 +26113,11 @@
       </c>
       <c r="AM63" s="106"/>
       <c r="AN63" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-HC_Att_ELC_HPN1</v>
       </c>
       <c r="AO63" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AP63" s="106" t="s">
@@ -26163,19 +26163,19 @@
       <c r="O64" s="50"/>
       <c r="P64" s="51"/>
       <c r="Q64" s="252">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="R64" s="26">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="S64" s="26">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="T64" s="59">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="U64" s="55">
@@ -26187,19 +26187,19 @@
         <v>4.2773760330578519</v>
       </c>
       <c r="X64" s="62">
-        <f t="shared" ref="X64:Z64" si="54">X50</f>
+        <f t="shared" ref="X64:Z64" si="55">X50</f>
         <v>4.2773760330578519</v>
       </c>
       <c r="Y64" s="62">
+        <f t="shared" si="55"/>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="Z64" s="62">
+        <f t="shared" si="55"/>
+        <v>4.2773760330578519</v>
+      </c>
+      <c r="AA64" s="62">
         <f t="shared" si="54"/>
-        <v>4.2773760330578519</v>
-      </c>
-      <c r="Z64" s="62">
-        <f t="shared" si="54"/>
-        <v>4.2773760330578519</v>
-      </c>
-      <c r="AA64" s="62">
-        <f t="shared" si="53"/>
         <v>0.12</v>
       </c>
       <c r="AB64" s="66"/>
@@ -26209,7 +26209,7 @@
       <c r="AF64" s="73"/>
       <c r="AG64" s="73"/>
       <c r="AH64" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI64" s="67"/>
@@ -26221,11 +26221,11 @@
       </c>
       <c r="AM64" s="106"/>
       <c r="AN64" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-SH_Att_ELC_HPN2</v>
       </c>
       <c r="AO64" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AP64" s="106" t="s">
@@ -26279,11 +26279,11 @@
       <c r="AK65" s="34"/>
       <c r="AM65" s="106"/>
       <c r="AN65" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-SW_Att_ELC_HPN1</v>
       </c>
       <c r="AO65" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AP65" s="106" t="s">
@@ -26364,7 +26364,7 @@
       <c r="AF66" s="84"/>
       <c r="AG66" s="84"/>
       <c r="AH66" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.63072000000000006</v>
       </c>
       <c r="AI66" s="83"/>
@@ -26376,11 +26376,11 @@
       </c>
       <c r="AM66" s="212"/>
       <c r="AN66" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-SW_Att_ELC_HPN2</v>
       </c>
       <c r="AO66" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AP66" s="106" t="s">
@@ -26434,11 +26434,11 @@
       <c r="AK67" s="34"/>
       <c r="AM67" s="212"/>
       <c r="AN67" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-SH_Att_ELC_HPN3</v>
       </c>
       <c r="AO67" s="105" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AP67" s="106" t="s">
@@ -26524,7 +26524,7 @@
       <c r="AF68" s="85"/>
       <c r="AG68" s="85"/>
       <c r="AH68" s="85">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.220752</v>
       </c>
       <c r="AI68" s="88"/>
@@ -26536,11 +26536,11 @@
       </c>
       <c r="AM68" s="112"/>
       <c r="AN68" s="108" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>R-HC_Att_ELC_HPN2</v>
       </c>
       <c r="AO68" s="108" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AP68" s="109" t="s">
@@ -26637,7 +26637,7 @@
       <c r="AF69" s="63"/>
       <c r="AG69" s="63"/>
       <c r="AH69" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AI69" s="66"/>
@@ -26737,7 +26737,7 @@
       <c r="AF70" s="62"/>
       <c r="AG70" s="62"/>
       <c r="AH70" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.220752</v>
       </c>
       <c r="AI70" s="65"/>
@@ -26809,15 +26809,15 @@
         <v>0.7</v>
       </c>
       <c r="R71" s="23">
-        <f t="shared" ref="R71:R72" si="55">J71*0.7</f>
+        <f t="shared" ref="R71:R72" si="56">J71*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="S71" s="23">
-        <f t="shared" ref="S71:S72" si="56">K71*0.7</f>
+        <f t="shared" ref="S71:S72" si="57">K71*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="T71" s="57">
-        <f t="shared" ref="T71:T72" si="57">L71*0.7</f>
+        <f t="shared" ref="T71:T72" si="58">L71*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="U71" s="53">
@@ -26850,7 +26850,7 @@
       <c r="AF71" s="63"/>
       <c r="AG71" s="63"/>
       <c r="AH71" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AI71" s="66"/>
@@ -26919,15 +26919,15 @@
         <v>0.7</v>
       </c>
       <c r="R72" s="29">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="S72" s="29">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T72" s="58">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="U72" s="54">
@@ -26965,7 +26965,7 @@
         <v>5</v>
       </c>
       <c r="AH72" s="62">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AI72" s="65"/>
@@ -27068,7 +27068,7 @@
       <c r="AF73" s="63"/>
       <c r="AG73" s="63"/>
       <c r="AH73" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.220752</v>
       </c>
       <c r="AI73" s="66"/>
@@ -27183,7 +27183,7 @@
       <c r="AF74" s="86"/>
       <c r="AG74" s="86"/>
       <c r="AH74" s="86">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.26805600000000002</v>
       </c>
       <c r="AI74" s="91"/>
@@ -27314,15 +27314,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="R76" s="20">
-        <f t="shared" ref="R76:R77" si="58">J76*0.7</f>
+        <f t="shared" ref="R76:R77" si="59">J76*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="S76" s="20">
-        <f t="shared" ref="S76:S77" si="59">K76*0.7</f>
+        <f t="shared" ref="S76:S77" si="60">K76*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T76" s="56">
-        <f t="shared" ref="T76:T77" si="60">L76*0.7</f>
+        <f t="shared" ref="T76:T77" si="61">L76*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="U76" s="89">
@@ -27356,7 +27356,7 @@
       <c r="AF76" s="85"/>
       <c r="AG76" s="85"/>
       <c r="AH76" s="85">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI76" s="88"/>
@@ -27429,15 +27429,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="R77" s="26">
-        <f t="shared" si="58"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="S77" s="26">
         <f t="shared" si="59"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="S77" s="26">
+        <f t="shared" si="60"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="T77" s="59">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="U77" s="27">
@@ -27564,15 +27564,15 @@
         <v>2.2084999999999999</v>
       </c>
       <c r="R79" s="26">
-        <f t="shared" ref="R79" si="61">J79*0.7</f>
+        <f t="shared" ref="R79" si="62">J79*0.7</f>
         <v>2.4464999999999999</v>
       </c>
       <c r="S79" s="26">
-        <f t="shared" ref="S79" si="62">K79*0.7</f>
+        <f t="shared" ref="S79" si="63">K79*0.7</f>
         <v>2.625</v>
       </c>
       <c r="T79" s="59">
-        <f t="shared" ref="T79" si="63">L79*0.7</f>
+        <f t="shared" ref="T79" si="64">L79*0.7</f>
         <v>2.625</v>
       </c>
       <c r="U79" s="3">
@@ -27583,15 +27583,15 @@
         <v>9.5138179028489738</v>
       </c>
       <c r="X79" s="79">
-        <f t="shared" ref="X79:Z79" si="64">(X71+X54)*0.8</f>
+        <f t="shared" ref="X79:Z79" si="65">(X71+X54)*0.8</f>
         <v>8.8944751180388462</v>
       </c>
       <c r="Y79" s="79">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>8.3308731838616321</v>
       </c>
       <c r="Z79" s="79">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>8.2751323332287203</v>
       </c>
       <c r="AA79" s="371">
@@ -27612,7 +27612,7 @@
         <v>5</v>
       </c>
       <c r="AH79" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.45017639999999998</v>
       </c>
       <c r="AI79" s="83"/>
@@ -27738,7 +27738,7 @@
       <c r="AF81" s="85"/>
       <c r="AG81" s="85"/>
       <c r="AH81" s="85">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI81" s="88"/>
@@ -27824,7 +27824,7 @@
       <c r="AF82" s="64"/>
       <c r="AG82" s="64"/>
       <c r="AH82" s="64">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.7884000000000001</v>
       </c>
       <c r="AI82" s="67"/>
@@ -27941,7 +27941,7 @@
       <c r="AF84" s="85"/>
       <c r="AG84" s="85"/>
       <c r="AH84" s="85">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AI84" s="88"/>
@@ -28021,7 +28021,7 @@
       <c r="AF85" s="63"/>
       <c r="AG85" s="63"/>
       <c r="AH85" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AI85" s="67"/>
@@ -28141,7 +28141,7 @@
       <c r="AF87" s="93"/>
       <c r="AG87" s="93"/>
       <c r="AH87" s="93">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.18921600000000002</v>
       </c>
       <c r="AI87" s="92"/>
@@ -28384,12 +28384,12 @@
         <v>85</v>
       </c>
       <c r="V94" s="535"/>
-      <c r="W94" s="536" t="s">
+      <c r="W94" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="X94" s="537"/>
-      <c r="Y94" s="537"/>
-      <c r="Z94" s="538"/>
+      <c r="X94" s="528"/>
+      <c r="Y94" s="528"/>
+      <c r="Z94" s="529"/>
       <c r="AA94" s="60"/>
       <c r="AB94" s="60"/>
       <c r="AC94" s="68" t="s">
@@ -28417,11 +28417,11 @@
       <c r="AK94" s="60"/>
       <c r="AM94" s="106"/>
       <c r="AN94" s="105" t="str">
-        <f t="shared" ref="AN94:AN108" si="65">C98</f>
+        <f t="shared" ref="AN94:AN108" si="66">C98</f>
         <v>R-SW_Det_KER_N1</v>
       </c>
       <c r="AO94" s="105" t="str">
-        <f t="shared" ref="AO94:AO108" si="66">D98</f>
+        <f t="shared" ref="AO94:AO108" si="67">D98</f>
         <v>Residential Kerosene Heating Oil - New 2 SH + WH</v>
       </c>
       <c r="AP94" s="106" t="s">
@@ -28475,11 +28475,11 @@
       <c r="AK95" s="372"/>
       <c r="AM95" s="106"/>
       <c r="AN95" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_KER_N2</v>
       </c>
       <c r="AO95" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Solar</v>
       </c>
       <c r="AP95" s="106" t="s">
@@ -28502,34 +28502,34 @@
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
       <c r="H96" s="39"/>
-      <c r="I96" s="527" t="s">
+      <c r="I96" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="J96" s="528"/>
-      <c r="K96" s="528"/>
-      <c r="L96" s="529"/>
-      <c r="M96" s="528" t="s">
+      <c r="J96" s="531"/>
+      <c r="K96" s="531"/>
+      <c r="L96" s="532"/>
+      <c r="M96" s="531" t="s">
         <v>34</v>
       </c>
-      <c r="N96" s="528"/>
-      <c r="O96" s="528"/>
-      <c r="P96" s="529"/>
-      <c r="Q96" s="527" t="s">
+      <c r="N96" s="531"/>
+      <c r="O96" s="531"/>
+      <c r="P96" s="532"/>
+      <c r="Q96" s="530" t="s">
         <v>34</v>
       </c>
-      <c r="R96" s="528"/>
-      <c r="S96" s="528"/>
-      <c r="T96" s="529"/>
-      <c r="U96" s="530" t="s">
+      <c r="R96" s="531"/>
+      <c r="S96" s="531"/>
+      <c r="T96" s="532"/>
+      <c r="U96" s="536" t="s">
         <v>68</v>
       </c>
-      <c r="V96" s="531"/>
-      <c r="W96" s="530" t="s">
+      <c r="V96" s="537"/>
+      <c r="W96" s="536" t="s">
         <v>525</v>
       </c>
-      <c r="X96" s="532"/>
-      <c r="Y96" s="532"/>
-      <c r="Z96" s="531"/>
+      <c r="X96" s="538"/>
+      <c r="Y96" s="538"/>
+      <c r="Z96" s="537"/>
       <c r="AA96" s="373" t="s">
         <v>537</v>
       </c>
@@ -28561,11 +28561,11 @@
       </c>
       <c r="AM96" s="106"/>
       <c r="AN96" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_KER_N3</v>
       </c>
       <c r="AO96" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Kerosene Heating Oil - New 3 SH+WH + Wood Stove</v>
       </c>
       <c r="AP96" s="107" t="s">
@@ -28622,15 +28622,15 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="X97" s="379">
-        <f t="shared" ref="X97:Z97" si="67">X101*1.3</f>
+        <f t="shared" ref="X97:Z97" si="68">X101*1.3</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y97" s="379">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z97" s="379">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="AA97" s="379">
@@ -28643,7 +28643,7 @@
       <c r="AF97" s="72"/>
       <c r="AG97" s="72"/>
       <c r="AH97" s="62">
-        <f t="shared" ref="AH97:AH135" si="68">31.536*(AK97/1000)</f>
+        <f t="shared" ref="AH97:AH135" si="69">31.536*(AK97/1000)</f>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI97" s="65"/>
@@ -28655,11 +28655,11 @@
       </c>
       <c r="AM97" s="106"/>
       <c r="AN97" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SH_Det_GAS_N1</v>
       </c>
       <c r="AO97" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Natural Gas Heating - New 1 SH</v>
       </c>
       <c r="AP97" s="106" t="s">
@@ -28710,15 +28710,15 @@
         <v>0.7</v>
       </c>
       <c r="R98" s="23">
-        <f t="shared" ref="R98:R100" si="69">J98*0.7</f>
+        <f t="shared" ref="R98:R100" si="70">J98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S98" s="23">
-        <f t="shared" ref="S98:S100" si="70">K98*0.7</f>
+        <f t="shared" ref="S98:S100" si="71">K98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T98" s="57">
-        <f t="shared" ref="T98:T100" si="71">L98*0.7</f>
+        <f t="shared" ref="T98:T100" si="72">L98*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U98" s="53">
@@ -28730,15 +28730,15 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="X98" s="380">
-        <f t="shared" ref="X98:Z98" si="72">X102*1.3</f>
+        <f t="shared" ref="X98:Z98" si="73">X102*1.3</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y98" s="380">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z98" s="380">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="AA98" s="380">
@@ -28751,7 +28751,7 @@
       <c r="AF98" s="73"/>
       <c r="AG98" s="73"/>
       <c r="AH98" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI98" s="66"/>
@@ -28763,11 +28763,11 @@
       </c>
       <c r="AM98" s="106"/>
       <c r="AN98" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_GAS_N1</v>
       </c>
       <c r="AO98" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Natural Gas Heating - New 2 SH + WH</v>
       </c>
       <c r="AP98" s="106" t="s">
@@ -28818,15 +28818,15 @@
         <v>0.7</v>
       </c>
       <c r="R99" s="29">
-        <f t="shared" si="69"/>
-        <v>0.7</v>
-      </c>
-      <c r="S99" s="29">
         <f t="shared" si="70"/>
         <v>0.7</v>
       </c>
+      <c r="S99" s="29">
+        <f t="shared" si="71"/>
+        <v>0.7</v>
+      </c>
       <c r="T99" s="58">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>0.7</v>
       </c>
       <c r="U99" s="54">
@@ -28864,7 +28864,7 @@
         <v>5</v>
       </c>
       <c r="AH99" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI99" s="65"/>
@@ -28876,11 +28876,11 @@
       </c>
       <c r="AM99" s="106"/>
       <c r="AN99" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_GAS_N2</v>
       </c>
       <c r="AO99" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Natural Gas Heating - New 3 SH + WH + Solar</v>
       </c>
       <c r="AP99" s="106" t="s">
@@ -28931,15 +28931,15 @@
         <v>0.7</v>
       </c>
       <c r="R100" s="23">
-        <f t="shared" si="69"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S100" s="23">
         <f t="shared" si="70"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="S100" s="23">
+        <f t="shared" si="71"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="T100" s="57">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="U100" s="53">
@@ -28977,7 +28977,7 @@
         <v>5</v>
       </c>
       <c r="AH100" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI100" s="66"/>
@@ -28989,11 +28989,11 @@
       </c>
       <c r="AM100" s="106"/>
       <c r="AN100" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_GAS_N3</v>
       </c>
       <c r="AO100" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Natural Gas Heating - New 4 SH + WH + Wood Stove</v>
       </c>
       <c r="AP100" s="106" t="s">
@@ -29052,15 +29052,15 @@
         <v>3.5249999999999999</v>
       </c>
       <c r="X101" s="379">
-        <f t="shared" ref="X101:Z101" si="73">3.525</f>
+        <f t="shared" ref="X101:Z101" si="74">3.525</f>
         <v>3.5249999999999999</v>
       </c>
       <c r="Y101" s="379">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="Z101" s="379">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="AA101" s="379">
@@ -29073,7 +29073,7 @@
       <c r="AF101" s="72"/>
       <c r="AG101" s="72"/>
       <c r="AH101" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI101" s="65"/>
@@ -29085,11 +29085,11 @@
       </c>
       <c r="AM101" s="106"/>
       <c r="AN101" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SH_Det_LPG_N1</v>
       </c>
       <c r="AO101" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Liquid Petroleum Gas- New 1 SH</v>
       </c>
       <c r="AP101" s="106" t="s">
@@ -29140,15 +29140,15 @@
         <v>0.7</v>
       </c>
       <c r="R102" s="23">
-        <f t="shared" ref="R102:R104" si="74">J102*0.7</f>
+        <f t="shared" ref="R102:R104" si="75">J102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S102" s="23">
-        <f t="shared" ref="S102:S104" si="75">K102*0.7</f>
+        <f t="shared" ref="S102:S104" si="76">K102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T102" s="57">
-        <f t="shared" ref="T102:T104" si="76">L102*0.7</f>
+        <f t="shared" ref="T102:T104" si="77">L102*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U102" s="53">
@@ -29181,7 +29181,7 @@
       <c r="AF102" s="73"/>
       <c r="AG102" s="73"/>
       <c r="AH102" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI102" s="66"/>
@@ -29193,11 +29193,11 @@
       </c>
       <c r="AM102" s="106"/>
       <c r="AN102" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_LPG_N1</v>
       </c>
       <c r="AO102" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Liquid Petroleum Gas- New 2 SH + WH</v>
       </c>
       <c r="AP102" s="106" t="s">
@@ -29248,15 +29248,15 @@
         <v>0.7</v>
       </c>
       <c r="R103" s="29">
-        <f t="shared" si="74"/>
-        <v>0.7</v>
-      </c>
-      <c r="S103" s="29">
         <f t="shared" si="75"/>
         <v>0.7</v>
       </c>
+      <c r="S103" s="29">
+        <f t="shared" si="76"/>
+        <v>0.7</v>
+      </c>
       <c r="T103" s="58">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.7</v>
       </c>
       <c r="U103" s="54">
@@ -29292,7 +29292,7 @@
         <v>5</v>
       </c>
       <c r="AH103" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI103" s="65"/>
@@ -29304,11 +29304,11 @@
       </c>
       <c r="AM103" s="106"/>
       <c r="AN103" s="105" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SH_Det_WOO_N1</v>
       </c>
       <c r="AO103" s="105" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Biomass Boiler - New 1 SH</v>
       </c>
       <c r="AP103" s="106" t="s">
@@ -29359,15 +29359,15 @@
         <v>0.7</v>
       </c>
       <c r="R104" s="23">
-        <f t="shared" si="74"/>
-        <v>0.71749999999999992</v>
-      </c>
-      <c r="S104" s="23">
         <f t="shared" si="75"/>
         <v>0.71749999999999992</v>
       </c>
+      <c r="S104" s="23">
+        <f t="shared" si="76"/>
+        <v>0.71749999999999992</v>
+      </c>
       <c r="T104" s="57">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>0.71749999999999992</v>
       </c>
       <c r="U104" s="53">
@@ -29405,7 +29405,7 @@
         <v>5</v>
       </c>
       <c r="AH104" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI104" s="66"/>
@@ -29417,11 +29417,11 @@
       </c>
       <c r="AM104" s="109"/>
       <c r="AN104" s="108" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_WOO_N1</v>
       </c>
       <c r="AO104" s="108" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential Biomass Boiler - New 2 SH + WH</v>
       </c>
       <c r="AP104" s="109" t="s">
@@ -29476,19 +29476,19 @@
       </c>
       <c r="V105" s="41"/>
       <c r="W105" s="379">
-        <f t="shared" ref="W105:Z106" si="77">W101+0.3</f>
+        <f t="shared" ref="W105:Z106" si="78">W101+0.3</f>
         <v>3.8249999999999997</v>
       </c>
       <c r="X105" s="379">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="Y105" s="379">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="Z105" s="379">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>3.8249999999999997</v>
       </c>
       <c r="AA105" s="379">
@@ -29502,7 +29502,7 @@
       <c r="AF105" s="72"/>
       <c r="AG105" s="72"/>
       <c r="AH105" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI105" s="65"/>
@@ -29517,7 +29517,7 @@
         <v>595</v>
       </c>
       <c r="AO105" s="108" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential  Stove New 1 - SH</v>
       </c>
       <c r="AP105" s="106" t="s">
@@ -29566,15 +29566,15 @@
         <v>0.7</v>
       </c>
       <c r="R106" s="23">
-        <f t="shared" ref="R106" si="78">J106*0.7</f>
+        <f t="shared" ref="R106" si="79">J106*0.7</f>
         <v>0.7</v>
       </c>
       <c r="S106" s="23">
-        <f t="shared" ref="S106" si="79">K106*0.7</f>
+        <f t="shared" ref="S106" si="80">K106*0.7</f>
         <v>0.7</v>
       </c>
       <c r="T106" s="57">
-        <f t="shared" ref="T106" si="80">L106*0.7</f>
+        <f t="shared" ref="T106" si="81">L106*0.7</f>
         <v>0.7</v>
       </c>
       <c r="U106" s="53">
@@ -29582,19 +29582,19 @@
       </c>
       <c r="V106" s="25"/>
       <c r="W106" s="380">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="X106" s="380">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="Y106" s="380">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="Z106" s="380">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>4.1040057915057915</v>
       </c>
       <c r="AA106" s="379">
@@ -29608,7 +29608,7 @@
       <c r="AF106" s="73"/>
       <c r="AG106" s="73"/>
       <c r="AH106" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI106" s="66"/>
@@ -29623,7 +29623,7 @@
         <v>596</v>
       </c>
       <c r="AO106" s="108" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential  Stove with back boiler New 1 - SH +WH</v>
       </c>
       <c r="AP106" s="109" t="s">
@@ -29700,7 +29700,7 @@
       <c r="AF107" s="72"/>
       <c r="AG107" s="72"/>
       <c r="AH107" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI107" s="65"/>
@@ -29712,11 +29712,11 @@
       </c>
       <c r="AM107" s="109"/>
       <c r="AN107" s="108" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SH_Det_HVO_N1</v>
       </c>
       <c r="AO107" s="108" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH</v>
       </c>
       <c r="AP107" s="109" t="s">
@@ -29763,19 +29763,19 @@
       <c r="O108" s="32"/>
       <c r="P108" s="45"/>
       <c r="Q108" s="22">
-        <f t="shared" ref="Q108:T108" si="81">I108*0.7</f>
+        <f t="shared" ref="Q108:T108" si="82">I108*0.7</f>
         <v>0.7</v>
       </c>
       <c r="R108" s="23">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>0.7</v>
       </c>
       <c r="S108" s="23">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>0.7</v>
       </c>
       <c r="T108" s="57">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>0.7</v>
       </c>
       <c r="U108" s="53">
@@ -29787,15 +29787,15 @@
         <v>22.778925619834713</v>
       </c>
       <c r="X108" s="380">
-        <f t="shared" ref="X108" si="82">X107*($V$156/$V$155)</f>
+        <f t="shared" ref="X108" si="83">X107*($V$156/$V$155)</f>
         <v>22.04476084710744</v>
       </c>
       <c r="Y108" s="380">
-        <f t="shared" ref="Y108" si="83">Y107*($V$156/$V$155)</f>
+        <f t="shared" ref="Y108" si="84">Y107*($V$156/$V$155)</f>
         <v>20.839163429752066</v>
       </c>
       <c r="Z108" s="380">
-        <f t="shared" ref="Z108" si="84">Z107*($V$156/$V$155)</f>
+        <f t="shared" ref="Z108" si="85">Z107*($V$156/$V$155)</f>
         <v>18.635439049586779</v>
       </c>
       <c r="AA108" s="380">
@@ -29808,7 +29808,7 @@
       <c r="AF108" s="73"/>
       <c r="AG108" s="73"/>
       <c r="AH108" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI108" s="66"/>
@@ -29820,11 +29820,11 @@
       </c>
       <c r="AM108" s="109"/>
       <c r="AN108" s="108" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>R-SW_Det_HVO_N1</v>
       </c>
       <c r="AO108" s="108" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>Residential  Hydrotreated vegetable oil - New 1 SH + WH</v>
       </c>
       <c r="AP108" s="109" t="s">
@@ -29904,7 +29904,7 @@
       <c r="AF109" s="73"/>
       <c r="AG109" s="73"/>
       <c r="AH109" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI109" s="66"/>
@@ -29967,19 +29967,19 @@
       <c r="O110" s="32"/>
       <c r="P110" s="45"/>
       <c r="Q110" s="22">
-        <f t="shared" ref="Q110:Q112" si="85">I110*0.7</f>
+        <f t="shared" ref="Q110:Q112" si="86">I110*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="R110" s="23">
-        <f t="shared" ref="R110:R112" si="86">J110*0.7</f>
+        <f t="shared" ref="R110:R112" si="87">J110*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="S110" s="23">
-        <f t="shared" ref="S110:S112" si="87">K110*0.7</f>
+        <f t="shared" ref="S110:S112" si="88">K110*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="T110" s="57">
-        <f t="shared" ref="T110:T112" si="88">L110*0.7</f>
+        <f t="shared" ref="T110:T112" si="89">L110*0.7</f>
         <v>0.38500000000000001</v>
       </c>
       <c r="U110" s="53">
@@ -30012,7 +30012,7 @@
       <c r="AF110" s="73"/>
       <c r="AG110" s="73"/>
       <c r="AH110" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI110" s="66"/>
@@ -30024,11 +30024,11 @@
       </c>
       <c r="AM110" s="104"/>
       <c r="AN110" s="103" t="str">
-        <f t="shared" ref="AN110:AN116" si="89">C116</f>
+        <f t="shared" ref="AN110:AN116" si="90">C116</f>
         <v>R-SH_Det_ELC_HPN1</v>
       </c>
       <c r="AO110" s="103" t="str">
-        <f t="shared" ref="AO110:AO116" si="90">D116</f>
+        <f t="shared" ref="AO110:AO116" si="91">D116</f>
         <v>Residential Electric Heat Pump - Air to Air - SH</v>
       </c>
       <c r="AP110" s="104" t="s">
@@ -30086,19 +30086,19 @@
         <v>4.5825000000000005</v>
       </c>
       <c r="X111" s="62">
-        <f t="shared" ref="X111:AA111" si="91">X97</f>
+        <f t="shared" ref="X111:AA111" si="92">X97</f>
         <v>4.5825000000000005</v>
       </c>
       <c r="Y111" s="62">
-        <f t="shared" si="91"/>
+        <f t="shared" si="92"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="Z111" s="62">
-        <f t="shared" si="91"/>
+        <f t="shared" si="92"/>
         <v>4.5825000000000005</v>
       </c>
       <c r="AA111" s="62">
-        <f t="shared" si="91"/>
+        <f t="shared" si="92"/>
         <v>0.12</v>
       </c>
       <c r="AB111" s="65"/>
@@ -30108,7 +30108,7 @@
       <c r="AF111" s="72"/>
       <c r="AG111" s="72"/>
       <c r="AH111" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI111" s="65"/>
@@ -30120,11 +30120,11 @@
       </c>
       <c r="AM111" s="106"/>
       <c r="AN111" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-HC_Det_ELC_HPN1</v>
       </c>
       <c r="AO111" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Air to Air - SH + SC</v>
       </c>
       <c r="AP111" s="106" t="s">
@@ -30170,19 +30170,19 @@
       <c r="O112" s="50"/>
       <c r="P112" s="51"/>
       <c r="Q112" s="252">
-        <f t="shared" si="85"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="R112" s="26">
         <f t="shared" si="86"/>
         <v>0.57399999999999995</v>
       </c>
-      <c r="S112" s="26">
+      <c r="R112" s="26">
         <f t="shared" si="87"/>
         <v>0.57399999999999995</v>
       </c>
+      <c r="S112" s="26">
+        <f t="shared" si="88"/>
+        <v>0.57399999999999995</v>
+      </c>
       <c r="T112" s="59">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>0.57399999999999995</v>
       </c>
       <c r="U112" s="55">
@@ -30194,19 +30194,19 @@
         <v>4.9452075289575284</v>
       </c>
       <c r="X112" s="62">
-        <f t="shared" ref="X112:AA112" si="92">X98</f>
+        <f t="shared" ref="X112:AA112" si="93">X98</f>
         <v>4.9452075289575284</v>
       </c>
       <c r="Y112" s="62">
-        <f t="shared" si="92"/>
+        <f t="shared" si="93"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="Z112" s="62">
-        <f t="shared" si="92"/>
+        <f t="shared" si="93"/>
         <v>4.9452075289575284</v>
       </c>
       <c r="AA112" s="62">
-        <f t="shared" si="92"/>
+        <f t="shared" si="93"/>
         <v>0.12</v>
       </c>
       <c r="AB112" s="66"/>
@@ -30216,7 +30216,7 @@
       <c r="AF112" s="73"/>
       <c r="AG112" s="73"/>
       <c r="AH112" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI112" s="67"/>
@@ -30228,11 +30228,11 @@
       </c>
       <c r="AM112" s="106"/>
       <c r="AN112" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-SH_Det_ELC_HPN2</v>
       </c>
       <c r="AO112" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Air to Water - SH</v>
       </c>
       <c r="AP112" s="106" t="s">
@@ -30286,11 +30286,11 @@
       <c r="AK113" s="34"/>
       <c r="AM113" s="106"/>
       <c r="AN113" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-SW_Det_ELC_HPN1</v>
       </c>
       <c r="AO113" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH</v>
       </c>
       <c r="AP113" s="106" t="s">
@@ -30371,7 +30371,7 @@
       <c r="AF114" s="84"/>
       <c r="AG114" s="84"/>
       <c r="AH114" s="82">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.94608000000000003</v>
       </c>
       <c r="AI114" s="83"/>
@@ -30383,11 +30383,11 @@
       </c>
       <c r="AM114" s="212"/>
       <c r="AN114" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-SW_Det_ELC_HPN2</v>
       </c>
       <c r="AO114" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Air to Water - SH + WH + Solar</v>
       </c>
       <c r="AP114" s="106" t="s">
@@ -30441,11 +30441,11 @@
       <c r="AK115" s="34"/>
       <c r="AM115" s="212"/>
       <c r="AN115" s="105" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-SH_Det_ELC_HPN3</v>
       </c>
       <c r="AO115" s="105" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH</v>
       </c>
       <c r="AP115" s="106" t="s">
@@ -30528,7 +30528,7 @@
       <c r="AF116" s="85"/>
       <c r="AG116" s="85"/>
       <c r="AH116" s="85">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AI116" s="88"/>
@@ -30540,11 +30540,11 @@
       </c>
       <c r="AM116" s="112"/>
       <c r="AN116" s="108" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" si="90"/>
         <v>R-HC_Det_ELC_HPN2</v>
       </c>
       <c r="AO116" s="108" t="str">
-        <f t="shared" si="90"/>
+        <f t="shared" si="91"/>
         <v>Residential Electric Heat Pump - Ground to Water - SH + SC</v>
       </c>
       <c r="AP116" s="109" t="s">
@@ -30635,7 +30635,7 @@
       <c r="AF117" s="63"/>
       <c r="AG117" s="63"/>
       <c r="AH117" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AI117" s="66"/>
@@ -30732,7 +30732,7 @@
       <c r="AF118" s="62"/>
       <c r="AG118" s="62"/>
       <c r="AH118" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AI118" s="65"/>
@@ -30801,15 +30801,15 @@
         <v>0.7</v>
       </c>
       <c r="R119" s="23">
-        <f t="shared" ref="R119:R120" si="93">J119*0.7</f>
+        <f t="shared" ref="R119:R120" si="94">J119*0.7</f>
         <v>0.76999999999999991</v>
       </c>
       <c r="S119" s="23">
-        <f t="shared" ref="S119:S120" si="94">K119*0.7</f>
+        <f t="shared" ref="S119:S120" si="95">K119*0.7</f>
         <v>0.86333333333333329</v>
       </c>
       <c r="T119" s="57">
-        <f t="shared" ref="T119:T120" si="95">L119*0.7</f>
+        <f t="shared" ref="T119:T120" si="96">L119*0.7</f>
         <v>0.93333333333333324</v>
       </c>
       <c r="U119" s="53">
@@ -30821,15 +30821,15 @@
         <v>9.9300970464135023</v>
       </c>
       <c r="X119" s="380">
-        <f t="shared" ref="X119" si="96">X118*($V$154/$V$153)</f>
+        <f t="shared" ref="X119" si="97">X118*($V$154/$V$153)</f>
         <v>9.0363883122362889</v>
       </c>
       <c r="Y119" s="380">
-        <f t="shared" ref="Y119" si="97">Y118*($V$154/$V$153)</f>
+        <f t="shared" ref="Y119" si="98">Y118*($V$154/$V$153)</f>
         <v>8.2231133641350223</v>
       </c>
       <c r="Z119" s="380">
-        <f t="shared" ref="Z119" si="98">Z118*($V$154/$V$153)</f>
+        <f t="shared" ref="Z119" si="99">Z118*($V$154/$V$153)</f>
         <v>8.1426795780590719</v>
       </c>
       <c r="AA119" s="380">
@@ -30842,7 +30842,7 @@
       <c r="AF119" s="63"/>
       <c r="AG119" s="63"/>
       <c r="AH119" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AI119" s="66"/>
@@ -30911,15 +30911,15 @@
         <v>0.7</v>
       </c>
       <c r="R120" s="29">
-        <f t="shared" si="93"/>
+        <f t="shared" si="94"/>
         <v>0.77700000000000002</v>
       </c>
       <c r="S120" s="29">
-        <f t="shared" si="94"/>
+        <f t="shared" si="95"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="T120" s="58">
-        <f t="shared" si="95"/>
+        <f t="shared" si="96"/>
         <v>0.83299999999999996</v>
       </c>
       <c r="U120" s="54">
@@ -30957,7 +30957,7 @@
         <v>5</v>
       </c>
       <c r="AH120" s="62">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AI120" s="65"/>
@@ -31056,7 +31056,7 @@
       <c r="AF121" s="63"/>
       <c r="AG121" s="63"/>
       <c r="AH121" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.31536000000000003</v>
       </c>
       <c r="AI121" s="66"/>
@@ -31163,7 +31163,7 @@
       <c r="AF122" s="86"/>
       <c r="AG122" s="86"/>
       <c r="AH122" s="86">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.37843200000000005</v>
       </c>
       <c r="AI122" s="91"/>
@@ -31175,11 +31175,11 @@
       </c>
       <c r="AM122" s="215"/>
       <c r="AN122" s="103" t="str">
-        <f t="shared" ref="AN122:AN123" si="99">C132</f>
+        <f t="shared" ref="AN122:AN123" si="100">C132</f>
         <v>R-WH_Det_ELC_N1</v>
       </c>
       <c r="AO122" s="103" t="str">
-        <f t="shared" ref="AO122:AO123" si="100">D132</f>
+        <f t="shared" ref="AO122:AO123" si="101">D132</f>
         <v xml:space="preserve">Residential Electric Water Heater </v>
       </c>
       <c r="AP122" s="104" t="s">
@@ -31233,11 +31233,11 @@
       <c r="AK123" s="34"/>
       <c r="AM123" s="2"/>
       <c r="AN123" s="105" t="str">
-        <f t="shared" si="99"/>
+        <f t="shared" si="100"/>
         <v>R-WH_Det_SOL_N1</v>
       </c>
       <c r="AO123" s="105" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="101"/>
         <v xml:space="preserve">Residential Solar Water Heater </v>
       </c>
       <c r="AP123" s="106" t="s">
@@ -31294,15 +31294,15 @@
         <v>1.1666666666666667</v>
       </c>
       <c r="R124" s="20">
-        <f t="shared" ref="R124:R125" si="101">J124*0.7</f>
+        <f t="shared" ref="R124:R125" si="102">J124*0.7</f>
         <v>1.2530864197530862</v>
       </c>
       <c r="S124" s="20">
-        <f t="shared" ref="S124:S125" si="102">K124*0.7</f>
+        <f t="shared" ref="S124:S125" si="103">K124*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="T124" s="56">
-        <f t="shared" ref="T124:T125" si="103">L124*0.7</f>
+        <f t="shared" ref="T124:T125" si="104">L124*0.7</f>
         <v>1.4691358024691357</v>
       </c>
       <c r="U124" s="89">
@@ -31336,7 +31336,7 @@
       <c r="AF124" s="85"/>
       <c r="AG124" s="85"/>
       <c r="AH124" s="85">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI124" s="88"/>
@@ -31409,15 +31409,15 @@
         <v>1.1666666666666665</v>
       </c>
       <c r="R125" s="26">
-        <f t="shared" si="101"/>
-        <v>1.2055555555555555</v>
-      </c>
-      <c r="S125" s="26">
         <f t="shared" si="102"/>
         <v>1.2055555555555555</v>
       </c>
+      <c r="S125" s="26">
+        <f t="shared" si="103"/>
+        <v>1.2055555555555555</v>
+      </c>
       <c r="T125" s="59">
-        <f t="shared" si="103"/>
+        <f t="shared" si="104"/>
         <v>1.2444444444444445</v>
       </c>
       <c r="U125" s="27">
@@ -31451,7 +31451,7 @@
       <c r="AF125" s="64"/>
       <c r="AG125" s="64"/>
       <c r="AH125" s="64">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI125" s="67"/>
@@ -31544,15 +31544,15 @@
         <v>2.2084999999999999</v>
       </c>
       <c r="R127" s="26">
-        <f t="shared" ref="R127" si="104">J127*0.7</f>
+        <f t="shared" ref="R127" si="105">J127*0.7</f>
         <v>2.4464999999999999</v>
       </c>
       <c r="S127" s="26">
-        <f t="shared" ref="S127" si="105">K127*0.7</f>
+        <f t="shared" ref="S127" si="106">K127*0.7</f>
         <v>2.625</v>
       </c>
       <c r="T127" s="59">
-        <f t="shared" ref="T127" si="106">L127*0.7</f>
+        <f t="shared" ref="T127" si="107">L127*0.7</f>
         <v>2.625</v>
       </c>
       <c r="U127" s="3">
@@ -31563,15 +31563,15 @@
         <v>10.987282270335434</v>
       </c>
       <c r="X127" s="79">
-        <f t="shared" ref="X127:Z127" si="107">(X119+X102)*0.8</f>
+        <f t="shared" ref="X127:Z127" si="108">(X119+X102)*0.8</f>
         <v>10.272315282993665</v>
       </c>
       <c r="Y127" s="79">
-        <f t="shared" si="107"/>
+        <f t="shared" si="108"/>
         <v>9.6216953245126504</v>
       </c>
       <c r="Z127" s="79">
-        <f t="shared" si="107"/>
+        <f t="shared" si="108"/>
         <v>9.5573482956518898</v>
       </c>
       <c r="AA127" s="371">
@@ -31592,7 +31592,7 @@
         <v>5</v>
       </c>
       <c r="AH127" s="82">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.66540960000000005</v>
       </c>
       <c r="AI127" s="83"/>
@@ -31718,7 +31718,7 @@
       <c r="AF129" s="85"/>
       <c r="AG129" s="85"/>
       <c r="AH129" s="85">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI129" s="88"/>
@@ -31804,7 +31804,7 @@
       <c r="AF130" s="64"/>
       <c r="AG130" s="64"/>
       <c r="AH130" s="64">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>1.1983680000000001</v>
       </c>
       <c r="AI130" s="67"/>
@@ -31921,7 +31921,7 @@
       <c r="AF132" s="85"/>
       <c r="AG132" s="85"/>
       <c r="AH132" s="85">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AI132" s="88"/>
@@ -32001,7 +32001,7 @@
       <c r="AF133" s="63"/>
       <c r="AG133" s="63"/>
       <c r="AH133" s="63">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AI133" s="67"/>
@@ -32118,7 +32118,7 @@
       <c r="AF135" s="93"/>
       <c r="AG135" s="93"/>
       <c r="AH135" s="93">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>0.25228800000000001</v>
       </c>
       <c r="AI135" s="92"/>
@@ -32202,7 +32202,7 @@
         <v>3</v>
       </c>
       <c r="V149" s="377">
-        <f t="shared" ref="V149:V158" si="108">W149/$W$157</f>
+        <f t="shared" ref="V149:V158" si="109">W149/$W$157</f>
         <v>0.72929037751472525</v>
       </c>
       <c r="W149" s="378">
@@ -32216,7 +32216,7 @@
         <v>5</v>
       </c>
       <c r="V150" s="377">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.79101166159768732</v>
       </c>
       <c r="W150" s="378">
@@ -32229,7 +32229,7 @@
         <v>8</v>
       </c>
       <c r="V151" s="377">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.85077698714062355</v>
       </c>
       <c r="W151" s="378">
@@ -32242,7 +32242,7 @@
         <v>10</v>
       </c>
       <c r="V152" s="377">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.86872586872586877</v>
       </c>
       <c r="W152" s="376">
@@ -32262,7 +32262,7 @@
         <v>15</v>
       </c>
       <c r="V153" s="367">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.91505791505791501</v>
       </c>
       <c r="W153" s="3">
@@ -32289,7 +32289,7 @@
         <v>18</v>
       </c>
       <c r="V154" s="367">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.92277992277992282</v>
       </c>
       <c r="W154" s="3">
@@ -32318,7 +32318,7 @@
         <v>20</v>
       </c>
       <c r="V155" s="377">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.93436293436293438</v>
       </c>
       <c r="W155" s="376">
@@ -32348,7 +32348,7 @@
         <v>24</v>
       </c>
       <c r="V156" s="367">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>0.94594594594594594</v>
       </c>
       <c r="W156" s="3">
@@ -32377,7 +32377,7 @@
         <v>30</v>
       </c>
       <c r="V157" s="367">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
       <c r="W157" s="3">
@@ -32406,7 +32406,7 @@
         <v>35</v>
       </c>
       <c r="V158" s="367">
-        <f t="shared" si="108"/>
+        <f t="shared" si="109"/>
         <v>1.0791505791505791</v>
       </c>
       <c r="W158" s="3">
@@ -32451,6 +32451,26 @@
     <row r="166" spans="14:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="I96:L96"/>
+    <mergeCell ref="M96:P96"/>
+    <mergeCell ref="Q96:T96"/>
+    <mergeCell ref="U96:V96"/>
+    <mergeCell ref="W96:Z96"/>
+    <mergeCell ref="I94:L94"/>
+    <mergeCell ref="M94:P94"/>
+    <mergeCell ref="Q94:T94"/>
+    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="W94:Z94"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="M48:P48"/>
+    <mergeCell ref="Q48:T48"/>
+    <mergeCell ref="U48:V48"/>
+    <mergeCell ref="W48:Z48"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="M46:P46"/>
+    <mergeCell ref="Q46:T46"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="W46:Z46"/>
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="W6:Z6"/>
     <mergeCell ref="I4:L4"/>
@@ -32461,26 +32481,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="M46:P46"/>
-    <mergeCell ref="Q46:T46"/>
-    <mergeCell ref="U46:V46"/>
-    <mergeCell ref="W46:Z46"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="M48:P48"/>
-    <mergeCell ref="Q48:T48"/>
-    <mergeCell ref="U48:V48"/>
-    <mergeCell ref="W48:Z48"/>
-    <mergeCell ref="I94:L94"/>
-    <mergeCell ref="M94:P94"/>
-    <mergeCell ref="Q94:T94"/>
-    <mergeCell ref="U94:V94"/>
-    <mergeCell ref="W94:Z94"/>
-    <mergeCell ref="I96:L96"/>
-    <mergeCell ref="M96:P96"/>
-    <mergeCell ref="Q96:T96"/>
-    <mergeCell ref="U96:V96"/>
-    <mergeCell ref="W96:Z96"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -32626,12 +32626,12 @@
       <c r="I5" s="127"/>
       <c r="J5" s="127"/>
       <c r="K5" s="127"/>
-      <c r="L5" s="536" t="s">
+      <c r="L5" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="537"/>
-      <c r="N5" s="537"/>
-      <c r="O5" s="538"/>
+      <c r="M5" s="528"/>
+      <c r="N5" s="528"/>
+      <c r="O5" s="529"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -32662,12 +32662,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="530" t="s">
+      <c r="L6" s="536" t="s">
         <v>525</v>
       </c>
-      <c r="M6" s="532"/>
-      <c r="N6" s="532"/>
-      <c r="O6" s="531"/>
+      <c r="M6" s="538"/>
+      <c r="N6" s="538"/>
+      <c r="O6" s="537"/>
       <c r="P6" s="373" t="s">
         <v>537</v>
       </c>
@@ -33553,23 +33553,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="536" t="s">
+      <c r="L33" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="537"/>
-      <c r="N33" s="537"/>
-      <c r="O33" s="538"/>
+      <c r="M33" s="528"/>
+      <c r="N33" s="528"/>
+      <c r="O33" s="529"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L34" s="530" t="s">
+      <c r="L34" s="536" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="532"/>
-      <c r="N34" s="532"/>
-      <c r="O34" s="531"/>
+      <c r="M34" s="538"/>
+      <c r="N34" s="538"/>
+      <c r="O34" s="537"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -33916,11 +33916,11 @@
       </c>
       <c r="I4" s="534"/>
       <c r="J4" s="535"/>
-      <c r="K4" s="536" t="s">
+      <c r="K4" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="537"/>
-      <c r="M4" s="538"/>
+      <c r="L4" s="528"/>
+      <c r="M4" s="529"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -33946,16 +33946,16 @@
       <c r="G5" s="381" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="542" t="s">
+      <c r="H5" s="539" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="543"/>
-      <c r="J5" s="544"/>
-      <c r="K5" s="542" t="s">
+      <c r="I5" s="540"/>
+      <c r="J5" s="541"/>
+      <c r="K5" s="539" t="s">
         <v>314</v>
       </c>
-      <c r="L5" s="543"/>
-      <c r="M5" s="544"/>
+      <c r="L5" s="540"/>
+      <c r="M5" s="541"/>
       <c r="N5" s="382" t="s">
         <v>92</v>
       </c>
@@ -33972,23 +33972,23 @@
         <v>218</v>
       </c>
       <c r="AA5" s="207"/>
-      <c r="AB5" s="539" t="s">
+      <c r="AB5" s="542" t="s">
         <v>567</v>
       </c>
-      <c r="AC5" s="539"/>
+      <c r="AC5" s="542"/>
       <c r="AD5" s="384"/>
-      <c r="AE5" s="540" t="s">
+      <c r="AE5" s="543" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="540"/>
-      <c r="AG5" s="540" t="s">
+      <c r="AF5" s="543"/>
+      <c r="AG5" s="543" t="s">
         <v>568</v>
       </c>
-      <c r="AH5" s="540"/>
-      <c r="AI5" s="541" t="s">
+      <c r="AH5" s="543"/>
+      <c r="AI5" s="544" t="s">
         <v>569</v>
       </c>
-      <c r="AJ5" s="541"/>
+      <c r="AJ5" s="544"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="428" t="str">
@@ -34726,12 +34726,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="536" t="s">
+      <c r="L27" s="527" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="537"/>
-      <c r="N27" s="537"/>
-      <c r="O27" s="538"/>
+      <c r="M27" s="528"/>
+      <c r="N27" s="528"/>
+      <c r="O27" s="529"/>
       <c r="T27" s="209"/>
       <c r="U27" s="209"/>
     </row>
@@ -34739,12 +34739,12 @@
       <c r="J28" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L28" s="527" t="s">
+      <c r="L28" s="530" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="528"/>
-      <c r="N28" s="528"/>
-      <c r="O28" s="529"/>
+      <c r="M28" s="531"/>
+      <c r="N28" s="531"/>
+      <c r="O28" s="532"/>
       <c r="T28" s="209"/>
       <c r="U28" s="209"/>
     </row>
@@ -36134,16 +36134,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -36574,103 +36574,103 @@
       <c r="C4" s="279" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="546" t="s">
+      <c r="D4" s="545" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="545"/>
-      <c r="F4" s="545"/>
-      <c r="G4" s="545"/>
+      <c r="E4" s="546"/>
+      <c r="F4" s="546"/>
+      <c r="G4" s="546"/>
       <c r="H4" s="547"/>
-      <c r="I4" s="545" t="s">
+      <c r="I4" s="546" t="s">
         <v>325</v>
       </c>
-      <c r="J4" s="545"/>
-      <c r="K4" s="545"/>
-      <c r="L4" s="545"/>
+      <c r="J4" s="546"/>
+      <c r="K4" s="546"/>
+      <c r="L4" s="546"/>
       <c r="M4" s="547"/>
-      <c r="N4" s="545" t="s">
+      <c r="N4" s="546" t="s">
         <v>326</v>
       </c>
-      <c r="O4" s="545"/>
-      <c r="P4" s="545"/>
-      <c r="Q4" s="545"/>
+      <c r="O4" s="546"/>
+      <c r="P4" s="546"/>
+      <c r="Q4" s="546"/>
       <c r="R4" s="547"/>
-      <c r="S4" s="545" t="s">
+      <c r="S4" s="546" t="s">
         <v>327</v>
       </c>
-      <c r="T4" s="545"/>
-      <c r="U4" s="545"/>
-      <c r="V4" s="545"/>
+      <c r="T4" s="546"/>
+      <c r="U4" s="546"/>
+      <c r="V4" s="546"/>
       <c r="W4" s="547"/>
-      <c r="X4" s="545" t="s">
+      <c r="X4" s="546" t="s">
         <v>328</v>
       </c>
-      <c r="Y4" s="545"/>
-      <c r="Z4" s="545"/>
-      <c r="AA4" s="545"/>
+      <c r="Y4" s="546"/>
+      <c r="Z4" s="546"/>
+      <c r="AA4" s="546"/>
       <c r="AB4" s="547"/>
-      <c r="AC4" s="545" t="s">
+      <c r="AC4" s="546" t="s">
         <v>329</v>
       </c>
-      <c r="AD4" s="545"/>
-      <c r="AE4" s="545"/>
-      <c r="AF4" s="545"/>
+      <c r="AD4" s="546"/>
+      <c r="AE4" s="546"/>
+      <c r="AF4" s="546"/>
       <c r="AG4" s="547"/>
-      <c r="AH4" s="545" t="s">
+      <c r="AH4" s="546" t="s">
         <v>330</v>
       </c>
-      <c r="AI4" s="545"/>
-      <c r="AJ4" s="545"/>
-      <c r="AK4" s="545"/>
+      <c r="AI4" s="546"/>
+      <c r="AJ4" s="546"/>
+      <c r="AK4" s="546"/>
       <c r="AL4" s="547"/>
-      <c r="AM4" s="545" t="s">
+      <c r="AM4" s="546" t="s">
         <v>331</v>
       </c>
-      <c r="AN4" s="545"/>
-      <c r="AO4" s="545"/>
-      <c r="AP4" s="545"/>
+      <c r="AN4" s="546"/>
+      <c r="AO4" s="546"/>
+      <c r="AP4" s="546"/>
       <c r="AQ4" s="547"/>
-      <c r="AR4" s="545" t="s">
+      <c r="AR4" s="546" t="s">
         <v>332</v>
       </c>
-      <c r="AS4" s="545"/>
-      <c r="AT4" s="545"/>
-      <c r="AU4" s="545"/>
+      <c r="AS4" s="546"/>
+      <c r="AT4" s="546"/>
+      <c r="AU4" s="546"/>
       <c r="AV4" s="547"/>
-      <c r="AW4" s="545" t="s">
+      <c r="AW4" s="546" t="s">
         <v>333</v>
       </c>
-      <c r="AX4" s="545"/>
-      <c r="AY4" s="545"/>
-      <c r="AZ4" s="545"/>
-      <c r="BA4" s="545"/>
-      <c r="BB4" s="546" t="s">
+      <c r="AX4" s="546"/>
+      <c r="AY4" s="546"/>
+      <c r="AZ4" s="546"/>
+      <c r="BA4" s="546"/>
+      <c r="BB4" s="545" t="s">
         <v>334</v>
       </c>
-      <c r="BC4" s="545"/>
-      <c r="BD4" s="545"/>
-      <c r="BE4" s="545"/>
+      <c r="BC4" s="546"/>
+      <c r="BD4" s="546"/>
+      <c r="BE4" s="546"/>
       <c r="BF4" s="547"/>
-      <c r="BG4" s="545" t="s">
+      <c r="BG4" s="546" t="s">
         <v>335</v>
       </c>
-      <c r="BH4" s="545"/>
-      <c r="BI4" s="545"/>
-      <c r="BJ4" s="545"/>
-      <c r="BK4" s="545"/>
-      <c r="BL4" s="546" t="s">
+      <c r="BH4" s="546"/>
+      <c r="BI4" s="546"/>
+      <c r="BJ4" s="546"/>
+      <c r="BK4" s="546"/>
+      <c r="BL4" s="545" t="s">
         <v>336</v>
       </c>
-      <c r="BM4" s="545"/>
-      <c r="BN4" s="545"/>
-      <c r="BO4" s="545"/>
-      <c r="BP4" s="545"/>
-      <c r="BQ4" s="546" t="s">
+      <c r="BM4" s="546"/>
+      <c r="BN4" s="546"/>
+      <c r="BO4" s="546"/>
+      <c r="BP4" s="546"/>
+      <c r="BQ4" s="545" t="s">
         <v>337</v>
       </c>
-      <c r="BR4" s="545"/>
-      <c r="BS4" s="545"/>
-      <c r="BT4" s="545"/>
+      <c r="BR4" s="546"/>
+      <c r="BS4" s="546"/>
+      <c r="BT4" s="546"/>
       <c r="BU4" s="547"/>
       <c r="BV4" s="280" t="s">
         <v>338</v>
@@ -50264,11 +50264,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -50281,6 +50276,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -50303,23 +50303,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="554" t="s">
+      <c r="A1" s="552" t="s">
         <v>611</v>
       </c>
-      <c r="B1" s="556" t="s">
+      <c r="B1" s="554" t="s">
         <v>612</v>
       </c>
-      <c r="C1" s="557"/>
-      <c r="D1" s="557"/>
-      <c r="E1" s="557"/>
-      <c r="F1" s="558"/>
-      <c r="G1" s="556" t="s">
+      <c r="C1" s="555"/>
+      <c r="D1" s="555"/>
+      <c r="E1" s="555"/>
+      <c r="F1" s="556"/>
+      <c r="G1" s="554" t="s">
         <v>613</v>
       </c>
-      <c r="H1" s="557"/>
-      <c r="I1" s="557"/>
-      <c r="J1" s="557"/>
-      <c r="K1" s="558"/>
+      <c r="H1" s="555"/>
+      <c r="I1" s="555"/>
+      <c r="J1" s="555"/>
+      <c r="K1" s="556"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -50329,7 +50329,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="555"/>
+      <c r="A2" s="553"/>
       <c r="B2" s="450" t="s">
         <v>270</v>
       </c>
@@ -51822,11 +51822,11 @@
       <c r="Y48" t="s">
         <v>662</v>
       </c>
-      <c r="Z48" s="552" t="s">
+      <c r="Z48" s="557" t="s">
         <v>600</v>
       </c>
-      <c r="AA48" s="553"/>
-      <c r="AB48" s="553"/>
+      <c r="AA48" s="558"/>
+      <c r="AB48" s="558"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -52043,11 +52043,11 @@
       <c r="Y53" t="s">
         <v>664</v>
       </c>
-      <c r="Z53" s="552" t="s">
+      <c r="Z53" s="557" t="s">
         <v>599</v>
       </c>
-      <c r="AA53" s="553"/>
-      <c r="AB53" s="553"/>
+      <c r="AA53" s="558"/>
+      <c r="AB53" s="558"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -52249,11 +52249,11 @@
       <c r="Y59" t="s">
         <v>665</v>
       </c>
-      <c r="Z59" s="552" t="s">
+      <c r="Z59" s="557" t="s">
         <v>666</v>
       </c>
-      <c r="AA59" s="553"/>
-      <c r="AB59" s="553"/>
+      <c r="AA59" s="558"/>
+      <c r="AB59" s="558"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="470" t="str">
@@ -53090,17 +53090,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Error - checking why demand drops off so much
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29197B3-356A-403B-A186-A5A53A30FCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9D08C6-2025-44E7-AD03-2391BC09B319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="-15150" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -8639,7 +8639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="797">
   <si>
     <t>Document type:</t>
   </si>
@@ -11033,6 +11033,24 @@
   </si>
   <si>
     <t>RSDSH_Apt-G,RSDSC_Apt</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-AB,RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-C,RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-D,RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-E,RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-F,RSDSC_Det</t>
+  </si>
+  <si>
+    <t>RSDSH_Det-G,RSDSC_Det</t>
   </si>
 </sst>
 </file>
@@ -13763,15 +13781,6 @@
     <xf numFmtId="0" fontId="37" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -13779,6 +13788,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13790,22 +13808,13 @@
     <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -13817,10 +13826,19 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13838,6 +13856,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -13852,12 +13876,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -14644,6 +14662,7 @@
       <sheetName val="ApartmentEnergyData"/>
       <sheetName val="AttachedEnergyData"/>
       <sheetName val="DettachedEnergyData"/>
+      <sheetName val="RES"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -14726,6 +14745,7 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
+      <sheetData sheetId="19" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -20779,8 +20799,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B141" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="G189" sqref="G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20970,12 +20990,12 @@
         <v>85</v>
       </c>
       <c r="U4" s="571"/>
-      <c r="V4" s="563" t="s">
+      <c r="V4" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="564"/>
-      <c r="X4" s="564"/>
-      <c r="Y4" s="565"/>
+      <c r="W4" s="573"/>
+      <c r="X4" s="573"/>
+      <c r="Y4" s="574"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21078,34 +21098,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="566" t="s">
+      <c r="H6" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="567"/>
-      <c r="J6" s="567"/>
-      <c r="K6" s="568"/>
-      <c r="L6" s="567" t="s">
+      <c r="I6" s="564"/>
+      <c r="J6" s="564"/>
+      <c r="K6" s="565"/>
+      <c r="L6" s="564" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="567"/>
-      <c r="N6" s="567"/>
-      <c r="O6" s="568"/>
-      <c r="P6" s="566" t="s">
+      <c r="M6" s="564"/>
+      <c r="N6" s="564"/>
+      <c r="O6" s="565"/>
+      <c r="P6" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="567"/>
-      <c r="R6" s="567"/>
-      <c r="S6" s="568"/>
-      <c r="T6" s="566" t="s">
+      <c r="Q6" s="564"/>
+      <c r="R6" s="564"/>
+      <c r="S6" s="565"/>
+      <c r="T6" s="563" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="568"/>
-      <c r="V6" s="566" t="s">
+      <c r="U6" s="565"/>
+      <c r="V6" s="563" t="s">
         <v>503</v>
       </c>
-      <c r="W6" s="567"/>
-      <c r="X6" s="567"/>
-      <c r="Y6" s="568"/>
+      <c r="W6" s="564"/>
+      <c r="X6" s="564"/>
+      <c r="Y6" s="565"/>
       <c r="Z6" s="521" t="s">
         <v>515</v>
       </c>
@@ -26318,12 +26338,12 @@
         <v>85</v>
       </c>
       <c r="U62" s="571"/>
-      <c r="V62" s="563" t="s">
+      <c r="V62" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="W62" s="564"/>
-      <c r="X62" s="564"/>
-      <c r="Y62" s="565"/>
+      <c r="W62" s="573"/>
+      <c r="X62" s="573"/>
+      <c r="Y62" s="574"/>
       <c r="Z62" s="60"/>
       <c r="AA62" s="60"/>
       <c r="AB62" s="68" t="s">
@@ -26426,34 +26446,34 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="39"/>
-      <c r="H64" s="566" t="s">
+      <c r="H64" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="I64" s="567"/>
-      <c r="J64" s="567"/>
-      <c r="K64" s="568"/>
-      <c r="L64" s="567" t="s">
+      <c r="I64" s="564"/>
+      <c r="J64" s="564"/>
+      <c r="K64" s="565"/>
+      <c r="L64" s="564" t="s">
         <v>34</v>
       </c>
-      <c r="M64" s="567"/>
-      <c r="N64" s="567"/>
-      <c r="O64" s="568"/>
-      <c r="P64" s="566" t="s">
+      <c r="M64" s="564"/>
+      <c r="N64" s="564"/>
+      <c r="O64" s="565"/>
+      <c r="P64" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="Q64" s="567"/>
-      <c r="R64" s="567"/>
-      <c r="S64" s="568"/>
-      <c r="T64" s="572" t="s">
+      <c r="Q64" s="564"/>
+      <c r="R64" s="564"/>
+      <c r="S64" s="565"/>
+      <c r="T64" s="566" t="s">
         <v>68</v>
       </c>
-      <c r="U64" s="573"/>
-      <c r="V64" s="572" t="s">
+      <c r="U64" s="567"/>
+      <c r="V64" s="566" t="s">
         <v>503</v>
       </c>
-      <c r="W64" s="574"/>
-      <c r="X64" s="574"/>
-      <c r="Y64" s="573"/>
+      <c r="W64" s="568"/>
+      <c r="X64" s="568"/>
+      <c r="Y64" s="567"/>
       <c r="Z64" s="367" t="s">
         <v>515</v>
       </c>
@@ -33090,12 +33110,12 @@
         <v>85</v>
       </c>
       <c r="U135" s="571"/>
-      <c r="V135" s="563" t="s">
+      <c r="V135" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="W135" s="564"/>
-      <c r="X135" s="564"/>
-      <c r="Y135" s="565"/>
+      <c r="W135" s="573"/>
+      <c r="X135" s="573"/>
+      <c r="Y135" s="574"/>
       <c r="Z135" s="60"/>
       <c r="AA135" s="60"/>
       <c r="AB135" s="68" t="s">
@@ -33210,34 +33230,34 @@
       <c r="E137" s="38"/>
       <c r="F137" s="38"/>
       <c r="G137" s="39"/>
-      <c r="H137" s="566" t="s">
+      <c r="H137" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="I137" s="567"/>
-      <c r="J137" s="567"/>
-      <c r="K137" s="568"/>
-      <c r="L137" s="567" t="s">
+      <c r="I137" s="564"/>
+      <c r="J137" s="564"/>
+      <c r="K137" s="565"/>
+      <c r="L137" s="564" t="s">
         <v>34</v>
       </c>
-      <c r="M137" s="567"/>
-      <c r="N137" s="567"/>
-      <c r="O137" s="568"/>
-      <c r="P137" s="566" t="s">
+      <c r="M137" s="564"/>
+      <c r="N137" s="564"/>
+      <c r="O137" s="565"/>
+      <c r="P137" s="563" t="s">
         <v>34</v>
       </c>
-      <c r="Q137" s="567"/>
-      <c r="R137" s="567"/>
-      <c r="S137" s="568"/>
-      <c r="T137" s="572" t="s">
+      <c r="Q137" s="564"/>
+      <c r="R137" s="564"/>
+      <c r="S137" s="565"/>
+      <c r="T137" s="566" t="s">
         <v>68</v>
       </c>
-      <c r="U137" s="573"/>
-      <c r="V137" s="572" t="s">
+      <c r="U137" s="567"/>
+      <c r="V137" s="566" t="s">
         <v>503</v>
       </c>
-      <c r="W137" s="574"/>
-      <c r="X137" s="574"/>
-      <c r="Y137" s="573"/>
+      <c r="W137" s="568"/>
+      <c r="X137" s="568"/>
+      <c r="Y137" s="567"/>
       <c r="Z137" s="367" t="s">
         <v>515</v>
       </c>
@@ -37861,7 +37881,7 @@
         <v>558</v>
       </c>
       <c r="G183" s="88" t="s">
-        <v>728</v>
+        <v>791</v>
       </c>
       <c r="H183" s="19">
         <v>1.0999999999999999</v>
@@ -37967,7 +37987,7 @@
         <v>558</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>762</v>
+        <v>792</v>
       </c>
       <c r="H184" s="22">
         <v>1.0999999999999999</v>
@@ -38070,7 +38090,7 @@
         <v>558</v>
       </c>
       <c r="G185" s="30" t="s">
-        <v>763</v>
+        <v>793</v>
       </c>
       <c r="H185" s="40">
         <v>1.0999999999999999</v>
@@ -38173,7 +38193,7 @@
         <v>558</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>764</v>
+        <v>794</v>
       </c>
       <c r="H186" s="22">
         <v>1.0999999999999999</v>
@@ -38276,7 +38296,7 @@
         <v>558</v>
       </c>
       <c r="G187" s="30" t="s">
-        <v>766</v>
+        <v>795</v>
       </c>
       <c r="H187" s="40">
         <v>1.0999999999999999</v>
@@ -38379,7 +38399,7 @@
         <v>558</v>
       </c>
       <c r="G188" s="27" t="s">
-        <v>765</v>
+        <v>796</v>
       </c>
       <c r="H188" s="246">
         <v>1.0999999999999999</v>
@@ -39750,26 +39770,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L137:O137"/>
-    <mergeCell ref="P137:S137"/>
-    <mergeCell ref="T137:U137"/>
-    <mergeCell ref="V137:Y137"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="L135:O135"/>
-    <mergeCell ref="P135:S135"/>
-    <mergeCell ref="T135:U135"/>
-    <mergeCell ref="V135:Y135"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="L64:O64"/>
-    <mergeCell ref="P64:S64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="L62:O62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="T62:U62"/>
-    <mergeCell ref="V62:Y62"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -39780,6 +39780,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="L62:O62"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="T62:U62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="L64:O64"/>
+    <mergeCell ref="P64:S64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="L135:O135"/>
+    <mergeCell ref="P135:S135"/>
+    <mergeCell ref="T135:U135"/>
+    <mergeCell ref="V135:Y135"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L137:O137"/>
+    <mergeCell ref="P137:S137"/>
+    <mergeCell ref="T137:U137"/>
+    <mergeCell ref="V137:Y137"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -39925,12 +39945,12 @@
       <c r="I5" s="121"/>
       <c r="J5" s="121"/>
       <c r="K5" s="121"/>
-      <c r="L5" s="563" t="s">
+      <c r="L5" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="564"/>
-      <c r="N5" s="564"/>
-      <c r="O5" s="565"/>
+      <c r="M5" s="573"/>
+      <c r="N5" s="573"/>
+      <c r="O5" s="574"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -39961,12 +39981,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="572" t="s">
+      <c r="L6" s="566" t="s">
         <v>503</v>
       </c>
-      <c r="M6" s="574"/>
-      <c r="N6" s="574"/>
-      <c r="O6" s="573"/>
+      <c r="M6" s="568"/>
+      <c r="N6" s="568"/>
+      <c r="O6" s="567"/>
       <c r="P6" s="367" t="s">
         <v>515</v>
       </c>
@@ -40852,23 +40872,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="563" t="s">
+      <c r="L33" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="564"/>
-      <c r="N33" s="564"/>
-      <c r="O33" s="565"/>
+      <c r="M33" s="573"/>
+      <c r="N33" s="573"/>
+      <c r="O33" s="574"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L34" s="572" t="s">
+      <c r="L34" s="566" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="574"/>
-      <c r="N34" s="574"/>
-      <c r="O34" s="573"/>
+      <c r="M34" s="568"/>
+      <c r="N34" s="568"/>
+      <c r="O34" s="567"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -41215,11 +41235,11 @@
       </c>
       <c r="I4" s="570"/>
       <c r="J4" s="571"/>
-      <c r="K4" s="563" t="s">
+      <c r="K4" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="564"/>
-      <c r="M4" s="565"/>
+      <c r="L4" s="573"/>
+      <c r="M4" s="574"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -41245,16 +41265,16 @@
       <c r="G5" s="375" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="575" t="s">
+      <c r="H5" s="578" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="576"/>
-      <c r="J5" s="577"/>
-      <c r="K5" s="575" t="s">
+      <c r="I5" s="579"/>
+      <c r="J5" s="580"/>
+      <c r="K5" s="578" t="s">
         <v>292</v>
       </c>
-      <c r="L5" s="576"/>
-      <c r="M5" s="577"/>
+      <c r="L5" s="579"/>
+      <c r="M5" s="580"/>
       <c r="N5" s="376" t="s">
         <v>92</v>
       </c>
@@ -41271,23 +41291,23 @@
         <v>210</v>
       </c>
       <c r="AA5" s="201"/>
-      <c r="AB5" s="578" t="s">
+      <c r="AB5" s="575" t="s">
         <v>541</v>
       </c>
-      <c r="AC5" s="578"/>
+      <c r="AC5" s="575"/>
       <c r="AD5" s="378"/>
-      <c r="AE5" s="579" t="s">
+      <c r="AE5" s="576" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="579"/>
-      <c r="AG5" s="579" t="s">
+      <c r="AF5" s="576"/>
+      <c r="AG5" s="576" t="s">
         <v>542</v>
       </c>
-      <c r="AH5" s="579"/>
-      <c r="AI5" s="580" t="s">
+      <c r="AH5" s="576"/>
+      <c r="AI5" s="577" t="s">
         <v>543</v>
       </c>
-      <c r="AJ5" s="580"/>
+      <c r="AJ5" s="577"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="422" t="str">
@@ -42025,12 +42045,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="563" t="s">
+      <c r="L27" s="572" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="564"/>
-      <c r="N27" s="564"/>
-      <c r="O27" s="565"/>
+      <c r="M27" s="573"/>
+      <c r="N27" s="573"/>
+      <c r="O27" s="574"/>
       <c r="T27" s="203"/>
       <c r="U27" s="203"/>
     </row>
@@ -42038,12 +42058,12 @@
       <c r="J28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L28" s="566" t="s">
+      <c r="L28" s="563" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="567"/>
-      <c r="N28" s="567"/>
-      <c r="O28" s="568"/>
+      <c r="M28" s="564"/>
+      <c r="N28" s="564"/>
+      <c r="O28" s="565"/>
       <c r="T28" s="203"/>
       <c r="U28" s="203"/>
     </row>
@@ -43433,16 +43453,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -43873,103 +43893,103 @@
       <c r="C4" s="273" t="s">
         <v>301</v>
       </c>
-      <c r="D4" s="581" t="s">
+      <c r="D4" s="582" t="s">
         <v>302</v>
       </c>
-      <c r="E4" s="582"/>
-      <c r="F4" s="582"/>
-      <c r="G4" s="582"/>
+      <c r="E4" s="581"/>
+      <c r="F4" s="581"/>
+      <c r="G4" s="581"/>
       <c r="H4" s="583"/>
-      <c r="I4" s="582" t="s">
+      <c r="I4" s="581" t="s">
         <v>303</v>
       </c>
-      <c r="J4" s="582"/>
-      <c r="K4" s="582"/>
-      <c r="L4" s="582"/>
+      <c r="J4" s="581"/>
+      <c r="K4" s="581"/>
+      <c r="L4" s="581"/>
       <c r="M4" s="583"/>
-      <c r="N4" s="582" t="s">
+      <c r="N4" s="581" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="582"/>
-      <c r="P4" s="582"/>
-      <c r="Q4" s="582"/>
+      <c r="O4" s="581"/>
+      <c r="P4" s="581"/>
+      <c r="Q4" s="581"/>
       <c r="R4" s="583"/>
-      <c r="S4" s="582" t="s">
+      <c r="S4" s="581" t="s">
         <v>305</v>
       </c>
-      <c r="T4" s="582"/>
-      <c r="U4" s="582"/>
-      <c r="V4" s="582"/>
+      <c r="T4" s="581"/>
+      <c r="U4" s="581"/>
+      <c r="V4" s="581"/>
       <c r="W4" s="583"/>
-      <c r="X4" s="582" t="s">
+      <c r="X4" s="581" t="s">
         <v>306</v>
       </c>
-      <c r="Y4" s="582"/>
-      <c r="Z4" s="582"/>
-      <c r="AA4" s="582"/>
+      <c r="Y4" s="581"/>
+      <c r="Z4" s="581"/>
+      <c r="AA4" s="581"/>
       <c r="AB4" s="583"/>
-      <c r="AC4" s="582" t="s">
+      <c r="AC4" s="581" t="s">
         <v>307</v>
       </c>
-      <c r="AD4" s="582"/>
-      <c r="AE4" s="582"/>
-      <c r="AF4" s="582"/>
+      <c r="AD4" s="581"/>
+      <c r="AE4" s="581"/>
+      <c r="AF4" s="581"/>
       <c r="AG4" s="583"/>
-      <c r="AH4" s="582" t="s">
+      <c r="AH4" s="581" t="s">
         <v>308</v>
       </c>
-      <c r="AI4" s="582"/>
-      <c r="AJ4" s="582"/>
-      <c r="AK4" s="582"/>
+      <c r="AI4" s="581"/>
+      <c r="AJ4" s="581"/>
+      <c r="AK4" s="581"/>
       <c r="AL4" s="583"/>
-      <c r="AM4" s="582" t="s">
+      <c r="AM4" s="581" t="s">
         <v>309</v>
       </c>
-      <c r="AN4" s="582"/>
-      <c r="AO4" s="582"/>
-      <c r="AP4" s="582"/>
+      <c r="AN4" s="581"/>
+      <c r="AO4" s="581"/>
+      <c r="AP4" s="581"/>
       <c r="AQ4" s="583"/>
-      <c r="AR4" s="582" t="s">
+      <c r="AR4" s="581" t="s">
         <v>310</v>
       </c>
-      <c r="AS4" s="582"/>
-      <c r="AT4" s="582"/>
-      <c r="AU4" s="582"/>
+      <c r="AS4" s="581"/>
+      <c r="AT4" s="581"/>
+      <c r="AU4" s="581"/>
       <c r="AV4" s="583"/>
-      <c r="AW4" s="582" t="s">
+      <c r="AW4" s="581" t="s">
         <v>311</v>
       </c>
-      <c r="AX4" s="582"/>
-      <c r="AY4" s="582"/>
-      <c r="AZ4" s="582"/>
-      <c r="BA4" s="582"/>
-      <c r="BB4" s="581" t="s">
+      <c r="AX4" s="581"/>
+      <c r="AY4" s="581"/>
+      <c r="AZ4" s="581"/>
+      <c r="BA4" s="581"/>
+      <c r="BB4" s="582" t="s">
         <v>312</v>
       </c>
-      <c r="BC4" s="582"/>
-      <c r="BD4" s="582"/>
-      <c r="BE4" s="582"/>
+      <c r="BC4" s="581"/>
+      <c r="BD4" s="581"/>
+      <c r="BE4" s="581"/>
       <c r="BF4" s="583"/>
-      <c r="BG4" s="582" t="s">
+      <c r="BG4" s="581" t="s">
         <v>313</v>
       </c>
-      <c r="BH4" s="582"/>
-      <c r="BI4" s="582"/>
-      <c r="BJ4" s="582"/>
-      <c r="BK4" s="582"/>
-      <c r="BL4" s="581" t="s">
+      <c r="BH4" s="581"/>
+      <c r="BI4" s="581"/>
+      <c r="BJ4" s="581"/>
+      <c r="BK4" s="581"/>
+      <c r="BL4" s="582" t="s">
         <v>314</v>
       </c>
-      <c r="BM4" s="582"/>
-      <c r="BN4" s="582"/>
-      <c r="BO4" s="582"/>
-      <c r="BP4" s="582"/>
-      <c r="BQ4" s="581" t="s">
+      <c r="BM4" s="581"/>
+      <c r="BN4" s="581"/>
+      <c r="BO4" s="581"/>
+      <c r="BP4" s="581"/>
+      <c r="BQ4" s="582" t="s">
         <v>315</v>
       </c>
-      <c r="BR4" s="582"/>
-      <c r="BS4" s="582"/>
-      <c r="BT4" s="582"/>
+      <c r="BR4" s="581"/>
+      <c r="BS4" s="581"/>
+      <c r="BT4" s="581"/>
       <c r="BU4" s="583"/>
       <c r="BV4" s="274" t="s">
         <v>316</v>
@@ -57563,6 +57583,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -57575,11 +57600,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -57602,23 +57622,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="588" t="s">
+      <c r="A1" s="590" t="s">
         <v>585</v>
       </c>
-      <c r="B1" s="590" t="s">
+      <c r="B1" s="592" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="591"/>
-      <c r="D1" s="591"/>
-      <c r="E1" s="591"/>
-      <c r="F1" s="592"/>
-      <c r="G1" s="590" t="s">
+      <c r="C1" s="593"/>
+      <c r="D1" s="593"/>
+      <c r="E1" s="593"/>
+      <c r="F1" s="594"/>
+      <c r="G1" s="592" t="s">
         <v>587</v>
       </c>
-      <c r="H1" s="591"/>
-      <c r="I1" s="591"/>
-      <c r="J1" s="591"/>
-      <c r="K1" s="592"/>
+      <c r="H1" s="593"/>
+      <c r="I1" s="593"/>
+      <c r="J1" s="593"/>
+      <c r="K1" s="594"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -57628,7 +57648,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="589"/>
+      <c r="A2" s="591"/>
       <c r="B2" s="443" t="s">
         <v>254</v>
       </c>
@@ -59121,11 +59141,11 @@
       <c r="Y48" t="s">
         <v>636</v>
       </c>
-      <c r="Z48" s="593" t="s">
+      <c r="Z48" s="588" t="s">
         <v>574</v>
       </c>
-      <c r="AA48" s="594"/>
-      <c r="AB48" s="594"/>
+      <c r="AA48" s="589"/>
+      <c r="AB48" s="589"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -59342,11 +59362,11 @@
       <c r="Y53" t="s">
         <v>638</v>
       </c>
-      <c r="Z53" s="593" t="s">
+      <c r="Z53" s="588" t="s">
         <v>573</v>
       </c>
-      <c r="AA53" s="594"/>
-      <c r="AB53" s="594"/>
+      <c r="AA53" s="589"/>
+      <c r="AB53" s="589"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -59548,11 +59568,11 @@
       <c r="Y59" t="s">
         <v>639</v>
       </c>
-      <c r="Z59" s="593" t="s">
+      <c r="Z59" s="588" t="s">
         <v>640</v>
       </c>
-      <c r="AA59" s="594"/>
-      <c r="AB59" s="594"/>
+      <c r="AA59" s="589"/>
+      <c r="AB59" s="589"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="463" t="str">
@@ -60389,17 +60409,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying to fix the missing Ambient from Translate table
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4FB151-7C10-42E5-BBBE-C7821010D5F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC2ECFB-CB59-4B1A-AF6A-C2E80D7F9F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2850" yWindow="555" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2CC7CA6E-3559-4BC7-B5C1-253B80EF5435}"/>
   </bookViews>
   <sheets>
@@ -13899,6 +13898,19 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="34" borderId="87" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="15" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="15" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="85" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="15" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -13944,6 +13956,42 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -13962,40 +14010,13 @@
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -14007,19 +14028,10 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14037,12 +14049,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14058,19 +14064,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="34" borderId="87" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="37" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="37" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="15" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="15" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="39" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="34" borderId="87" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="34" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="34" borderId="85" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="15" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -15270,10 +15269,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15710,12 +15706,12 @@
       <c r="Z15" s="493"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="578" t="s">
+      <c r="A16" s="591" t="s">
         <v>676</v>
       </c>
-      <c r="B16" s="578"/>
-      <c r="C16" s="578"/>
-      <c r="D16" s="578"/>
+      <c r="B16" s="591"/>
+      <c r="C16" s="591"/>
+      <c r="D16" s="591"/>
       <c r="E16" s="495"/>
       <c r="F16" s="495"/>
       <c r="G16" s="496"/>
@@ -15799,11 +15795,11 @@
       <c r="A19" s="500" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="577" t="s">
+      <c r="B19" s="590" t="s">
         <v>692</v>
       </c>
-      <c r="C19" s="577"/>
-      <c r="D19" s="577"/>
+      <c r="C19" s="590"/>
+      <c r="D19" s="590"/>
       <c r="E19" s="501"/>
       <c r="F19" s="501"/>
       <c r="G19" s="502"/>
@@ -15831,11 +15827,11 @@
       <c r="A20" s="500" t="s">
         <v>677</v>
       </c>
-      <c r="B20" s="577" t="s">
+      <c r="B20" s="590" t="s">
         <v>687</v>
       </c>
-      <c r="C20" s="577"/>
-      <c r="D20" s="577"/>
+      <c r="C20" s="590"/>
+      <c r="D20" s="590"/>
       <c r="E20" s="501"/>
       <c r="F20" s="501"/>
       <c r="G20" s="502"/>
@@ -15923,11 +15919,11 @@
       <c r="A23" s="500" t="s">
         <v>679</v>
       </c>
-      <c r="B23" s="577" t="s">
+      <c r="B23" s="590" t="s">
         <v>689</v>
       </c>
-      <c r="C23" s="577"/>
-      <c r="D23" s="577"/>
+      <c r="C23" s="590"/>
+      <c r="D23" s="590"/>
       <c r="E23" s="493"/>
       <c r="F23" s="493"/>
       <c r="G23" s="493"/>
@@ -15953,11 +15949,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="500"/>
-      <c r="B24" s="577" t="s">
+      <c r="B24" s="590" t="s">
         <v>690</v>
       </c>
-      <c r="C24" s="577"/>
-      <c r="D24" s="577"/>
+      <c r="C24" s="590"/>
+      <c r="D24" s="590"/>
       <c r="E24" s="493"/>
       <c r="F24" s="493"/>
       <c r="G24" s="493"/>
@@ -15983,11 +15979,11 @@
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="500"/>
-      <c r="B25" s="577" t="s">
+      <c r="B25" s="590" t="s">
         <v>691</v>
       </c>
-      <c r="C25" s="577"/>
-      <c r="D25" s="577"/>
+      <c r="C25" s="590"/>
+      <c r="D25" s="590"/>
       <c r="E25" s="493"/>
       <c r="F25" s="493"/>
       <c r="G25" s="493"/>
@@ -16015,11 +16011,11 @@
       <c r="A26" s="500" t="s">
         <v>680</v>
       </c>
-      <c r="B26" s="577" t="s">
+      <c r="B26" s="590" t="s">
         <v>689</v>
       </c>
-      <c r="C26" s="577"/>
-      <c r="D26" s="577"/>
+      <c r="C26" s="590"/>
+      <c r="D26" s="590"/>
       <c r="E26" s="493"/>
       <c r="F26" s="493"/>
       <c r="G26" s="493"/>
@@ -16045,11 +16041,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="500"/>
-      <c r="B27" s="577" t="s">
+      <c r="B27" s="590" t="s">
         <v>691</v>
       </c>
-      <c r="C27" s="577"/>
-      <c r="D27" s="577"/>
+      <c r="C27" s="590"/>
+      <c r="D27" s="590"/>
       <c r="E27" s="493"/>
       <c r="F27" s="493"/>
       <c r="G27" s="493"/>
@@ -16137,11 +16133,11 @@
       <c r="A30" s="500" t="s">
         <v>682</v>
       </c>
-      <c r="B30" s="579" t="s">
+      <c r="B30" s="592" t="s">
         <v>683</v>
       </c>
-      <c r="C30" s="577"/>
-      <c r="D30" s="577"/>
+      <c r="C30" s="590"/>
+      <c r="D30" s="590"/>
       <c r="E30" s="505"/>
       <c r="F30" s="505"/>
       <c r="G30" s="493"/>
@@ -16169,11 +16165,11 @@
       <c r="A31" s="500" t="s">
         <v>684</v>
       </c>
-      <c r="B31" s="577" t="s">
+      <c r="B31" s="590" t="s">
         <v>685</v>
       </c>
-      <c r="C31" s="577"/>
-      <c r="D31" s="577"/>
+      <c r="C31" s="590"/>
+      <c r="D31" s="590"/>
       <c r="E31" s="505"/>
       <c r="F31" s="505"/>
       <c r="G31" s="493"/>
@@ -18133,10 +18129,7 @@
   </sheetPr>
   <dimension ref="B1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18153,16 +18146,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="580" t="s">
+      <c r="B2" s="593" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="581"/>
-      <c r="D2" s="581"/>
-      <c r="E2" s="582"/>
-      <c r="G2" s="580" t="s">
+      <c r="C2" s="594"/>
+      <c r="D2" s="594"/>
+      <c r="E2" s="595"/>
+      <c r="G2" s="593" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="582"/>
+      <c r="H2" s="595"/>
       <c r="I2" s="147"/>
       <c r="J2" s="147"/>
       <c r="K2" s="148"/>
@@ -18445,10 +18438,10 @@
       <c r="E14" s="163" t="s">
         <v>180</v>
       </c>
-      <c r="G14" s="580" t="s">
+      <c r="G14" s="593" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="582"/>
+      <c r="H14" s="595"/>
     </row>
     <row r="15" spans="2:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="160" t="s">
@@ -18532,12 +18525,12 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="583" t="s">
+      <c r="B20" s="596" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="584"/>
-      <c r="D20" s="584"/>
-      <c r="E20" s="585"/>
+      <c r="C20" s="597"/>
+      <c r="D20" s="597"/>
+      <c r="E20" s="598"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="175" t="s">
@@ -18720,16 +18713,16 @@
     </row>
     <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="580" t="s">
+      <c r="B36" s="593" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="581"/>
-      <c r="D36" s="581"/>
-      <c r="E36" s="582"/>
-      <c r="G36" s="586" t="s">
+      <c r="C36" s="594"/>
+      <c r="D36" s="594"/>
+      <c r="E36" s="595"/>
+      <c r="G36" s="599" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="587"/>
+      <c r="H36" s="600"/>
     </row>
     <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="191" t="s">
@@ -18828,10 +18821,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AM103"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18890,13 +18880,13 @@
       <c r="J3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="588" t="s">
+      <c r="S3" s="601" t="s">
         <v>248</v>
       </c>
-      <c r="T3" s="588"/>
-      <c r="U3" s="588"/>
-      <c r="V3" s="588"/>
-      <c r="W3" s="588"/>
+      <c r="T3" s="601"/>
+      <c r="U3" s="601"/>
+      <c r="V3" s="601"/>
+      <c r="W3" s="601"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
@@ -20997,10 +20987,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS251"/>
   <sheetViews>
-    <sheetView topLeftCell="I203" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AM242" sqref="AM242"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AB41" sqref="AB41"/>
     </sheetView>
   </sheetViews>
@@ -21176,34 +21163,34 @@
       <c r="G4" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="604" t="s">
+      <c r="H4" s="611" t="s">
         <v>258</v>
       </c>
-      <c r="I4" s="605"/>
-      <c r="J4" s="605"/>
-      <c r="K4" s="606"/>
-      <c r="L4" s="604" t="s">
+      <c r="I4" s="612"/>
+      <c r="J4" s="612"/>
+      <c r="K4" s="613"/>
+      <c r="L4" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="605"/>
-      <c r="N4" s="605"/>
-      <c r="O4" s="606"/>
-      <c r="P4" s="604" t="s">
+      <c r="M4" s="612"/>
+      <c r="N4" s="612"/>
+      <c r="O4" s="613"/>
+      <c r="P4" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="605"/>
-      <c r="R4" s="605"/>
-      <c r="S4" s="606"/>
-      <c r="T4" s="604" t="s">
+      <c r="Q4" s="612"/>
+      <c r="R4" s="612"/>
+      <c r="S4" s="613"/>
+      <c r="T4" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U4" s="606"/>
-      <c r="V4" s="607" t="s">
+      <c r="U4" s="613"/>
+      <c r="V4" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="608"/>
-      <c r="X4" s="608"/>
-      <c r="Y4" s="609"/>
+      <c r="W4" s="606"/>
+      <c r="X4" s="606"/>
+      <c r="Y4" s="607"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21306,34 +21293,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="598" t="s">
+      <c r="H6" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="599"/>
-      <c r="J6" s="599"/>
-      <c r="K6" s="600"/>
-      <c r="L6" s="599" t="s">
+      <c r="I6" s="609"/>
+      <c r="J6" s="609"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="599"/>
-      <c r="N6" s="599"/>
-      <c r="O6" s="600"/>
-      <c r="P6" s="598" t="s">
+      <c r="M6" s="609"/>
+      <c r="N6" s="609"/>
+      <c r="O6" s="610"/>
+      <c r="P6" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="599"/>
-      <c r="R6" s="599"/>
-      <c r="S6" s="600"/>
-      <c r="T6" s="598" t="s">
+      <c r="Q6" s="609"/>
+      <c r="R6" s="609"/>
+      <c r="S6" s="610"/>
+      <c r="T6" s="608" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="600"/>
-      <c r="V6" s="598" t="s">
+      <c r="U6" s="610"/>
+      <c r="V6" s="608" t="s">
         <v>503</v>
       </c>
-      <c r="W6" s="599"/>
-      <c r="X6" s="599"/>
-      <c r="Y6" s="600"/>
+      <c r="W6" s="609"/>
+      <c r="X6" s="609"/>
+      <c r="Y6" s="610"/>
       <c r="Z6" s="520" t="s">
         <v>515</v>
       </c>
@@ -22685,7 +22672,7 @@
         <f>JRC_Data!$BL$18/1000</f>
         <v>0.15</v>
       </c>
-      <c r="AA20" s="642"/>
+      <c r="AA20" s="589"/>
       <c r="AB20" s="254"/>
       <c r="AC20" s="254"/>
       <c r="AD20" s="254"/>
@@ -26528,34 +26515,34 @@
       <c r="G62" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H62" s="604" t="s">
+      <c r="H62" s="611" t="s">
         <v>82</v>
       </c>
-      <c r="I62" s="605"/>
-      <c r="J62" s="605"/>
-      <c r="K62" s="606"/>
-      <c r="L62" s="604" t="s">
+      <c r="I62" s="612"/>
+      <c r="J62" s="612"/>
+      <c r="K62" s="613"/>
+      <c r="L62" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M62" s="605"/>
-      <c r="N62" s="605"/>
-      <c r="O62" s="606"/>
-      <c r="P62" s="604" t="s">
+      <c r="M62" s="612"/>
+      <c r="N62" s="612"/>
+      <c r="O62" s="613"/>
+      <c r="P62" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q62" s="605"/>
-      <c r="R62" s="605"/>
-      <c r="S62" s="606"/>
-      <c r="T62" s="604" t="s">
+      <c r="Q62" s="612"/>
+      <c r="R62" s="612"/>
+      <c r="S62" s="613"/>
+      <c r="T62" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U62" s="606"/>
-      <c r="V62" s="607" t="s">
+      <c r="U62" s="613"/>
+      <c r="V62" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W62" s="608"/>
-      <c r="X62" s="608"/>
-      <c r="Y62" s="609"/>
+      <c r="W62" s="606"/>
+      <c r="X62" s="606"/>
+      <c r="Y62" s="607"/>
       <c r="Z62" s="60"/>
       <c r="AA62" s="60"/>
       <c r="AB62" s="68" t="s">
@@ -26658,34 +26645,34 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="39"/>
-      <c r="H64" s="598" t="s">
+      <c r="H64" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I64" s="599"/>
-      <c r="J64" s="599"/>
-      <c r="K64" s="600"/>
-      <c r="L64" s="599" t="s">
+      <c r="I64" s="609"/>
+      <c r="J64" s="609"/>
+      <c r="K64" s="610"/>
+      <c r="L64" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M64" s="599"/>
-      <c r="N64" s="599"/>
-      <c r="O64" s="600"/>
-      <c r="P64" s="598" t="s">
+      <c r="M64" s="609"/>
+      <c r="N64" s="609"/>
+      <c r="O64" s="610"/>
+      <c r="P64" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q64" s="599"/>
-      <c r="R64" s="599"/>
-      <c r="S64" s="600"/>
-      <c r="T64" s="601" t="s">
+      <c r="Q64" s="609"/>
+      <c r="R64" s="609"/>
+      <c r="S64" s="610"/>
+      <c r="T64" s="614" t="s">
         <v>68</v>
       </c>
-      <c r="U64" s="602"/>
-      <c r="V64" s="601" t="s">
+      <c r="U64" s="615"/>
+      <c r="V64" s="614" t="s">
         <v>503</v>
       </c>
-      <c r="W64" s="603"/>
-      <c r="X64" s="603"/>
-      <c r="Y64" s="602"/>
+      <c r="W64" s="616"/>
+      <c r="X64" s="616"/>
+      <c r="Y64" s="615"/>
       <c r="Z64" s="367" t="s">
         <v>515</v>
       </c>
@@ -33300,34 +33287,34 @@
       <c r="G135" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H135" s="604" t="s">
+      <c r="H135" s="611" t="s">
         <v>82</v>
       </c>
-      <c r="I135" s="605"/>
-      <c r="J135" s="605"/>
-      <c r="K135" s="606"/>
-      <c r="L135" s="604" t="s">
+      <c r="I135" s="612"/>
+      <c r="J135" s="612"/>
+      <c r="K135" s="613"/>
+      <c r="L135" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M135" s="605"/>
-      <c r="N135" s="605"/>
-      <c r="O135" s="606"/>
-      <c r="P135" s="604" t="s">
+      <c r="M135" s="612"/>
+      <c r="N135" s="612"/>
+      <c r="O135" s="613"/>
+      <c r="P135" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q135" s="605"/>
-      <c r="R135" s="605"/>
-      <c r="S135" s="606"/>
-      <c r="T135" s="604" t="s">
+      <c r="Q135" s="612"/>
+      <c r="R135" s="612"/>
+      <c r="S135" s="613"/>
+      <c r="T135" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U135" s="606"/>
-      <c r="V135" s="607" t="s">
+      <c r="U135" s="613"/>
+      <c r="V135" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W135" s="608"/>
-      <c r="X135" s="608"/>
-      <c r="Y135" s="609"/>
+      <c r="W135" s="606"/>
+      <c r="X135" s="606"/>
+      <c r="Y135" s="607"/>
       <c r="Z135" s="60"/>
       <c r="AA135" s="60"/>
       <c r="AB135" s="68" t="s">
@@ -33442,34 +33429,34 @@
       <c r="E137" s="38"/>
       <c r="F137" s="38"/>
       <c r="G137" s="39"/>
-      <c r="H137" s="598" t="s">
+      <c r="H137" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I137" s="599"/>
-      <c r="J137" s="599"/>
-      <c r="K137" s="600"/>
-      <c r="L137" s="599" t="s">
+      <c r="I137" s="609"/>
+      <c r="J137" s="609"/>
+      <c r="K137" s="610"/>
+      <c r="L137" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M137" s="599"/>
-      <c r="N137" s="599"/>
-      <c r="O137" s="600"/>
-      <c r="P137" s="598" t="s">
+      <c r="M137" s="609"/>
+      <c r="N137" s="609"/>
+      <c r="O137" s="610"/>
+      <c r="P137" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q137" s="599"/>
-      <c r="R137" s="599"/>
-      <c r="S137" s="600"/>
-      <c r="T137" s="601" t="s">
+      <c r="Q137" s="609"/>
+      <c r="R137" s="609"/>
+      <c r="S137" s="610"/>
+      <c r="T137" s="614" t="s">
         <v>68</v>
       </c>
-      <c r="U137" s="602"/>
-      <c r="V137" s="601" t="s">
+      <c r="U137" s="615"/>
+      <c r="V137" s="614" t="s">
         <v>503</v>
       </c>
-      <c r="W137" s="603"/>
-      <c r="X137" s="603"/>
-      <c r="Y137" s="602"/>
+      <c r="W137" s="616"/>
+      <c r="X137" s="616"/>
+      <c r="Y137" s="615"/>
       <c r="Z137" s="367" t="s">
         <v>515</v>
       </c>
@@ -39790,12 +39777,12 @@
         <f>V221-(V223-V221)</f>
         <v>2250</v>
       </c>
-      <c r="Z218" s="592" t="s">
+      <c r="Z218" s="617" t="s">
         <v>810</v>
       </c>
-      <c r="AA218" s="593"/>
-      <c r="AB218" s="593"/>
-      <c r="AC218" s="594"/>
+      <c r="AA218" s="618"/>
+      <c r="AB218" s="618"/>
+      <c r="AC218" s="619"/>
       <c r="AD218" s="124" t="s">
         <v>811</v>
       </c>
@@ -39817,14 +39804,14 @@
       </c>
     </row>
     <row r="219" spans="10:36" x14ac:dyDescent="0.2">
-      <c r="L219" s="596" t="s">
+      <c r="L219" s="621" t="s">
         <v>504</v>
       </c>
-      <c r="M219" s="596"/>
-      <c r="N219" s="596"/>
-      <c r="O219" s="596"/>
-      <c r="P219" s="596"/>
-      <c r="Q219" s="596"/>
+      <c r="M219" s="621"/>
+      <c r="N219" s="621"/>
+      <c r="O219" s="621"/>
+      <c r="P219" s="621"/>
+      <c r="Q219" s="621"/>
       <c r="T219" s="3">
         <v>15</v>
       </c>
@@ -39852,10 +39839,10 @@
       <c r="AD219" s="124" t="s">
         <v>812</v>
       </c>
-      <c r="AF219" s="595" t="s">
+      <c r="AF219" s="620" t="s">
         <v>813</v>
       </c>
-      <c r="AG219" s="595"/>
+      <c r="AG219" s="620"/>
     </row>
     <row r="220" spans="10:36" x14ac:dyDescent="0.2">
       <c r="L220" s="124" t="s">
@@ -40239,22 +40226,22 @@
       <c r="I230" s="4"/>
       <c r="J230" s="4"/>
       <c r="K230" s="4"/>
-      <c r="AB230" s="597" t="s">
+      <c r="AB230" s="622" t="s">
         <v>819</v>
       </c>
-      <c r="AC230" s="597"/>
-      <c r="AD230" s="597"/>
-      <c r="AE230" s="597"/>
-      <c r="AG230" s="589" t="s">
+      <c r="AC230" s="622"/>
+      <c r="AD230" s="622"/>
+      <c r="AE230" s="622"/>
+      <c r="AG230" s="602" t="s">
         <v>816</v>
       </c>
-      <c r="AH230" s="590"/>
-      <c r="AI230" s="591"/>
-      <c r="AJ230" s="589" t="s">
+      <c r="AH230" s="603"/>
+      <c r="AI230" s="604"/>
+      <c r="AJ230" s="602" t="s">
         <v>65</v>
       </c>
-      <c r="AK230" s="590"/>
-      <c r="AL230" s="591"/>
+      <c r="AK230" s="603"/>
+      <c r="AL230" s="604"/>
     </row>
     <row r="231" spans="8:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H231" s="4"/>
@@ -40726,16 +40713,16 @@
       <c r="AC240" s="4"/>
       <c r="AD240" s="4"/>
       <c r="AF240" s="4"/>
-      <c r="AG240" s="589" t="s">
+      <c r="AG240" s="602" t="s">
         <v>816</v>
       </c>
-      <c r="AH240" s="590"/>
-      <c r="AI240" s="591"/>
-      <c r="AJ240" s="589" t="s">
+      <c r="AH240" s="603"/>
+      <c r="AI240" s="604"/>
+      <c r="AJ240" s="602" t="s">
         <v>65</v>
       </c>
-      <c r="AK240" s="590"/>
-      <c r="AL240" s="591"/>
+      <c r="AK240" s="603"/>
+      <c r="AL240" s="604"/>
     </row>
     <row r="241" spans="8:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H241" s="4"/>
@@ -40815,13 +40802,13 @@
       <c r="AI242" s="558">
         <v>0</v>
       </c>
-      <c r="AJ242" s="631">
+      <c r="AJ242" s="578">
         <v>1</v>
       </c>
-      <c r="AK242" s="632">
+      <c r="AK242" s="579">
         <v>1</v>
       </c>
-      <c r="AL242" s="633">
+      <c r="AL242" s="580">
         <v>1</v>
       </c>
     </row>
@@ -40836,13 +40823,13 @@
         <f>AI233</f>
         <v>2520.0000000000009</v>
       </c>
-      <c r="AJ243" s="631">
+      <c r="AJ243" s="578">
         <v>1</v>
       </c>
-      <c r="AK243" s="632">
+      <c r="AK243" s="579">
         <v>1</v>
       </c>
-      <c r="AL243" s="634">
+      <c r="AL243" s="581">
         <f>AL233</f>
         <v>0.85285285285285284</v>
       </c>
@@ -40859,14 +40846,14 @@
         <f>AI243+(AI247-AI243)/4</f>
         <v>2835.0000000000009</v>
       </c>
-      <c r="AJ244" s="631">
+      <c r="AJ244" s="578">
         <v>1</v>
       </c>
-      <c r="AK244" s="635">
+      <c r="AK244" s="582">
         <f>AK234</f>
         <v>0.85285285285285284</v>
       </c>
-      <c r="AL244" s="634">
+      <c r="AL244" s="581">
         <f>AL243+(AL247-AL243)/4</f>
         <v>0.81606606606606602</v>
       </c>
@@ -40884,15 +40871,15 @@
         <f>AI244+(AI247-AI243)/4</f>
         <v>3150.0000000000009</v>
       </c>
-      <c r="AJ245" s="636">
+      <c r="AJ245" s="583">
         <f>AJ235</f>
         <v>0.85285285285285284</v>
       </c>
-      <c r="AK245" s="635">
+      <c r="AK245" s="582">
         <f>AK244+(AK247-AK244)/3</f>
         <v>0.80380380380380378</v>
       </c>
-      <c r="AL245" s="637">
+      <c r="AL245" s="584">
         <f>AL244+(AL247-AL243)/4</f>
         <v>0.7792792792792792</v>
       </c>
@@ -40910,22 +40897,22 @@
         <f>AI245+(AI247-AI243)/4</f>
         <v>3465.0000000000009</v>
       </c>
-      <c r="AJ246" s="636">
+      <c r="AJ246" s="583">
         <f>(AJ247+AJ245)/2</f>
         <v>0.77927927927927931</v>
       </c>
-      <c r="AK246" s="638">
+      <c r="AK246" s="585">
         <f>AK245+(AK247-AK244)/3</f>
         <v>0.75475475475475473</v>
       </c>
-      <c r="AL246" s="637">
+      <c r="AL246" s="584">
         <f>AL245+(AL247-AL243)/4</f>
         <v>0.74249249249249238</v>
       </c>
     </row>
     <row r="247" spans="8:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG247" s="630">
-        <f t="shared" ref="AG246:AG247" si="141">AG237</f>
+      <c r="AG247" s="577">
+        <f t="shared" ref="AG247" si="141">AG237</f>
         <v>1575</v>
       </c>
       <c r="AH247" s="564">
@@ -40936,15 +40923,15 @@
         <f>AI237</f>
         <v>3780.0000000000005</v>
       </c>
-      <c r="AJ247" s="639">
+      <c r="AJ247" s="586">
         <f t="shared" ref="AJ247" si="142">AJ237</f>
         <v>0.70570570570570568</v>
       </c>
-      <c r="AK247" s="640">
+      <c r="AK247" s="587">
         <f>AK237</f>
         <v>0.70570570570570568</v>
       </c>
-      <c r="AL247" s="641">
+      <c r="AL247" s="588">
         <f>AL237</f>
         <v>0.70570570570570568</v>
       </c>
@@ -40975,6 +40962,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="AJ230:AL230"/>
+    <mergeCell ref="Z218:AC218"/>
+    <mergeCell ref="AF219:AG219"/>
+    <mergeCell ref="L219:Q219"/>
+    <mergeCell ref="AB230:AE230"/>
+    <mergeCell ref="AG230:AI230"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L137:O137"/>
+    <mergeCell ref="P137:S137"/>
+    <mergeCell ref="T137:U137"/>
+    <mergeCell ref="V137:Y137"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="L135:O135"/>
+    <mergeCell ref="P135:S135"/>
+    <mergeCell ref="T135:U135"/>
+    <mergeCell ref="V135:Y135"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="L64:O64"/>
+    <mergeCell ref="P64:S64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="V64:Y64"/>
     <mergeCell ref="AG240:AI240"/>
     <mergeCell ref="AJ240:AL240"/>
     <mergeCell ref="V4:Y4"/>
@@ -40991,28 +41000,6 @@
     <mergeCell ref="L62:O62"/>
     <mergeCell ref="P62:S62"/>
     <mergeCell ref="T62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="L64:O64"/>
-    <mergeCell ref="P64:S64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="L135:O135"/>
-    <mergeCell ref="P135:S135"/>
-    <mergeCell ref="T135:U135"/>
-    <mergeCell ref="V135:Y135"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L137:O137"/>
-    <mergeCell ref="P137:S137"/>
-    <mergeCell ref="T137:U137"/>
-    <mergeCell ref="V137:Y137"/>
-    <mergeCell ref="AJ230:AL230"/>
-    <mergeCell ref="Z218:AC218"/>
-    <mergeCell ref="AF219:AG219"/>
-    <mergeCell ref="L219:Q219"/>
-    <mergeCell ref="AB230:AE230"/>
-    <mergeCell ref="AG230:AI230"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -41030,10 +41017,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="C2:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -41159,12 +41143,12 @@
       <c r="I5" s="121"/>
       <c r="J5" s="121"/>
       <c r="K5" s="121"/>
-      <c r="L5" s="607" t="s">
+      <c r="L5" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="608"/>
-      <c r="N5" s="608"/>
-      <c r="O5" s="609"/>
+      <c r="M5" s="606"/>
+      <c r="N5" s="606"/>
+      <c r="O5" s="607"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -41195,12 +41179,12 @@
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
       <c r="K6" s="37"/>
-      <c r="L6" s="601" t="s">
+      <c r="L6" s="614" t="s">
         <v>503</v>
       </c>
-      <c r="M6" s="603"/>
-      <c r="N6" s="603"/>
-      <c r="O6" s="602"/>
+      <c r="M6" s="616"/>
+      <c r="N6" s="616"/>
+      <c r="O6" s="615"/>
       <c r="P6" s="367" t="s">
         <v>515</v>
       </c>
@@ -42086,23 +42070,23 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="607" t="s">
+      <c r="L33" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="608"/>
-      <c r="N33" s="608"/>
-      <c r="O33" s="609"/>
+      <c r="M33" s="606"/>
+      <c r="N33" s="606"/>
+      <c r="O33" s="607"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L34" s="601" t="s">
+      <c r="L34" s="614" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="603"/>
-      <c r="N34" s="603"/>
-      <c r="O34" s="602"/>
+      <c r="M34" s="616"/>
+      <c r="N34" s="616"/>
+      <c r="O34" s="615"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="3" t="s">
@@ -42347,10 +42331,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C2:AK347"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -42445,16 +42426,16 @@
       <c r="G4" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="604" t="s">
+      <c r="H4" s="611" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="605"/>
-      <c r="J4" s="606"/>
-      <c r="K4" s="607" t="s">
+      <c r="I4" s="612"/>
+      <c r="J4" s="613"/>
+      <c r="K4" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="608"/>
-      <c r="M4" s="609"/>
+      <c r="L4" s="606"/>
+      <c r="M4" s="607"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -42480,16 +42461,16 @@
       <c r="G5" s="375" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="613" t="s">
+      <c r="H5" s="623" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="614"/>
-      <c r="J5" s="615"/>
-      <c r="K5" s="613" t="s">
+      <c r="I5" s="624"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="623" t="s">
         <v>292</v>
       </c>
-      <c r="L5" s="614"/>
-      <c r="M5" s="615"/>
+      <c r="L5" s="624"/>
+      <c r="M5" s="625"/>
       <c r="N5" s="376" t="s">
         <v>92</v>
       </c>
@@ -42506,23 +42487,23 @@
         <v>210</v>
       </c>
       <c r="AA5" s="201"/>
-      <c r="AB5" s="610" t="s">
+      <c r="AB5" s="626" t="s">
         <v>541</v>
       </c>
-      <c r="AC5" s="610"/>
+      <c r="AC5" s="626"/>
       <c r="AD5" s="378"/>
-      <c r="AE5" s="611" t="s">
+      <c r="AE5" s="627" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="611"/>
-      <c r="AG5" s="611" t="s">
+      <c r="AF5" s="627"/>
+      <c r="AG5" s="627" t="s">
         <v>542</v>
       </c>
-      <c r="AH5" s="611"/>
-      <c r="AI5" s="612" t="s">
+      <c r="AH5" s="627"/>
+      <c r="AI5" s="628" t="s">
         <v>543</v>
       </c>
-      <c r="AJ5" s="612"/>
+      <c r="AJ5" s="628"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="422" t="str">
@@ -43260,12 +43241,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="607" t="s">
+      <c r="L27" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="608"/>
-      <c r="N27" s="608"/>
-      <c r="O27" s="609"/>
+      <c r="M27" s="606"/>
+      <c r="N27" s="606"/>
+      <c r="O27" s="607"/>
       <c r="T27" s="203"/>
       <c r="U27" s="203"/>
     </row>
@@ -43273,12 +43254,12 @@
       <c r="J28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L28" s="598" t="s">
+      <c r="L28" s="608" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="599"/>
-      <c r="N28" s="599"/>
-      <c r="O28" s="600"/>
+      <c r="M28" s="609"/>
+      <c r="N28" s="609"/>
+      <c r="O28" s="610"/>
       <c r="T28" s="203"/>
       <c r="U28" s="203"/>
     </row>
@@ -44668,16 +44649,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -44695,10 +44676,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CK183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BC20" sqref="BC20"/>
-    </sheetView>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -45111,128 +45089,128 @@
       <c r="C4" s="273" t="s">
         <v>301</v>
       </c>
-      <c r="D4" s="617" t="s">
+      <c r="D4" s="629" t="s">
         <v>302</v>
       </c>
-      <c r="E4" s="616"/>
-      <c r="F4" s="616"/>
-      <c r="G4" s="616"/>
-      <c r="H4" s="618"/>
-      <c r="I4" s="616" t="s">
+      <c r="E4" s="630"/>
+      <c r="F4" s="630"/>
+      <c r="G4" s="630"/>
+      <c r="H4" s="631"/>
+      <c r="I4" s="630" t="s">
         <v>303</v>
       </c>
-      <c r="J4" s="616"/>
-      <c r="K4" s="616"/>
-      <c r="L4" s="616"/>
-      <c r="M4" s="618"/>
-      <c r="N4" s="616" t="s">
+      <c r="J4" s="630"/>
+      <c r="K4" s="630"/>
+      <c r="L4" s="630"/>
+      <c r="M4" s="631"/>
+      <c r="N4" s="630" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="616"/>
-      <c r="P4" s="616"/>
-      <c r="Q4" s="616"/>
-      <c r="R4" s="618"/>
-      <c r="S4" s="616" t="s">
+      <c r="O4" s="630"/>
+      <c r="P4" s="630"/>
+      <c r="Q4" s="630"/>
+      <c r="R4" s="631"/>
+      <c r="S4" s="630" t="s">
         <v>305</v>
       </c>
-      <c r="T4" s="616"/>
-      <c r="U4" s="616"/>
-      <c r="V4" s="616"/>
-      <c r="W4" s="618"/>
-      <c r="X4" s="616" t="s">
+      <c r="T4" s="630"/>
+      <c r="U4" s="630"/>
+      <c r="V4" s="630"/>
+      <c r="W4" s="631"/>
+      <c r="X4" s="630" t="s">
         <v>306</v>
       </c>
-      <c r="Y4" s="616"/>
-      <c r="Z4" s="616"/>
-      <c r="AA4" s="616"/>
-      <c r="AB4" s="618"/>
-      <c r="AC4" s="616" t="s">
+      <c r="Y4" s="630"/>
+      <c r="Z4" s="630"/>
+      <c r="AA4" s="630"/>
+      <c r="AB4" s="631"/>
+      <c r="AC4" s="630" t="s">
         <v>307</v>
       </c>
-      <c r="AD4" s="616"/>
-      <c r="AE4" s="616"/>
-      <c r="AF4" s="616"/>
-      <c r="AG4" s="618"/>
-      <c r="AH4" s="616" t="s">
+      <c r="AD4" s="630"/>
+      <c r="AE4" s="630"/>
+      <c r="AF4" s="630"/>
+      <c r="AG4" s="631"/>
+      <c r="AH4" s="630" t="s">
         <v>308</v>
       </c>
-      <c r="AI4" s="616"/>
-      <c r="AJ4" s="616"/>
-      <c r="AK4" s="616"/>
-      <c r="AL4" s="618"/>
-      <c r="AM4" s="616" t="s">
+      <c r="AI4" s="630"/>
+      <c r="AJ4" s="630"/>
+      <c r="AK4" s="630"/>
+      <c r="AL4" s="631"/>
+      <c r="AM4" s="630" t="s">
         <v>309</v>
       </c>
-      <c r="AN4" s="616"/>
-      <c r="AO4" s="616"/>
-      <c r="AP4" s="616"/>
-      <c r="AQ4" s="618"/>
-      <c r="AR4" s="616" t="s">
+      <c r="AN4" s="630"/>
+      <c r="AO4" s="630"/>
+      <c r="AP4" s="630"/>
+      <c r="AQ4" s="631"/>
+      <c r="AR4" s="630" t="s">
         <v>310</v>
       </c>
-      <c r="AS4" s="616"/>
-      <c r="AT4" s="616"/>
-      <c r="AU4" s="616"/>
-      <c r="AV4" s="618"/>
-      <c r="AW4" s="616" t="s">
+      <c r="AS4" s="630"/>
+      <c r="AT4" s="630"/>
+      <c r="AU4" s="630"/>
+      <c r="AV4" s="631"/>
+      <c r="AW4" s="630" t="s">
         <v>311</v>
       </c>
-      <c r="AX4" s="616"/>
-      <c r="AY4" s="616"/>
-      <c r="AZ4" s="616"/>
-      <c r="BA4" s="616"/>
-      <c r="BB4" s="617" t="s">
+      <c r="AX4" s="630"/>
+      <c r="AY4" s="630"/>
+      <c r="AZ4" s="630"/>
+      <c r="BA4" s="630"/>
+      <c r="BB4" s="629" t="s">
         <v>312</v>
       </c>
-      <c r="BC4" s="616"/>
-      <c r="BD4" s="616"/>
-      <c r="BE4" s="616"/>
-      <c r="BF4" s="618"/>
-      <c r="BG4" s="616" t="s">
+      <c r="BC4" s="630"/>
+      <c r="BD4" s="630"/>
+      <c r="BE4" s="630"/>
+      <c r="BF4" s="631"/>
+      <c r="BG4" s="630" t="s">
         <v>313</v>
       </c>
-      <c r="BH4" s="616"/>
-      <c r="BI4" s="616"/>
-      <c r="BJ4" s="616"/>
-      <c r="BK4" s="616"/>
-      <c r="BL4" s="617" t="s">
+      <c r="BH4" s="630"/>
+      <c r="BI4" s="630"/>
+      <c r="BJ4" s="630"/>
+      <c r="BK4" s="630"/>
+      <c r="BL4" s="629" t="s">
         <v>314</v>
       </c>
-      <c r="BM4" s="616"/>
-      <c r="BN4" s="616"/>
-      <c r="BO4" s="616"/>
-      <c r="BP4" s="616"/>
-      <c r="BQ4" s="617" t="s">
+      <c r="BM4" s="630"/>
+      <c r="BN4" s="630"/>
+      <c r="BO4" s="630"/>
+      <c r="BP4" s="630"/>
+      <c r="BQ4" s="629" t="s">
         <v>315</v>
       </c>
-      <c r="BR4" s="616"/>
-      <c r="BS4" s="616"/>
-      <c r="BT4" s="616"/>
-      <c r="BU4" s="618"/>
+      <c r="BR4" s="630"/>
+      <c r="BS4" s="630"/>
+      <c r="BT4" s="630"/>
+      <c r="BU4" s="631"/>
       <c r="BV4" s="274" t="s">
         <v>316</v>
       </c>
-      <c r="BW4" s="619" t="s">
+      <c r="BW4" s="632" t="s">
         <v>317</v>
       </c>
-      <c r="BX4" s="620"/>
-      <c r="BY4" s="620"/>
-      <c r="BZ4" s="620"/>
-      <c r="CA4" s="621"/>
-      <c r="CB4" s="619" t="s">
+      <c r="BX4" s="633"/>
+      <c r="BY4" s="633"/>
+      <c r="BZ4" s="633"/>
+      <c r="CA4" s="634"/>
+      <c r="CB4" s="632" t="s">
         <v>318</v>
       </c>
-      <c r="CC4" s="620"/>
-      <c r="CD4" s="620"/>
-      <c r="CE4" s="620"/>
-      <c r="CF4" s="621"/>
-      <c r="CG4" s="619" t="s">
+      <c r="CC4" s="633"/>
+      <c r="CD4" s="633"/>
+      <c r="CE4" s="633"/>
+      <c r="CF4" s="634"/>
+      <c r="CG4" s="632" t="s">
         <v>319</v>
       </c>
-      <c r="CH4" s="620"/>
-      <c r="CI4" s="620"/>
-      <c r="CJ4" s="620"/>
-      <c r="CK4" s="621"/>
+      <c r="CH4" s="633"/>
+      <c r="CI4" s="633"/>
+      <c r="CJ4" s="633"/>
+      <c r="CK4" s="634"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="276"/>
@@ -58801,11 +58779,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -58818,6 +58791,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -58829,10 +58807,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AD121"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -58843,23 +58818,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="625" t="s">
+      <c r="A1" s="636" t="s">
         <v>585</v>
       </c>
-      <c r="B1" s="627" t="s">
+      <c r="B1" s="638" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="628"/>
-      <c r="D1" s="628"/>
-      <c r="E1" s="628"/>
-      <c r="F1" s="629"/>
-      <c r="G1" s="627" t="s">
+      <c r="C1" s="639"/>
+      <c r="D1" s="639"/>
+      <c r="E1" s="639"/>
+      <c r="F1" s="640"/>
+      <c r="G1" s="638" t="s">
         <v>587</v>
       </c>
-      <c r="H1" s="628"/>
-      <c r="I1" s="628"/>
-      <c r="J1" s="628"/>
-      <c r="K1" s="629"/>
+      <c r="H1" s="639"/>
+      <c r="I1" s="639"/>
+      <c r="J1" s="639"/>
+      <c r="K1" s="640"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -58869,7 +58844,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="626"/>
+      <c r="A2" s="637"/>
       <c r="B2" s="443" t="s">
         <v>254</v>
       </c>
@@ -59015,12 +58990,12 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="622" t="s">
+      <c r="A7" s="635" t="s">
         <v>588</v>
       </c>
-      <c r="B7" s="622"/>
-      <c r="C7" s="622"/>
-      <c r="D7" s="622"/>
+      <c r="B7" s="635"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -59306,12 +59281,12 @@
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="622" t="s">
+      <c r="A18" s="635" t="s">
         <v>602</v>
       </c>
-      <c r="B18" s="622"/>
-      <c r="C18" s="622"/>
-      <c r="D18" s="622"/>
+      <c r="B18" s="635"/>
+      <c r="C18" s="635"/>
+      <c r="D18" s="635"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -59566,12 +59541,12 @@
       <c r="R27" s="3"/>
     </row>
     <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="622" t="s">
+      <c r="A28" s="635" t="s">
         <v>610</v>
       </c>
-      <c r="B28" s="622"/>
-      <c r="C28" s="622"/>
-      <c r="D28" s="622"/>
+      <c r="B28" s="635"/>
+      <c r="C28" s="635"/>
+      <c r="D28" s="635"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -60059,12 +60034,12 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="622" t="s">
+      <c r="A40" s="635" t="s">
         <v>591</v>
       </c>
-      <c r="B40" s="622"/>
-      <c r="C40" s="622"/>
-      <c r="D40" s="622"/>
+      <c r="B40" s="635"/>
+      <c r="C40" s="635"/>
+      <c r="D40" s="635"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -60240,12 +60215,12 @@
       <c r="T44" s="3"/>
     </row>
     <row r="45" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="622" t="s">
+      <c r="A45" s="635" t="s">
         <v>619</v>
       </c>
-      <c r="B45" s="622"/>
-      <c r="C45" s="622"/>
-      <c r="D45" s="622"/>
+      <c r="B45" s="635"/>
+      <c r="C45" s="635"/>
+      <c r="D45" s="635"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -60362,11 +60337,11 @@
       <c r="Y48" t="s">
         <v>636</v>
       </c>
-      <c r="Z48" s="623" t="s">
+      <c r="Z48" s="641" t="s">
         <v>574</v>
       </c>
-      <c r="AA48" s="624"/>
-      <c r="AB48" s="624"/>
+      <c r="AA48" s="642"/>
+      <c r="AB48" s="642"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -60583,11 +60558,11 @@
       <c r="Y53" t="s">
         <v>638</v>
       </c>
-      <c r="Z53" s="623" t="s">
+      <c r="Z53" s="641" t="s">
         <v>573</v>
       </c>
-      <c r="AA53" s="624"/>
-      <c r="AB53" s="624"/>
+      <c r="AA53" s="642"/>
+      <c r="AB53" s="642"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -60789,11 +60764,11 @@
       <c r="Y59" t="s">
         <v>639</v>
       </c>
-      <c r="Z59" s="623" t="s">
+      <c r="Z59" s="641" t="s">
         <v>640</v>
       </c>
-      <c r="AA59" s="624"/>
-      <c r="AB59" s="624"/>
+      <c r="AA59" s="642"/>
+      <c r="AB59" s="642"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="463" t="str">
@@ -61630,17 +61605,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Tech CEFF~2019 changed to CEFF
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC2ECFB-CB59-4B1A-AF6A-C2E80D7F9F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18652DE8-F8DE-4BFB-82ED-82AACE9F2B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2CC7CA6E-3559-4BC7-B5C1-253B80EF5435}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2CC7CA6E-3559-4BC7-B5C1-253B80EF5435}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -8639,7 +8639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2647" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2647" uniqueCount="823">
   <si>
     <t>Document type:</t>
   </si>
@@ -10849,9 +10849,6 @@
     <t>RSDSH_Det-AB</t>
   </si>
   <si>
-    <t>CEFF~2019</t>
-  </si>
-  <si>
     <t>CEFF~2030</t>
   </si>
   <si>
@@ -11126,6 +11123,12 @@
   </si>
   <si>
     <t>Smoothed</t>
+  </si>
+  <si>
+    <t>CEFF</t>
+  </si>
+  <si>
+    <t>INVCOST</t>
   </si>
 </sst>
 </file>
@@ -13956,42 +13959,6 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -14010,13 +13977,40 @@
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -14028,10 +14022,19 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14049,6 +14052,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14063,12 +14072,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -20987,8 +20990,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB41" sqref="AB41"/>
+    <sheetView tabSelected="1" topLeftCell="G124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V135" sqref="V135:Y135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21060,16 +21063,16 @@
         <v>24</v>
       </c>
       <c r="H3" s="17" t="s">
+        <v>821</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>729</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="J3" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="K3" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>218</v>
@@ -21102,7 +21105,7 @@
         <v>76</v>
       </c>
       <c r="V3" s="17" t="s">
-        <v>236</v>
+        <v>822</v>
       </c>
       <c r="W3" s="17" t="s">
         <v>88</v>
@@ -21163,34 +21166,34 @@
       <c r="G4" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="611" t="s">
+      <c r="H4" s="617" t="s">
         <v>258</v>
       </c>
-      <c r="I4" s="612"/>
-      <c r="J4" s="612"/>
-      <c r="K4" s="613"/>
-      <c r="L4" s="611" t="s">
+      <c r="I4" s="618"/>
+      <c r="J4" s="618"/>
+      <c r="K4" s="619"/>
+      <c r="L4" s="617" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="612"/>
-      <c r="N4" s="612"/>
-      <c r="O4" s="613"/>
-      <c r="P4" s="611" t="s">
+      <c r="M4" s="618"/>
+      <c r="N4" s="618"/>
+      <c r="O4" s="619"/>
+      <c r="P4" s="617" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="612"/>
-      <c r="R4" s="612"/>
-      <c r="S4" s="613"/>
-      <c r="T4" s="611" t="s">
+      <c r="Q4" s="618"/>
+      <c r="R4" s="618"/>
+      <c r="S4" s="619"/>
+      <c r="T4" s="617" t="s">
         <v>85</v>
       </c>
-      <c r="U4" s="613"/>
-      <c r="V4" s="605" t="s">
+      <c r="U4" s="619"/>
+      <c r="V4" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="606"/>
-      <c r="X4" s="606"/>
-      <c r="Y4" s="607"/>
+      <c r="W4" s="621"/>
+      <c r="X4" s="621"/>
+      <c r="Y4" s="622"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21293,34 +21296,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="608" t="s">
+      <c r="H6" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="609"/>
-      <c r="J6" s="609"/>
-      <c r="K6" s="610"/>
-      <c r="L6" s="609" t="s">
+      <c r="I6" s="612"/>
+      <c r="J6" s="612"/>
+      <c r="K6" s="613"/>
+      <c r="L6" s="612" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="609"/>
-      <c r="N6" s="609"/>
-      <c r="O6" s="610"/>
-      <c r="P6" s="608" t="s">
+      <c r="M6" s="612"/>
+      <c r="N6" s="612"/>
+      <c r="O6" s="613"/>
+      <c r="P6" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="609"/>
-      <c r="R6" s="609"/>
-      <c r="S6" s="610"/>
-      <c r="T6" s="608" t="s">
+      <c r="Q6" s="612"/>
+      <c r="R6" s="612"/>
+      <c r="S6" s="613"/>
+      <c r="T6" s="611" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="610"/>
-      <c r="V6" s="608" t="s">
+      <c r="U6" s="613"/>
+      <c r="V6" s="611" t="s">
         <v>503</v>
       </c>
-      <c r="W6" s="609"/>
-      <c r="X6" s="609"/>
-      <c r="Y6" s="610"/>
+      <c r="W6" s="612"/>
+      <c r="X6" s="612"/>
+      <c r="Y6" s="613"/>
       <c r="Z6" s="520" t="s">
         <v>515</v>
       </c>
@@ -23128,7 +23131,7 @@
         <v>R-SH_Apt_ELC_HPN2-G</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E25" s="27" t="s">
         <v>148</v>
@@ -23137,7 +23140,7 @@
         <v>558</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H25" s="22">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ247</f>
@@ -23805,7 +23808,7 @@
         <v>R-SW_Apt_ELC_HPN1-G</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E31" s="27" t="s">
         <v>148</v>
@@ -23814,7 +23817,7 @@
         <v>660</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H31" s="246">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ247</f>
@@ -23920,7 +23923,7 @@
         <v>R-SH_Apt_ELC_HPN3-AB</v>
       </c>
       <c r="D32" s="88" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E32" s="88" t="s">
         <v>148</v>
@@ -24023,7 +24026,7 @@
         <v>R-SH_Apt_ELC_HPN3-C</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>148</v>
@@ -24126,7 +24129,7 @@
         <v>R-SH_Apt_ELC_HPN3-D</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E34" s="30" t="s">
         <v>148</v>
@@ -24228,7 +24231,7 @@
         <v>R-SH_Apt_ELC_HPN3-E</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>148</v>
@@ -24331,7 +24334,7 @@
         <v>R-SH_Apt_ELC_HPN3-F</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E36" s="30" t="s">
         <v>148</v>
@@ -24434,7 +24437,7 @@
         <v>R-SH_Apt_ELC_HPN3-G</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E37" s="27" t="s">
         <v>148</v>
@@ -24443,7 +24446,7 @@
         <v>558</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H37" s="22">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ247</f>
@@ -24537,7 +24540,7 @@
         <v>R-HC_Apt_ELC_HPN2-AB</v>
       </c>
       <c r="D38" s="88" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E38" s="88" t="s">
         <v>148</v>
@@ -24546,7 +24549,7 @@
         <v>558</v>
       </c>
       <c r="G38" s="88" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H38" s="19">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -24650,7 +24653,7 @@
         <v>R-HC_Apt_ELC_HPN2-C</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>148</v>
@@ -24659,7 +24662,7 @@
         <v>558</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H39" s="22">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -24764,7 +24767,7 @@
         <v>R-HC_Apt_ELC_HPN2-D</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E40" s="30" t="s">
         <v>148</v>
@@ -24773,7 +24776,7 @@
         <v>558</v>
       </c>
       <c r="G40" s="30" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H40" s="40">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -24877,7 +24880,7 @@
         <v>R-HC_Apt_ELC_HPN2-E</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>148</v>
@@ -24886,7 +24889,7 @@
         <v>558</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H41" s="22">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ245</f>
@@ -24987,7 +24990,7 @@
         <v>R-HC_Apt_ELC_HPN2-F</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E42" s="30" t="s">
         <v>148</v>
@@ -24996,7 +24999,7 @@
         <v>558</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H42" s="40">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ246</f>
@@ -25097,7 +25100,7 @@
         <v>R-HC_Apt_ELC_HPN2-G</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>148</v>
@@ -25106,7 +25109,7 @@
         <v>558</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H43" s="22">
         <f>(JRC_Data!$AC$18/JRC_Data!$AC$16)*AJ247</f>
@@ -26379,7 +26382,7 @@
         <v>659</v>
       </c>
       <c r="AN60" s="482" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="AO60" s="483" t="s">
         <v>13</v>
@@ -26412,16 +26415,16 @@
         <v>24</v>
       </c>
       <c r="H61" s="17" t="s">
+        <v>821</v>
+      </c>
+      <c r="I61" s="17" t="s">
         <v>729</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="J61" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="J61" s="17" t="s">
+      <c r="K61" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="K61" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="L61" s="17" t="s">
         <v>226</v>
@@ -26454,7 +26457,7 @@
         <v>76</v>
       </c>
       <c r="V61" s="17" t="s">
-        <v>236</v>
+        <v>822</v>
       </c>
       <c r="W61" s="17" t="s">
         <v>88</v>
@@ -26515,34 +26518,34 @@
       <c r="G62" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H62" s="611" t="s">
+      <c r="H62" s="617" t="s">
         <v>82</v>
       </c>
-      <c r="I62" s="612"/>
-      <c r="J62" s="612"/>
-      <c r="K62" s="613"/>
-      <c r="L62" s="611" t="s">
+      <c r="I62" s="618"/>
+      <c r="J62" s="618"/>
+      <c r="K62" s="619"/>
+      <c r="L62" s="617" t="s">
         <v>83</v>
       </c>
-      <c r="M62" s="612"/>
-      <c r="N62" s="612"/>
-      <c r="O62" s="613"/>
-      <c r="P62" s="611" t="s">
+      <c r="M62" s="618"/>
+      <c r="N62" s="618"/>
+      <c r="O62" s="619"/>
+      <c r="P62" s="617" t="s">
         <v>84</v>
       </c>
-      <c r="Q62" s="612"/>
-      <c r="R62" s="612"/>
-      <c r="S62" s="613"/>
-      <c r="T62" s="611" t="s">
+      <c r="Q62" s="618"/>
+      <c r="R62" s="618"/>
+      <c r="S62" s="619"/>
+      <c r="T62" s="617" t="s">
         <v>85</v>
       </c>
-      <c r="U62" s="613"/>
-      <c r="V62" s="605" t="s">
+      <c r="U62" s="619"/>
+      <c r="V62" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="W62" s="606"/>
-      <c r="X62" s="606"/>
-      <c r="Y62" s="607"/>
+      <c r="W62" s="621"/>
+      <c r="X62" s="621"/>
+      <c r="Y62" s="622"/>
       <c r="Z62" s="60"/>
       <c r="AA62" s="60"/>
       <c r="AB62" s="68" t="s">
@@ -26645,24 +26648,24 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="39"/>
-      <c r="H64" s="608" t="s">
+      <c r="H64" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="I64" s="609"/>
-      <c r="J64" s="609"/>
-      <c r="K64" s="610"/>
-      <c r="L64" s="609" t="s">
+      <c r="I64" s="612"/>
+      <c r="J64" s="612"/>
+      <c r="K64" s="613"/>
+      <c r="L64" s="612" t="s">
         <v>34</v>
       </c>
-      <c r="M64" s="609"/>
-      <c r="N64" s="609"/>
-      <c r="O64" s="610"/>
-      <c r="P64" s="608" t="s">
+      <c r="M64" s="612"/>
+      <c r="N64" s="612"/>
+      <c r="O64" s="613"/>
+      <c r="P64" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="Q64" s="609"/>
-      <c r="R64" s="609"/>
-      <c r="S64" s="610"/>
+      <c r="Q64" s="612"/>
+      <c r="R64" s="612"/>
+      <c r="S64" s="613"/>
       <c r="T64" s="614" t="s">
         <v>68</v>
       </c>
@@ -28916,7 +28919,7 @@
         <v>558</v>
       </c>
       <c r="G87" s="24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H87" s="22">
         <v>1</v>
@@ -29008,7 +29011,7 @@
         <v>R-SH_Att_ELC_HPN2-D</v>
       </c>
       <c r="D88" s="30" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E88" s="30" t="s">
         <v>148</v>
@@ -29017,7 +29020,7 @@
         <v>558</v>
       </c>
       <c r="G88" s="30" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H88" s="40">
         <v>1</v>
@@ -29118,7 +29121,7 @@
         <v>558</v>
       </c>
       <c r="G89" s="24" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H89" s="22">
         <v>1</v>
@@ -29219,7 +29222,7 @@
         <v>558</v>
       </c>
       <c r="G90" s="30" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H90" s="40">
         <v>1</v>
@@ -29311,7 +29314,7 @@
         <v>R-SH_Att_ELC_HPN2-G</v>
       </c>
       <c r="D91" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E91" s="27" t="s">
         <v>148</v>
@@ -29320,7 +29323,7 @@
         <v>558</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H91" s="246">
         <v>1</v>
@@ -29421,7 +29424,7 @@
         <v>660</v>
       </c>
       <c r="G92" s="88" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H92" s="19">
         <v>1</v>
@@ -29534,7 +29537,7 @@
         <v>660</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H93" s="22">
         <v>1</v>
@@ -29646,7 +29649,7 @@
         <v>660</v>
       </c>
       <c r="G94" s="30" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H94" s="40">
         <v>1</v>
@@ -29758,7 +29761,7 @@
         <v>660</v>
       </c>
       <c r="G95" s="24" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H95" s="22">
         <v>1</v>
@@ -29870,7 +29873,7 @@
         <v>660</v>
       </c>
       <c r="G96" s="30" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H96" s="40">
         <v>1</v>
@@ -29973,7 +29976,7 @@
         <v>R-SW_Att_ELC_HPN1-G</v>
       </c>
       <c r="D97" s="27" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E97" s="27" t="s">
         <v>148</v>
@@ -29982,7 +29985,7 @@
         <v>660</v>
       </c>
       <c r="G97" s="27" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H97" s="246">
         <v>1</v>
@@ -30085,7 +30088,7 @@
         <v>R-SW_Att_ELC_HPN2-AB</v>
       </c>
       <c r="D98" s="88" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E98" s="88" t="s">
         <v>550</v>
@@ -30094,7 +30097,7 @@
         <v>660</v>
       </c>
       <c r="G98" s="88" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H98" s="19">
         <v>1</v>
@@ -30199,7 +30202,7 @@
         <v>R-SW_Att_ELC_HPN2-C</v>
       </c>
       <c r="D99" s="24" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E99" s="24" t="s">
         <v>550</v>
@@ -30208,7 +30211,7 @@
         <v>660</v>
       </c>
       <c r="G99" s="24" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H99" s="22">
         <v>1</v>
@@ -30313,7 +30316,7 @@
         <v>R-SW_Att_ELC_HPN2-D</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>550</v>
@@ -30322,7 +30325,7 @@
         <v>660</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H100" s="40">
         <v>1</v>
@@ -30427,7 +30430,7 @@
         <v>R-SW_Att_ELC_HPN2-E</v>
       </c>
       <c r="D101" s="24" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E101" s="24" t="s">
         <v>550</v>
@@ -30436,7 +30439,7 @@
         <v>660</v>
       </c>
       <c r="G101" s="24" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H101" s="22">
         <v>1</v>
@@ -30541,7 +30544,7 @@
         <v>R-SW_Att_ELC_HPN2-F</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E102" s="30" t="s">
         <v>550</v>
@@ -30550,7 +30553,7 @@
         <v>660</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H102" s="40">
         <v>1</v>
@@ -30655,7 +30658,7 @@
         <v>R-SW_Att_ELC_HPN2-G</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E103" s="27" t="s">
         <v>550</v>
@@ -30664,7 +30667,7 @@
         <v>660</v>
       </c>
       <c r="G103" s="27" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H103" s="246">
         <v>1</v>
@@ -30769,7 +30772,7 @@
         <v>R-SH_Att_ELC_HPN3-AB</v>
       </c>
       <c r="D104" s="88" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E104" s="88" t="s">
         <v>148</v>
@@ -30871,7 +30874,7 @@
         <v>R-SH_Att_ELC_HPN3-C</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>148</v>
@@ -30880,7 +30883,7 @@
         <v>558</v>
       </c>
       <c r="G105" s="24" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H105" s="22">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -30973,7 +30976,7 @@
         <v>R-SH_Att_ELC_HPN3-D</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E106" s="30" t="s">
         <v>148</v>
@@ -30982,7 +30985,7 @@
         <v>558</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H106" s="40">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31075,7 +31078,7 @@
         <v>R-SH_Att_ELC_HPN3-E</v>
       </c>
       <c r="D107" s="24" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E107" s="24" t="s">
         <v>148</v>
@@ -31084,7 +31087,7 @@
         <v>558</v>
       </c>
       <c r="G107" s="24" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H107" s="22">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31177,7 +31180,7 @@
         <v>R-SH_Att_ELC_HPN3-F</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E108" s="30" t="s">
         <v>148</v>
@@ -31186,7 +31189,7 @@
         <v>558</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H108" s="40">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31279,7 +31282,7 @@
         <v>R-SH_Att_ELC_HPN3-G</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E109" s="27" t="s">
         <v>148</v>
@@ -31288,7 +31291,7 @@
         <v>558</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H109" s="246">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31381,7 +31384,7 @@
         <v>R-HC_Att_ELC_HPN2-AB</v>
       </c>
       <c r="D110" s="88" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E110" s="88" t="s">
         <v>148</v>
@@ -31390,7 +31393,7 @@
         <v>558</v>
       </c>
       <c r="G110" s="88" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H110" s="19">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31495,7 +31498,7 @@
         <v>R-HC_Att_ELC_HPN2-C</v>
       </c>
       <c r="D111" s="24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>148</v>
@@ -31504,7 +31507,7 @@
         <v>558</v>
       </c>
       <c r="G111" s="24" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H111" s="22">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31609,7 +31612,7 @@
         <v>R-HC_Att_ELC_HPN2-D</v>
       </c>
       <c r="D112" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E112" s="30" t="s">
         <v>148</v>
@@ -31618,7 +31621,7 @@
         <v>558</v>
       </c>
       <c r="G112" s="30" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H112" s="40">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31723,7 +31726,7 @@
         <v>R-HC_Att_ELC_HPN2-E</v>
       </c>
       <c r="D113" s="24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>148</v>
@@ -31732,7 +31735,7 @@
         <v>558</v>
       </c>
       <c r="G113" s="24" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H113" s="22">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31837,7 +31840,7 @@
         <v>R-HC_Att_ELC_HPN2-F</v>
       </c>
       <c r="D114" s="30" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E114" s="30" t="s">
         <v>148</v>
@@ -31846,7 +31849,7 @@
         <v>558</v>
       </c>
       <c r="G114" s="30" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H114" s="40">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -31952,7 +31955,7 @@
         <v>R-HC_Att_ELC_HPN2-G</v>
       </c>
       <c r="D115" s="27" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E115" s="27" t="s">
         <v>148</v>
@@ -31961,7 +31964,7 @@
         <v>558</v>
       </c>
       <c r="G115" s="27" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H115" s="246">
         <f>JRC_Data!AC20/JRC_Data!$AC$16</f>
@@ -33163,16 +33166,16 @@
         <v>24</v>
       </c>
       <c r="H134" s="17" t="s">
+        <v>821</v>
+      </c>
+      <c r="I134" s="17" t="s">
         <v>729</v>
       </c>
-      <c r="I134" s="17" t="s">
+      <c r="J134" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="J134" s="17" t="s">
+      <c r="K134" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="K134" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="L134" s="17" t="s">
         <v>530</v>
@@ -33205,7 +33208,7 @@
         <v>76</v>
       </c>
       <c r="V134" s="17" t="s">
-        <v>236</v>
+        <v>822</v>
       </c>
       <c r="W134" s="17" t="s">
         <v>88</v>
@@ -33287,34 +33290,34 @@
       <c r="G135" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H135" s="611" t="s">
+      <c r="H135" s="617" t="s">
         <v>82</v>
       </c>
-      <c r="I135" s="612"/>
-      <c r="J135" s="612"/>
-      <c r="K135" s="613"/>
-      <c r="L135" s="611" t="s">
+      <c r="I135" s="618"/>
+      <c r="J135" s="618"/>
+      <c r="K135" s="619"/>
+      <c r="L135" s="617" t="s">
         <v>83</v>
       </c>
-      <c r="M135" s="612"/>
-      <c r="N135" s="612"/>
-      <c r="O135" s="613"/>
-      <c r="P135" s="611" t="s">
+      <c r="M135" s="618"/>
+      <c r="N135" s="618"/>
+      <c r="O135" s="619"/>
+      <c r="P135" s="617" t="s">
         <v>84</v>
       </c>
-      <c r="Q135" s="612"/>
-      <c r="R135" s="612"/>
-      <c r="S135" s="613"/>
-      <c r="T135" s="611" t="s">
+      <c r="Q135" s="618"/>
+      <c r="R135" s="618"/>
+      <c r="S135" s="619"/>
+      <c r="T135" s="617" t="s">
         <v>85</v>
       </c>
-      <c r="U135" s="613"/>
-      <c r="V135" s="605" t="s">
+      <c r="U135" s="619"/>
+      <c r="V135" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="W135" s="606"/>
-      <c r="X135" s="606"/>
-      <c r="Y135" s="607"/>
+      <c r="W135" s="621"/>
+      <c r="X135" s="621"/>
+      <c r="Y135" s="622"/>
       <c r="Z135" s="60"/>
       <c r="AA135" s="60"/>
       <c r="AB135" s="68" t="s">
@@ -33429,24 +33432,24 @@
       <c r="E137" s="38"/>
       <c r="F137" s="38"/>
       <c r="G137" s="39"/>
-      <c r="H137" s="608" t="s">
+      <c r="H137" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="I137" s="609"/>
-      <c r="J137" s="609"/>
-      <c r="K137" s="610"/>
-      <c r="L137" s="609" t="s">
+      <c r="I137" s="612"/>
+      <c r="J137" s="612"/>
+      <c r="K137" s="613"/>
+      <c r="L137" s="612" t="s">
         <v>34</v>
       </c>
-      <c r="M137" s="609"/>
-      <c r="N137" s="609"/>
-      <c r="O137" s="610"/>
-      <c r="P137" s="608" t="s">
+      <c r="M137" s="612"/>
+      <c r="N137" s="612"/>
+      <c r="O137" s="613"/>
+      <c r="P137" s="611" t="s">
         <v>34</v>
       </c>
-      <c r="Q137" s="609"/>
-      <c r="R137" s="609"/>
-      <c r="S137" s="610"/>
+      <c r="Q137" s="612"/>
+      <c r="R137" s="612"/>
+      <c r="S137" s="613"/>
       <c r="T137" s="614" t="s">
         <v>68</v>
       </c>
@@ -35684,7 +35687,7 @@
         <v>558</v>
       </c>
       <c r="G160" s="24" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H160" s="22">
         <v>1</v>
@@ -35781,7 +35784,7 @@
         <v>558</v>
       </c>
       <c r="G161" s="30" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H161" s="40">
         <v>1</v>
@@ -35878,7 +35881,7 @@
         <v>558</v>
       </c>
       <c r="G162" s="24" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H162" s="22">
         <v>1</v>
@@ -35975,7 +35978,7 @@
         <v>558</v>
       </c>
       <c r="G163" s="30" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H163" s="40">
         <v>1</v>
@@ -36063,7 +36066,7 @@
         <v>R-SH_Det_ELC_HPN2-G</v>
       </c>
       <c r="D164" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E164" s="27" t="s">
         <v>148</v>
@@ -36072,7 +36075,7 @@
         <v>558</v>
       </c>
       <c r="G164" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H164" s="246">
         <v>1</v>
@@ -36169,7 +36172,7 @@
         <v>660</v>
       </c>
       <c r="G165" s="88" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H165" s="19">
         <v>1</v>
@@ -36278,7 +36281,7 @@
         <v>660</v>
       </c>
       <c r="G166" s="24" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H166" s="22">
         <v>1</v>
@@ -36387,7 +36390,7 @@
         <v>660</v>
       </c>
       <c r="G167" s="30" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H167" s="40">
         <v>1</v>
@@ -36496,7 +36499,7 @@
         <v>660</v>
       </c>
       <c r="G168" s="24" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H168" s="22">
         <v>1</v>
@@ -36605,7 +36608,7 @@
         <v>660</v>
       </c>
       <c r="G169" s="30" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H169" s="40">
         <v>1</v>
@@ -36705,7 +36708,7 @@
         <v>R-SW_Det_ELC_HPN1-G</v>
       </c>
       <c r="D170" s="27" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E170" s="27" t="s">
         <v>148</v>
@@ -36714,7 +36717,7 @@
         <v>660</v>
       </c>
       <c r="G170" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H170" s="246">
         <v>1</v>
@@ -36814,7 +36817,7 @@
         <v>R-SW_Det_ELC_HPN2-AB</v>
       </c>
       <c r="D171" s="88" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E171" s="88" t="s">
         <v>550</v>
@@ -36823,7 +36826,7 @@
         <v>660</v>
       </c>
       <c r="G171" s="88" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H171" s="19">
         <v>1</v>
@@ -36928,7 +36931,7 @@
         <v>R-SW_Det_ELC_HPN2-C</v>
       </c>
       <c r="D172" s="24" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E172" s="24" t="s">
         <v>550</v>
@@ -36937,7 +36940,7 @@
         <v>660</v>
       </c>
       <c r="G172" s="24" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H172" s="22">
         <v>1</v>
@@ -37042,7 +37045,7 @@
         <v>R-SW_Det_ELC_HPN2-D</v>
       </c>
       <c r="D173" s="30" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E173" s="30" t="s">
         <v>550</v>
@@ -37051,7 +37054,7 @@
         <v>660</v>
       </c>
       <c r="G173" s="30" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H173" s="40">
         <v>1</v>
@@ -37156,7 +37159,7 @@
         <v>R-SW_Det_ELC_HPN2-E</v>
       </c>
       <c r="D174" s="24" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E174" s="24" t="s">
         <v>550</v>
@@ -37165,7 +37168,7 @@
         <v>660</v>
       </c>
       <c r="G174" s="24" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H174" s="22">
         <v>1</v>
@@ -37270,7 +37273,7 @@
         <v>R-SW_Det_ELC_HPN2-F</v>
       </c>
       <c r="D175" s="30" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E175" s="30" t="s">
         <v>550</v>
@@ -37279,7 +37282,7 @@
         <v>660</v>
       </c>
       <c r="G175" s="30" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H175" s="40">
         <v>1</v>
@@ -37384,7 +37387,7 @@
         <v>R-SW_Det_ELC_HPN2-G</v>
       </c>
       <c r="D176" s="27" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E176" s="27" t="s">
         <v>550</v>
@@ -37393,7 +37396,7 @@
         <v>660</v>
       </c>
       <c r="G176" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H176" s="246">
         <v>1</v>
@@ -37498,7 +37501,7 @@
         <v>R-SH_Det_ELC_HPN3-AB</v>
       </c>
       <c r="D177" s="88" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E177" s="88" t="s">
         <v>148</v>
@@ -37596,7 +37599,7 @@
         <v>R-SH_Det_ELC_HPN3-C</v>
       </c>
       <c r="D178" s="24" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E178" s="24" t="s">
         <v>148</v>
@@ -37605,7 +37608,7 @@
         <v>558</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H178" s="22">
         <v>1.0999999999999999</v>
@@ -37691,7 +37694,7 @@
         <v>R-SH_Det_ELC_HPN3-D</v>
       </c>
       <c r="D179" s="30" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E179" s="30" t="s">
         <v>148</v>
@@ -37700,7 +37703,7 @@
         <v>558</v>
       </c>
       <c r="G179" s="30" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H179" s="40">
         <v>1.0999999999999999</v>
@@ -37786,7 +37789,7 @@
         <v>R-SH_Det_ELC_HPN3-E</v>
       </c>
       <c r="D180" s="24" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E180" s="24" t="s">
         <v>148</v>
@@ -37795,7 +37798,7 @@
         <v>558</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H180" s="22">
         <v>1.0999999999999999</v>
@@ -37881,7 +37884,7 @@
         <v>R-SH_Det_ELC_HPN3-F</v>
       </c>
       <c r="D181" s="30" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E181" s="30" t="s">
         <v>148</v>
@@ -37890,7 +37893,7 @@
         <v>558</v>
       </c>
       <c r="G181" s="30" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H181" s="40">
         <v>1.0999999999999999</v>
@@ -37976,7 +37979,7 @@
         <v>R-SH_Det_ELC_HPN3-G</v>
       </c>
       <c r="D182" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E182" s="27" t="s">
         <v>148</v>
@@ -37985,7 +37988,7 @@
         <v>558</v>
       </c>
       <c r="G182" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H182" s="246">
         <v>1.0999999999999999</v>
@@ -38071,7 +38074,7 @@
         <v>R-HC_Det_ELC_HPN2-AB</v>
       </c>
       <c r="D183" s="88" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E183" s="88" t="s">
         <v>148</v>
@@ -38080,7 +38083,7 @@
         <v>558</v>
       </c>
       <c r="G183" s="88" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H183" s="19">
         <v>1.0999999999999999</v>
@@ -38177,7 +38180,7 @@
         <v>R-HC_Det_ELC_HPN2-C</v>
       </c>
       <c r="D184" s="24" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E184" s="24" t="s">
         <v>148</v>
@@ -38186,7 +38189,7 @@
         <v>558</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H184" s="22">
         <v>1.0999999999999999</v>
@@ -38280,7 +38283,7 @@
         <v>R-HC_Det_ELC_HPN2-D</v>
       </c>
       <c r="D185" s="30" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E185" s="30" t="s">
         <v>148</v>
@@ -38289,7 +38292,7 @@
         <v>558</v>
       </c>
       <c r="G185" s="30" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H185" s="40">
         <v>1.0999999999999999</v>
@@ -38383,7 +38386,7 @@
         <v>R-HC_Det_ELC_HPN2-E</v>
       </c>
       <c r="D186" s="24" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E186" s="24" t="s">
         <v>148</v>
@@ -38392,7 +38395,7 @@
         <v>558</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H186" s="22">
         <v>1.0999999999999999</v>
@@ -38486,7 +38489,7 @@
         <v>R-HC_Det_ELC_HPN2-F</v>
       </c>
       <c r="D187" s="30" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E187" s="30" t="s">
         <v>148</v>
@@ -38495,7 +38498,7 @@
         <v>558</v>
       </c>
       <c r="G187" s="30" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H187" s="40">
         <v>1.0999999999999999</v>
@@ -38589,7 +38592,7 @@
         <v>R-HC_Det_ELC_HPN2-G</v>
       </c>
       <c r="D188" s="27" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E188" s="27" t="s">
         <v>148</v>
@@ -38598,7 +38601,7 @@
         <v>558</v>
       </c>
       <c r="G188" s="27" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H188" s="246">
         <v>1.0999999999999999</v>
@@ -39759,10 +39762,10 @@
       <c r="AC217" s="124"/>
       <c r="AE217" s="3"/>
       <c r="AG217" s="124" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="AH217" s="124" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="218" spans="10:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -39777,18 +39780,18 @@
         <f>V221-(V223-V221)</f>
         <v>2250</v>
       </c>
-      <c r="Z218" s="617" t="s">
+      <c r="Z218" s="605" t="s">
+        <v>809</v>
+      </c>
+      <c r="AA218" s="606"/>
+      <c r="AB218" s="606"/>
+      <c r="AC218" s="607"/>
+      <c r="AD218" s="124" t="s">
         <v>810</v>
-      </c>
-      <c r="AA218" s="618"/>
-      <c r="AB218" s="618"/>
-      <c r="AC218" s="619"/>
-      <c r="AD218" s="124" t="s">
-        <v>811</v>
       </c>
       <c r="AE218" s="124"/>
       <c r="AF218" s="124" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="AG218" s="124" t="s">
         <v>55</v>
@@ -39804,14 +39807,14 @@
       </c>
     </row>
     <row r="219" spans="10:36" x14ac:dyDescent="0.2">
-      <c r="L219" s="621" t="s">
+      <c r="L219" s="609" t="s">
         <v>504</v>
       </c>
-      <c r="M219" s="621"/>
-      <c r="N219" s="621"/>
-      <c r="O219" s="621"/>
-      <c r="P219" s="621"/>
-      <c r="Q219" s="621"/>
+      <c r="M219" s="609"/>
+      <c r="N219" s="609"/>
+      <c r="O219" s="609"/>
+      <c r="P219" s="609"/>
+      <c r="Q219" s="609"/>
       <c r="T219" s="3">
         <v>15</v>
       </c>
@@ -39825,28 +39828,28 @@
       <c r="X219" s="4"/>
       <c r="Y219" s="4"/>
       <c r="Z219" s="546" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="AA219" s="547" t="s">
+        <v>796</v>
+      </c>
+      <c r="AB219" s="547" t="s">
         <v>797</v>
       </c>
-      <c r="AB219" s="547" t="s">
-        <v>798</v>
-      </c>
       <c r="AC219" s="548" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="AD219" s="124" t="s">
+        <v>811</v>
+      </c>
+      <c r="AF219" s="608" t="s">
         <v>812</v>
       </c>
-      <c r="AF219" s="620" t="s">
-        <v>813</v>
-      </c>
-      <c r="AG219" s="620"/>
+      <c r="AG219" s="608"/>
     </row>
     <row r="220" spans="10:36" x14ac:dyDescent="0.2">
       <c r="L220" s="124" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M220" s="3" t="s">
         <v>512</v>
@@ -39876,10 +39879,10 @@
       <c r="X220" s="4"/>
       <c r="Y220" s="4"/>
       <c r="Z220" s="537" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="AA220" s="538" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="AB220" s="2">
         <v>35</v>
@@ -39944,7 +39947,7 @@
         <v>483</v>
       </c>
       <c r="AA221" s="541" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="AB221" s="542">
         <v>40</v>
@@ -40008,10 +40011,10 @@
       <c r="X222" s="4"/>
       <c r="Y222" s="4"/>
       <c r="Z222" s="537" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="AA222" s="538" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="AB222" s="2">
         <v>45</v>
@@ -40075,10 +40078,10 @@
       <c r="X223" s="4"/>
       <c r="Y223" s="4"/>
       <c r="Z223" s="540" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="AA223" s="541" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="AB223" s="542">
         <v>50</v>
@@ -40140,13 +40143,13 @@
         <v>2795</v>
       </c>
       <c r="Z224" s="544" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="AA224" s="545" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="AB224" s="545" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="AC224" s="555">
         <v>2.35</v>
@@ -40226,14 +40229,14 @@
       <c r="I230" s="4"/>
       <c r="J230" s="4"/>
       <c r="K230" s="4"/>
-      <c r="AB230" s="622" t="s">
-        <v>819</v>
-      </c>
-      <c r="AC230" s="622"/>
-      <c r="AD230" s="622"/>
-      <c r="AE230" s="622"/>
+      <c r="AB230" s="610" t="s">
+        <v>818</v>
+      </c>
+      <c r="AC230" s="610"/>
+      <c r="AD230" s="610"/>
+      <c r="AE230" s="610"/>
       <c r="AG230" s="602" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="AH230" s="603"/>
       <c r="AI230" s="604"/>
@@ -40294,7 +40297,7 @@
       <c r="Z232" s="4"/>
       <c r="AA232" s="4"/>
       <c r="AB232" s="124" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="AC232" s="550">
         <v>1.5</v>
@@ -40306,7 +40309,7 @@
         <v>1.95</v>
       </c>
       <c r="AF232" s="124" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="AG232" s="556">
         <v>0</v>
@@ -40682,7 +40685,7 @@
       <c r="AD239" s="4"/>
       <c r="AF239" s="4"/>
       <c r="AG239" s="124" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="AH239" s="4"/>
       <c r="AI239" s="4"/>
@@ -40714,7 +40717,7 @@
       <c r="AD240" s="4"/>
       <c r="AF240" s="4"/>
       <c r="AG240" s="602" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="AH240" s="603"/>
       <c r="AI240" s="604"/>
@@ -40962,28 +40965,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="AJ230:AL230"/>
-    <mergeCell ref="Z218:AC218"/>
-    <mergeCell ref="AF219:AG219"/>
-    <mergeCell ref="L219:Q219"/>
-    <mergeCell ref="AB230:AE230"/>
-    <mergeCell ref="AG230:AI230"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L137:O137"/>
-    <mergeCell ref="P137:S137"/>
-    <mergeCell ref="T137:U137"/>
-    <mergeCell ref="V137:Y137"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="L135:O135"/>
-    <mergeCell ref="P135:S135"/>
-    <mergeCell ref="T135:U135"/>
-    <mergeCell ref="V135:Y135"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="L64:O64"/>
-    <mergeCell ref="P64:S64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="V64:Y64"/>
     <mergeCell ref="AG240:AI240"/>
     <mergeCell ref="AJ240:AL240"/>
     <mergeCell ref="V4:Y4"/>
@@ -41000,6 +40981,28 @@
     <mergeCell ref="L62:O62"/>
     <mergeCell ref="P62:S62"/>
     <mergeCell ref="T62:U62"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="L64:O64"/>
+    <mergeCell ref="P64:S64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="V64:Y64"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="L135:O135"/>
+    <mergeCell ref="P135:S135"/>
+    <mergeCell ref="T135:U135"/>
+    <mergeCell ref="V135:Y135"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L137:O137"/>
+    <mergeCell ref="P137:S137"/>
+    <mergeCell ref="T137:U137"/>
+    <mergeCell ref="V137:Y137"/>
+    <mergeCell ref="AJ230:AL230"/>
+    <mergeCell ref="Z218:AC218"/>
+    <mergeCell ref="AF219:AG219"/>
+    <mergeCell ref="L219:Q219"/>
+    <mergeCell ref="AB230:AE230"/>
+    <mergeCell ref="AG230:AI230"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -41143,12 +41146,12 @@
       <c r="I5" s="121"/>
       <c r="J5" s="121"/>
       <c r="K5" s="121"/>
-      <c r="L5" s="605" t="s">
+      <c r="L5" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="606"/>
-      <c r="N5" s="606"/>
-      <c r="O5" s="607"/>
+      <c r="M5" s="621"/>
+      <c r="N5" s="621"/>
+      <c r="O5" s="622"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -42070,12 +42073,12 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="605" t="s">
+      <c r="L33" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="606"/>
-      <c r="N33" s="606"/>
-      <c r="O33" s="607"/>
+      <c r="M33" s="621"/>
+      <c r="N33" s="621"/>
+      <c r="O33" s="622"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
@@ -42426,16 +42429,16 @@
       <c r="G4" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="611" t="s">
+      <c r="H4" s="617" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="612"/>
-      <c r="J4" s="613"/>
-      <c r="K4" s="605" t="s">
+      <c r="I4" s="618"/>
+      <c r="J4" s="619"/>
+      <c r="K4" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="606"/>
-      <c r="M4" s="607"/>
+      <c r="L4" s="621"/>
+      <c r="M4" s="622"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -42461,16 +42464,16 @@
       <c r="G5" s="375" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="623" t="s">
+      <c r="H5" s="626" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="624"/>
-      <c r="J5" s="625"/>
-      <c r="K5" s="623" t="s">
+      <c r="I5" s="627"/>
+      <c r="J5" s="628"/>
+      <c r="K5" s="626" t="s">
         <v>292</v>
       </c>
-      <c r="L5" s="624"/>
-      <c r="M5" s="625"/>
+      <c r="L5" s="627"/>
+      <c r="M5" s="628"/>
       <c r="N5" s="376" t="s">
         <v>92</v>
       </c>
@@ -42487,23 +42490,23 @@
         <v>210</v>
       </c>
       <c r="AA5" s="201"/>
-      <c r="AB5" s="626" t="s">
+      <c r="AB5" s="623" t="s">
         <v>541</v>
       </c>
-      <c r="AC5" s="626"/>
+      <c r="AC5" s="623"/>
       <c r="AD5" s="378"/>
-      <c r="AE5" s="627" t="s">
+      <c r="AE5" s="624" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="627"/>
-      <c r="AG5" s="627" t="s">
+      <c r="AF5" s="624"/>
+      <c r="AG5" s="624" t="s">
         <v>542</v>
       </c>
-      <c r="AH5" s="627"/>
-      <c r="AI5" s="628" t="s">
+      <c r="AH5" s="624"/>
+      <c r="AI5" s="625" t="s">
         <v>543</v>
       </c>
-      <c r="AJ5" s="628"/>
+      <c r="AJ5" s="625"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="422" t="str">
@@ -43241,12 +43244,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="605" t="s">
+      <c r="L27" s="620" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="606"/>
-      <c r="N27" s="606"/>
-      <c r="O27" s="607"/>
+      <c r="M27" s="621"/>
+      <c r="N27" s="621"/>
+      <c r="O27" s="622"/>
       <c r="T27" s="203"/>
       <c r="U27" s="203"/>
     </row>
@@ -43254,12 +43257,12 @@
       <c r="J28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L28" s="608" t="s">
+      <c r="L28" s="611" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="609"/>
-      <c r="N28" s="609"/>
-      <c r="O28" s="610"/>
+      <c r="M28" s="612"/>
+      <c r="N28" s="612"/>
+      <c r="O28" s="613"/>
       <c r="T28" s="203"/>
       <c r="U28" s="203"/>
     </row>
@@ -44649,16 +44652,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -45089,103 +45092,103 @@
       <c r="C4" s="273" t="s">
         <v>301</v>
       </c>
-      <c r="D4" s="629" t="s">
+      <c r="D4" s="630" t="s">
         <v>302</v>
       </c>
-      <c r="E4" s="630"/>
-      <c r="F4" s="630"/>
-      <c r="G4" s="630"/>
+      <c r="E4" s="629"/>
+      <c r="F4" s="629"/>
+      <c r="G4" s="629"/>
       <c r="H4" s="631"/>
-      <c r="I4" s="630" t="s">
+      <c r="I4" s="629" t="s">
         <v>303</v>
       </c>
-      <c r="J4" s="630"/>
-      <c r="K4" s="630"/>
-      <c r="L4" s="630"/>
+      <c r="J4" s="629"/>
+      <c r="K4" s="629"/>
+      <c r="L4" s="629"/>
       <c r="M4" s="631"/>
-      <c r="N4" s="630" t="s">
+      <c r="N4" s="629" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="630"/>
-      <c r="P4" s="630"/>
-      <c r="Q4" s="630"/>
+      <c r="O4" s="629"/>
+      <c r="P4" s="629"/>
+      <c r="Q4" s="629"/>
       <c r="R4" s="631"/>
-      <c r="S4" s="630" t="s">
+      <c r="S4" s="629" t="s">
         <v>305</v>
       </c>
-      <c r="T4" s="630"/>
-      <c r="U4" s="630"/>
-      <c r="V4" s="630"/>
+      <c r="T4" s="629"/>
+      <c r="U4" s="629"/>
+      <c r="V4" s="629"/>
       <c r="W4" s="631"/>
-      <c r="X4" s="630" t="s">
+      <c r="X4" s="629" t="s">
         <v>306</v>
       </c>
-      <c r="Y4" s="630"/>
-      <c r="Z4" s="630"/>
-      <c r="AA4" s="630"/>
+      <c r="Y4" s="629"/>
+      <c r="Z4" s="629"/>
+      <c r="AA4" s="629"/>
       <c r="AB4" s="631"/>
-      <c r="AC4" s="630" t="s">
+      <c r="AC4" s="629" t="s">
         <v>307</v>
       </c>
-      <c r="AD4" s="630"/>
-      <c r="AE4" s="630"/>
-      <c r="AF4" s="630"/>
+      <c r="AD4" s="629"/>
+      <c r="AE4" s="629"/>
+      <c r="AF4" s="629"/>
       <c r="AG4" s="631"/>
-      <c r="AH4" s="630" t="s">
+      <c r="AH4" s="629" t="s">
         <v>308</v>
       </c>
-      <c r="AI4" s="630"/>
-      <c r="AJ4" s="630"/>
-      <c r="AK4" s="630"/>
+      <c r="AI4" s="629"/>
+      <c r="AJ4" s="629"/>
+      <c r="AK4" s="629"/>
       <c r="AL4" s="631"/>
-      <c r="AM4" s="630" t="s">
+      <c r="AM4" s="629" t="s">
         <v>309</v>
       </c>
-      <c r="AN4" s="630"/>
-      <c r="AO4" s="630"/>
-      <c r="AP4" s="630"/>
+      <c r="AN4" s="629"/>
+      <c r="AO4" s="629"/>
+      <c r="AP4" s="629"/>
       <c r="AQ4" s="631"/>
-      <c r="AR4" s="630" t="s">
+      <c r="AR4" s="629" t="s">
         <v>310</v>
       </c>
-      <c r="AS4" s="630"/>
-      <c r="AT4" s="630"/>
-      <c r="AU4" s="630"/>
+      <c r="AS4" s="629"/>
+      <c r="AT4" s="629"/>
+      <c r="AU4" s="629"/>
       <c r="AV4" s="631"/>
-      <c r="AW4" s="630" t="s">
+      <c r="AW4" s="629" t="s">
         <v>311</v>
       </c>
-      <c r="AX4" s="630"/>
-      <c r="AY4" s="630"/>
-      <c r="AZ4" s="630"/>
-      <c r="BA4" s="630"/>
-      <c r="BB4" s="629" t="s">
+      <c r="AX4" s="629"/>
+      <c r="AY4" s="629"/>
+      <c r="AZ4" s="629"/>
+      <c r="BA4" s="629"/>
+      <c r="BB4" s="630" t="s">
         <v>312</v>
       </c>
-      <c r="BC4" s="630"/>
-      <c r="BD4" s="630"/>
-      <c r="BE4" s="630"/>
+      <c r="BC4" s="629"/>
+      <c r="BD4" s="629"/>
+      <c r="BE4" s="629"/>
       <c r="BF4" s="631"/>
-      <c r="BG4" s="630" t="s">
+      <c r="BG4" s="629" t="s">
         <v>313</v>
       </c>
-      <c r="BH4" s="630"/>
-      <c r="BI4" s="630"/>
-      <c r="BJ4" s="630"/>
-      <c r="BK4" s="630"/>
-      <c r="BL4" s="629" t="s">
+      <c r="BH4" s="629"/>
+      <c r="BI4" s="629"/>
+      <c r="BJ4" s="629"/>
+      <c r="BK4" s="629"/>
+      <c r="BL4" s="630" t="s">
         <v>314</v>
       </c>
-      <c r="BM4" s="630"/>
-      <c r="BN4" s="630"/>
-      <c r="BO4" s="630"/>
-      <c r="BP4" s="630"/>
-      <c r="BQ4" s="629" t="s">
+      <c r="BM4" s="629"/>
+      <c r="BN4" s="629"/>
+      <c r="BO4" s="629"/>
+      <c r="BP4" s="629"/>
+      <c r="BQ4" s="630" t="s">
         <v>315</v>
       </c>
-      <c r="BR4" s="630"/>
-      <c r="BS4" s="630"/>
-      <c r="BT4" s="630"/>
+      <c r="BR4" s="629"/>
+      <c r="BS4" s="629"/>
+      <c r="BT4" s="629"/>
       <c r="BU4" s="631"/>
       <c r="BV4" s="274" t="s">
         <v>316</v>
@@ -58779,6 +58782,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -58791,11 +58799,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -58818,23 +58821,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="636" t="s">
+      <c r="A1" s="638" t="s">
         <v>585</v>
       </c>
-      <c r="B1" s="638" t="s">
+      <c r="B1" s="640" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="639"/>
-      <c r="D1" s="639"/>
-      <c r="E1" s="639"/>
-      <c r="F1" s="640"/>
-      <c r="G1" s="638" t="s">
+      <c r="C1" s="641"/>
+      <c r="D1" s="641"/>
+      <c r="E1" s="641"/>
+      <c r="F1" s="642"/>
+      <c r="G1" s="640" t="s">
         <v>587</v>
       </c>
-      <c r="H1" s="639"/>
-      <c r="I1" s="639"/>
-      <c r="J1" s="639"/>
-      <c r="K1" s="640"/>
+      <c r="H1" s="641"/>
+      <c r="I1" s="641"/>
+      <c r="J1" s="641"/>
+      <c r="K1" s="642"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -58844,7 +58847,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="637"/>
+      <c r="A2" s="639"/>
       <c r="B2" s="443" t="s">
         <v>254</v>
       </c>
@@ -60337,11 +60340,11 @@
       <c r="Y48" t="s">
         <v>636</v>
       </c>
-      <c r="Z48" s="641" t="s">
+      <c r="Z48" s="636" t="s">
         <v>574</v>
       </c>
-      <c r="AA48" s="642"/>
-      <c r="AB48" s="642"/>
+      <c r="AA48" s="637"/>
+      <c r="AB48" s="637"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -60558,11 +60561,11 @@
       <c r="Y53" t="s">
         <v>638</v>
       </c>
-      <c r="Z53" s="641" t="s">
+      <c r="Z53" s="636" t="s">
         <v>573</v>
       </c>
-      <c r="AA53" s="642"/>
-      <c r="AB53" s="642"/>
+      <c r="AA53" s="637"/>
+      <c r="AB53" s="637"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -60764,11 +60767,11 @@
       <c r="Y59" t="s">
         <v>639</v>
       </c>
-      <c r="Z59" s="641" t="s">
+      <c r="Z59" s="636" t="s">
         <v>640</v>
       </c>
-      <c r="AA59" s="642"/>
-      <c r="AB59" s="642"/>
+      <c r="AA59" s="637"/>
+      <c r="AB59" s="637"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="463" t="str">
@@ -61605,17 +61608,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gas Apartment HP COP below 1
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_RSD_NewTechs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18652DE8-F8DE-4BFB-82ED-82AACE9F2B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64930D97-B1A4-474A-8E20-F918DE4024BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2CC7CA6E-3559-4BC7-B5C1-253B80EF5435}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2CC7CA6E-3559-4BC7-B5C1-253B80EF5435}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="62" r:id="rId1"/>
@@ -13959,6 +13959,42 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -13977,40 +14013,13 @@
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -14022,19 +14031,10 @@
     <xf numFmtId="0" fontId="53" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14052,12 +14052,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14072,6 +14066,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -20990,8 +20990,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AS251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V135" sqref="V135:Y135"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21166,34 +21166,34 @@
       <c r="G4" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="617" t="s">
+      <c r="H4" s="611" t="s">
         <v>258</v>
       </c>
-      <c r="I4" s="618"/>
-      <c r="J4" s="618"/>
-      <c r="K4" s="619"/>
-      <c r="L4" s="617" t="s">
+      <c r="I4" s="612"/>
+      <c r="J4" s="612"/>
+      <c r="K4" s="613"/>
+      <c r="L4" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="618"/>
-      <c r="N4" s="618"/>
-      <c r="O4" s="619"/>
-      <c r="P4" s="617" t="s">
+      <c r="M4" s="612"/>
+      <c r="N4" s="612"/>
+      <c r="O4" s="613"/>
+      <c r="P4" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="618"/>
-      <c r="R4" s="618"/>
-      <c r="S4" s="619"/>
-      <c r="T4" s="617" t="s">
+      <c r="Q4" s="612"/>
+      <c r="R4" s="612"/>
+      <c r="S4" s="613"/>
+      <c r="T4" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U4" s="619"/>
-      <c r="V4" s="620" t="s">
+      <c r="U4" s="613"/>
+      <c r="V4" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="621"/>
-      <c r="X4" s="621"/>
-      <c r="Y4" s="622"/>
+      <c r="W4" s="606"/>
+      <c r="X4" s="606"/>
+      <c r="Y4" s="607"/>
       <c r="Z4" s="60"/>
       <c r="AA4" s="60"/>
       <c r="AB4" s="68" t="s">
@@ -21296,34 +21296,34 @@
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39"/>
-      <c r="H6" s="611" t="s">
+      <c r="H6" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="612"/>
-      <c r="J6" s="612"/>
-      <c r="K6" s="613"/>
-      <c r="L6" s="612" t="s">
+      <c r="I6" s="609"/>
+      <c r="J6" s="609"/>
+      <c r="K6" s="610"/>
+      <c r="L6" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="612"/>
-      <c r="N6" s="612"/>
-      <c r="O6" s="613"/>
-      <c r="P6" s="611" t="s">
+      <c r="M6" s="609"/>
+      <c r="N6" s="609"/>
+      <c r="O6" s="610"/>
+      <c r="P6" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="612"/>
-      <c r="R6" s="612"/>
-      <c r="S6" s="613"/>
-      <c r="T6" s="611" t="s">
+      <c r="Q6" s="609"/>
+      <c r="R6" s="609"/>
+      <c r="S6" s="610"/>
+      <c r="T6" s="608" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="613"/>
-      <c r="V6" s="611" t="s">
+      <c r="U6" s="610"/>
+      <c r="V6" s="608" t="s">
         <v>503</v>
       </c>
-      <c r="W6" s="612"/>
-      <c r="X6" s="612"/>
-      <c r="Y6" s="613"/>
+      <c r="W6" s="609"/>
+      <c r="X6" s="609"/>
+      <c r="Y6" s="610"/>
       <c r="Z6" s="520" t="s">
         <v>515</v>
       </c>
@@ -26518,34 +26518,34 @@
       <c r="G62" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H62" s="617" t="s">
+      <c r="H62" s="611" t="s">
         <v>82</v>
       </c>
-      <c r="I62" s="618"/>
-      <c r="J62" s="618"/>
-      <c r="K62" s="619"/>
-      <c r="L62" s="617" t="s">
+      <c r="I62" s="612"/>
+      <c r="J62" s="612"/>
+      <c r="K62" s="613"/>
+      <c r="L62" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M62" s="618"/>
-      <c r="N62" s="618"/>
-      <c r="O62" s="619"/>
-      <c r="P62" s="617" t="s">
+      <c r="M62" s="612"/>
+      <c r="N62" s="612"/>
+      <c r="O62" s="613"/>
+      <c r="P62" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q62" s="618"/>
-      <c r="R62" s="618"/>
-      <c r="S62" s="619"/>
-      <c r="T62" s="617" t="s">
+      <c r="Q62" s="612"/>
+      <c r="R62" s="612"/>
+      <c r="S62" s="613"/>
+      <c r="T62" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U62" s="619"/>
-      <c r="V62" s="620" t="s">
+      <c r="U62" s="613"/>
+      <c r="V62" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W62" s="621"/>
-      <c r="X62" s="621"/>
-      <c r="Y62" s="622"/>
+      <c r="W62" s="606"/>
+      <c r="X62" s="606"/>
+      <c r="Y62" s="607"/>
       <c r="Z62" s="60"/>
       <c r="AA62" s="60"/>
       <c r="AB62" s="68" t="s">
@@ -26648,24 +26648,24 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="39"/>
-      <c r="H64" s="611" t="s">
+      <c r="H64" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I64" s="612"/>
-      <c r="J64" s="612"/>
-      <c r="K64" s="613"/>
-      <c r="L64" s="612" t="s">
+      <c r="I64" s="609"/>
+      <c r="J64" s="609"/>
+      <c r="K64" s="610"/>
+      <c r="L64" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M64" s="612"/>
-      <c r="N64" s="612"/>
-      <c r="O64" s="613"/>
-      <c r="P64" s="611" t="s">
+      <c r="M64" s="609"/>
+      <c r="N64" s="609"/>
+      <c r="O64" s="610"/>
+      <c r="P64" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q64" s="612"/>
-      <c r="R64" s="612"/>
-      <c r="S64" s="613"/>
+      <c r="Q64" s="609"/>
+      <c r="R64" s="609"/>
+      <c r="S64" s="610"/>
       <c r="T64" s="614" t="s">
         <v>68</v>
       </c>
@@ -33290,34 +33290,34 @@
       <c r="G135" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H135" s="617" t="s">
+      <c r="H135" s="611" t="s">
         <v>82</v>
       </c>
-      <c r="I135" s="618"/>
-      <c r="J135" s="618"/>
-      <c r="K135" s="619"/>
-      <c r="L135" s="617" t="s">
+      <c r="I135" s="612"/>
+      <c r="J135" s="612"/>
+      <c r="K135" s="613"/>
+      <c r="L135" s="611" t="s">
         <v>83</v>
       </c>
-      <c r="M135" s="618"/>
-      <c r="N135" s="618"/>
-      <c r="O135" s="619"/>
-      <c r="P135" s="617" t="s">
+      <c r="M135" s="612"/>
+      <c r="N135" s="612"/>
+      <c r="O135" s="613"/>
+      <c r="P135" s="611" t="s">
         <v>84</v>
       </c>
-      <c r="Q135" s="618"/>
-      <c r="R135" s="618"/>
-      <c r="S135" s="619"/>
-      <c r="T135" s="617" t="s">
+      <c r="Q135" s="612"/>
+      <c r="R135" s="612"/>
+      <c r="S135" s="613"/>
+      <c r="T135" s="611" t="s">
         <v>85</v>
       </c>
-      <c r="U135" s="619"/>
-      <c r="V135" s="620" t="s">
+      <c r="U135" s="613"/>
+      <c r="V135" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="W135" s="621"/>
-      <c r="X135" s="621"/>
-      <c r="Y135" s="622"/>
+      <c r="W135" s="606"/>
+      <c r="X135" s="606"/>
+      <c r="Y135" s="607"/>
       <c r="Z135" s="60"/>
       <c r="AA135" s="60"/>
       <c r="AB135" s="68" t="s">
@@ -33432,24 +33432,24 @@
       <c r="E137" s="38"/>
       <c r="F137" s="38"/>
       <c r="G137" s="39"/>
-      <c r="H137" s="611" t="s">
+      <c r="H137" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="I137" s="612"/>
-      <c r="J137" s="612"/>
-      <c r="K137" s="613"/>
-      <c r="L137" s="612" t="s">
+      <c r="I137" s="609"/>
+      <c r="J137" s="609"/>
+      <c r="K137" s="610"/>
+      <c r="L137" s="609" t="s">
         <v>34</v>
       </c>
-      <c r="M137" s="612"/>
-      <c r="N137" s="612"/>
-      <c r="O137" s="613"/>
-      <c r="P137" s="611" t="s">
+      <c r="M137" s="609"/>
+      <c r="N137" s="609"/>
+      <c r="O137" s="610"/>
+      <c r="P137" s="608" t="s">
         <v>34</v>
       </c>
-      <c r="Q137" s="612"/>
-      <c r="R137" s="612"/>
-      <c r="S137" s="613"/>
+      <c r="Q137" s="609"/>
+      <c r="R137" s="609"/>
+      <c r="S137" s="610"/>
       <c r="T137" s="614" t="s">
         <v>68</v>
       </c>
@@ -39780,12 +39780,12 @@
         <f>V221-(V223-V221)</f>
         <v>2250</v>
       </c>
-      <c r="Z218" s="605" t="s">
+      <c r="Z218" s="617" t="s">
         <v>809</v>
       </c>
-      <c r="AA218" s="606"/>
-      <c r="AB218" s="606"/>
-      <c r="AC218" s="607"/>
+      <c r="AA218" s="618"/>
+      <c r="AB218" s="618"/>
+      <c r="AC218" s="619"/>
       <c r="AD218" s="124" t="s">
         <v>810</v>
       </c>
@@ -39807,14 +39807,14 @@
       </c>
     </row>
     <row r="219" spans="10:36" x14ac:dyDescent="0.2">
-      <c r="L219" s="609" t="s">
+      <c r="L219" s="621" t="s">
         <v>504</v>
       </c>
-      <c r="M219" s="609"/>
-      <c r="N219" s="609"/>
-      <c r="O219" s="609"/>
-      <c r="P219" s="609"/>
-      <c r="Q219" s="609"/>
+      <c r="M219" s="621"/>
+      <c r="N219" s="621"/>
+      <c r="O219" s="621"/>
+      <c r="P219" s="621"/>
+      <c r="Q219" s="621"/>
       <c r="T219" s="3">
         <v>15</v>
       </c>
@@ -39842,10 +39842,10 @@
       <c r="AD219" s="124" t="s">
         <v>811</v>
       </c>
-      <c r="AF219" s="608" t="s">
+      <c r="AF219" s="620" t="s">
         <v>812</v>
       </c>
-      <c r="AG219" s="608"/>
+      <c r="AG219" s="620"/>
     </row>
     <row r="220" spans="10:36" x14ac:dyDescent="0.2">
       <c r="L220" s="124" t="s">
@@ -40229,12 +40229,12 @@
       <c r="I230" s="4"/>
       <c r="J230" s="4"/>
       <c r="K230" s="4"/>
-      <c r="AB230" s="610" t="s">
+      <c r="AB230" s="622" t="s">
         <v>818</v>
       </c>
-      <c r="AC230" s="610"/>
-      <c r="AD230" s="610"/>
-      <c r="AE230" s="610"/>
+      <c r="AC230" s="622"/>
+      <c r="AD230" s="622"/>
+      <c r="AE230" s="622"/>
       <c r="AG230" s="602" t="s">
         <v>815</v>
       </c>
@@ -40965,6 +40965,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="AJ230:AL230"/>
+    <mergeCell ref="Z218:AC218"/>
+    <mergeCell ref="AF219:AG219"/>
+    <mergeCell ref="L219:Q219"/>
+    <mergeCell ref="AB230:AE230"/>
+    <mergeCell ref="AG230:AI230"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="L137:O137"/>
+    <mergeCell ref="P137:S137"/>
+    <mergeCell ref="T137:U137"/>
+    <mergeCell ref="V137:Y137"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="L135:O135"/>
+    <mergeCell ref="P135:S135"/>
+    <mergeCell ref="T135:U135"/>
+    <mergeCell ref="V135:Y135"/>
+    <mergeCell ref="V62:Y62"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="L64:O64"/>
+    <mergeCell ref="P64:S64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="V64:Y64"/>
     <mergeCell ref="AG240:AI240"/>
     <mergeCell ref="AJ240:AL240"/>
     <mergeCell ref="V4:Y4"/>
@@ -40981,28 +41003,6 @@
     <mergeCell ref="L62:O62"/>
     <mergeCell ref="P62:S62"/>
     <mergeCell ref="T62:U62"/>
-    <mergeCell ref="V62:Y62"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="L64:O64"/>
-    <mergeCell ref="P64:S64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="V64:Y64"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="L135:O135"/>
-    <mergeCell ref="P135:S135"/>
-    <mergeCell ref="T135:U135"/>
-    <mergeCell ref="V135:Y135"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="L137:O137"/>
-    <mergeCell ref="P137:S137"/>
-    <mergeCell ref="T137:U137"/>
-    <mergeCell ref="V137:Y137"/>
-    <mergeCell ref="AJ230:AL230"/>
-    <mergeCell ref="Z218:AC218"/>
-    <mergeCell ref="AF219:AG219"/>
-    <mergeCell ref="L219:Q219"/>
-    <mergeCell ref="AB230:AE230"/>
-    <mergeCell ref="AG230:AI230"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -41146,12 +41146,12 @@
       <c r="I5" s="121"/>
       <c r="J5" s="121"/>
       <c r="K5" s="121"/>
-      <c r="L5" s="620" t="s">
+      <c r="L5" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="621"/>
-      <c r="N5" s="621"/>
-      <c r="O5" s="622"/>
+      <c r="M5" s="606"/>
+      <c r="N5" s="606"/>
+      <c r="O5" s="607"/>
       <c r="P5" s="60"/>
       <c r="Q5" s="60" t="s">
         <v>87</v>
@@ -42073,12 +42073,12 @@
       <c r="K33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="620" t="s">
+      <c r="L33" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M33" s="621"/>
-      <c r="N33" s="621"/>
-      <c r="O33" s="622"/>
+      <c r="M33" s="606"/>
+      <c r="N33" s="606"/>
+      <c r="O33" s="607"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="3" t="s">
@@ -42429,16 +42429,16 @@
       <c r="G4" s="121" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="617" t="s">
+      <c r="H4" s="611" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="618"/>
-      <c r="J4" s="619"/>
-      <c r="K4" s="620" t="s">
+      <c r="I4" s="612"/>
+      <c r="J4" s="613"/>
+      <c r="K4" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="621"/>
-      <c r="M4" s="622"/>
+      <c r="L4" s="606"/>
+      <c r="M4" s="607"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60" t="s">
         <v>87</v>
@@ -42464,16 +42464,16 @@
       <c r="G5" s="375" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="626" t="s">
+      <c r="H5" s="623" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="627"/>
-      <c r="J5" s="628"/>
-      <c r="K5" s="626" t="s">
+      <c r="I5" s="624"/>
+      <c r="J5" s="625"/>
+      <c r="K5" s="623" t="s">
         <v>292</v>
       </c>
-      <c r="L5" s="627"/>
-      <c r="M5" s="628"/>
+      <c r="L5" s="624"/>
+      <c r="M5" s="625"/>
       <c r="N5" s="376" t="s">
         <v>92</v>
       </c>
@@ -42490,23 +42490,23 @@
         <v>210</v>
       </c>
       <c r="AA5" s="201"/>
-      <c r="AB5" s="623" t="s">
+      <c r="AB5" s="626" t="s">
         <v>541</v>
       </c>
-      <c r="AC5" s="623"/>
+      <c r="AC5" s="626"/>
       <c r="AD5" s="378"/>
-      <c r="AE5" s="624" t="s">
+      <c r="AE5" s="627" t="s">
         <v>65</v>
       </c>
-      <c r="AF5" s="624"/>
-      <c r="AG5" s="624" t="s">
+      <c r="AF5" s="627"/>
+      <c r="AG5" s="627" t="s">
         <v>542</v>
       </c>
-      <c r="AH5" s="624"/>
-      <c r="AI5" s="625" t="s">
+      <c r="AH5" s="627"/>
+      <c r="AI5" s="628" t="s">
         <v>543</v>
       </c>
-      <c r="AJ5" s="625"/>
+      <c r="AJ5" s="628"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="422" t="str">
@@ -43244,12 +43244,12 @@
       <c r="K27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="620" t="s">
+      <c r="L27" s="605" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="621"/>
-      <c r="N27" s="621"/>
-      <c r="O27" s="622"/>
+      <c r="M27" s="606"/>
+      <c r="N27" s="606"/>
+      <c r="O27" s="607"/>
       <c r="T27" s="203"/>
       <c r="U27" s="203"/>
     </row>
@@ -43257,12 +43257,12 @@
       <c r="J28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L28" s="611" t="s">
+      <c r="L28" s="608" t="s">
         <v>91</v>
       </c>
-      <c r="M28" s="612"/>
-      <c r="N28" s="612"/>
-      <c r="O28" s="613"/>
+      <c r="M28" s="609"/>
+      <c r="N28" s="609"/>
+      <c r="O28" s="610"/>
       <c r="T28" s="203"/>
       <c r="U28" s="203"/>
     </row>
@@ -44652,16 +44652,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -45092,103 +45092,103 @@
       <c r="C4" s="273" t="s">
         <v>301</v>
       </c>
-      <c r="D4" s="630" t="s">
+      <c r="D4" s="629" t="s">
         <v>302</v>
       </c>
-      <c r="E4" s="629"/>
-      <c r="F4" s="629"/>
-      <c r="G4" s="629"/>
+      <c r="E4" s="630"/>
+      <c r="F4" s="630"/>
+      <c r="G4" s="630"/>
       <c r="H4" s="631"/>
-      <c r="I4" s="629" t="s">
+      <c r="I4" s="630" t="s">
         <v>303</v>
       </c>
-      <c r="J4" s="629"/>
-      <c r="K4" s="629"/>
-      <c r="L4" s="629"/>
+      <c r="J4" s="630"/>
+      <c r="K4" s="630"/>
+      <c r="L4" s="630"/>
       <c r="M4" s="631"/>
-      <c r="N4" s="629" t="s">
+      <c r="N4" s="630" t="s">
         <v>304</v>
       </c>
-      <c r="O4" s="629"/>
-      <c r="P4" s="629"/>
-      <c r="Q4" s="629"/>
+      <c r="O4" s="630"/>
+      <c r="P4" s="630"/>
+      <c r="Q4" s="630"/>
       <c r="R4" s="631"/>
-      <c r="S4" s="629" t="s">
+      <c r="S4" s="630" t="s">
         <v>305</v>
       </c>
-      <c r="T4" s="629"/>
-      <c r="U4" s="629"/>
-      <c r="V4" s="629"/>
+      <c r="T4" s="630"/>
+      <c r="U4" s="630"/>
+      <c r="V4" s="630"/>
       <c r="W4" s="631"/>
-      <c r="X4" s="629" t="s">
+      <c r="X4" s="630" t="s">
         <v>306</v>
       </c>
-      <c r="Y4" s="629"/>
-      <c r="Z4" s="629"/>
-      <c r="AA4" s="629"/>
+      <c r="Y4" s="630"/>
+      <c r="Z4" s="630"/>
+      <c r="AA4" s="630"/>
       <c r="AB4" s="631"/>
-      <c r="AC4" s="629" t="s">
+      <c r="AC4" s="630" t="s">
         <v>307</v>
       </c>
-      <c r="AD4" s="629"/>
-      <c r="AE4" s="629"/>
-      <c r="AF4" s="629"/>
+      <c r="AD4" s="630"/>
+      <c r="AE4" s="630"/>
+      <c r="AF4" s="630"/>
       <c r="AG4" s="631"/>
-      <c r="AH4" s="629" t="s">
+      <c r="AH4" s="630" t="s">
         <v>308</v>
       </c>
-      <c r="AI4" s="629"/>
-      <c r="AJ4" s="629"/>
-      <c r="AK4" s="629"/>
+      <c r="AI4" s="630"/>
+      <c r="AJ4" s="630"/>
+      <c r="AK4" s="630"/>
       <c r="AL4" s="631"/>
-      <c r="AM4" s="629" t="s">
+      <c r="AM4" s="630" t="s">
         <v>309</v>
       </c>
-      <c r="AN4" s="629"/>
-      <c r="AO4" s="629"/>
-      <c r="AP4" s="629"/>
+      <c r="AN4" s="630"/>
+      <c r="AO4" s="630"/>
+      <c r="AP4" s="630"/>
       <c r="AQ4" s="631"/>
-      <c r="AR4" s="629" t="s">
+      <c r="AR4" s="630" t="s">
         <v>310</v>
       </c>
-      <c r="AS4" s="629"/>
-      <c r="AT4" s="629"/>
-      <c r="AU4" s="629"/>
+      <c r="AS4" s="630"/>
+      <c r="AT4" s="630"/>
+      <c r="AU4" s="630"/>
       <c r="AV4" s="631"/>
-      <c r="AW4" s="629" t="s">
+      <c r="AW4" s="630" t="s">
         <v>311</v>
       </c>
-      <c r="AX4" s="629"/>
-      <c r="AY4" s="629"/>
-      <c r="AZ4" s="629"/>
-      <c r="BA4" s="629"/>
-      <c r="BB4" s="630" t="s">
+      <c r="AX4" s="630"/>
+      <c r="AY4" s="630"/>
+      <c r="AZ4" s="630"/>
+      <c r="BA4" s="630"/>
+      <c r="BB4" s="629" t="s">
         <v>312</v>
       </c>
-      <c r="BC4" s="629"/>
-      <c r="BD4" s="629"/>
-      <c r="BE4" s="629"/>
+      <c r="BC4" s="630"/>
+      <c r="BD4" s="630"/>
+      <c r="BE4" s="630"/>
       <c r="BF4" s="631"/>
-      <c r="BG4" s="629" t="s">
+      <c r="BG4" s="630" t="s">
         <v>313</v>
       </c>
-      <c r="BH4" s="629"/>
-      <c r="BI4" s="629"/>
-      <c r="BJ4" s="629"/>
-      <c r="BK4" s="629"/>
-      <c r="BL4" s="630" t="s">
+      <c r="BH4" s="630"/>
+      <c r="BI4" s="630"/>
+      <c r="BJ4" s="630"/>
+      <c r="BK4" s="630"/>
+      <c r="BL4" s="629" t="s">
         <v>314</v>
       </c>
-      <c r="BM4" s="629"/>
-      <c r="BN4" s="629"/>
-      <c r="BO4" s="629"/>
-      <c r="BP4" s="629"/>
-      <c r="BQ4" s="630" t="s">
+      <c r="BM4" s="630"/>
+      <c r="BN4" s="630"/>
+      <c r="BO4" s="630"/>
+      <c r="BP4" s="630"/>
+      <c r="BQ4" s="629" t="s">
         <v>315</v>
       </c>
-      <c r="BR4" s="629"/>
-      <c r="BS4" s="629"/>
-      <c r="BT4" s="629"/>
+      <c r="BR4" s="630"/>
+      <c r="BS4" s="630"/>
+      <c r="BT4" s="630"/>
       <c r="BU4" s="631"/>
       <c r="BV4" s="274" t="s">
         <v>316</v>
@@ -58782,11 +58782,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -58799,6 +58794,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -58821,23 +58821,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="638" t="s">
+      <c r="A1" s="636" t="s">
         <v>585</v>
       </c>
-      <c r="B1" s="640" t="s">
+      <c r="B1" s="638" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="641"/>
-      <c r="D1" s="641"/>
-      <c r="E1" s="641"/>
-      <c r="F1" s="642"/>
-      <c r="G1" s="640" t="s">
+      <c r="C1" s="639"/>
+      <c r="D1" s="639"/>
+      <c r="E1" s="639"/>
+      <c r="F1" s="640"/>
+      <c r="G1" s="638" t="s">
         <v>587</v>
       </c>
-      <c r="H1" s="641"/>
-      <c r="I1" s="641"/>
-      <c r="J1" s="641"/>
-      <c r="K1" s="642"/>
+      <c r="H1" s="639"/>
+      <c r="I1" s="639"/>
+      <c r="J1" s="639"/>
+      <c r="K1" s="640"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -58847,7 +58847,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="639"/>
+      <c r="A2" s="637"/>
       <c r="B2" s="443" t="s">
         <v>254</v>
       </c>
@@ -60340,11 +60340,11 @@
       <c r="Y48" t="s">
         <v>636</v>
       </c>
-      <c r="Z48" s="636" t="s">
+      <c r="Z48" s="641" t="s">
         <v>574</v>
       </c>
-      <c r="AA48" s="637"/>
-      <c r="AB48" s="637"/>
+      <c r="AA48" s="642"/>
+      <c r="AB48" s="642"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
@@ -60561,11 +60561,11 @@
       <c r="Y53" t="s">
         <v>638</v>
       </c>
-      <c r="Z53" s="636" t="s">
+      <c r="Z53" s="641" t="s">
         <v>573</v>
       </c>
-      <c r="AA53" s="637"/>
-      <c r="AB53" s="637"/>
+      <c r="AA53" s="642"/>
+      <c r="AB53" s="642"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
@@ -60767,11 +60767,11 @@
       <c r="Y59" t="s">
         <v>639</v>
       </c>
-      <c r="Z59" s="636" t="s">
+      <c r="Z59" s="641" t="s">
         <v>640</v>
       </c>
-      <c r="AA59" s="637"/>
-      <c r="AB59" s="637"/>
+      <c r="AA59" s="642"/>
+      <c r="AB59" s="642"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="463" t="str">
@@ -61608,17 +61608,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="54" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>